<commit_message>
Added Slides - Day 1
</commit_message>
<xml_diff>
--- a/Java Apps @ DXC - Domain - TOC.xlsx
+++ b/Java Apps @ DXC - Domain - TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="1" activeTab="5"/>
+    <workbookView windowWidth="20490" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="7" r:id="rId1"/>
@@ -1404,10 +1404,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="35">
     <font>
@@ -1521,14 +1521,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1542,6 +1542,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -1550,17 +1558,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1597,14 +1605,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -1636,7 +1636,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1651,7 +1651,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1697,13 +1697,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1715,13 +1763,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1739,55 +1781,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1811,24 +1823,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1841,25 +1835,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1871,13 +1859,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2045,6 +2045,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2059,27 +2068,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -2089,130 +2089,130 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2651,8 +2651,8 @@
   <sheetPr/>
   <dimension ref="A7:I23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -2787,7 +2787,7 @@
       <c r="E21" s="40"/>
       <c r="F21" s="40"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" ht="26" customHeight="1" spans="1:6">
       <c r="A22" s="38"/>
       <c r="B22" s="41" t="s">
         <v>15</v>
@@ -5849,8 +5849,8 @@
   <sheetPr/>
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3:A63"/>
     </sheetView>

</xml_diff>

<commit_message>
Added Course Materials - Day 3
</commit_message>
<xml_diff>
--- a/Java Apps @ DXC - Domain - TOC.xlsx
+++ b/Java Apps @ DXC - Domain - TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815"/>
+    <workbookView windowWidth="20490" windowHeight="7815" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="7" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="452">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -303,6 +303,12 @@
     <t>8. CalcEngine with For-each Loop</t>
   </si>
   <si>
+    <t>Java Fundamentals</t>
+  </si>
+  <si>
+    <t>Hands On Exercises - Java Fundamentals</t>
+  </si>
+  <si>
     <t>Day 4</t>
   </si>
   <si>
@@ -403,12 +409,6 @@
   </si>
   <si>
     <t>10. Adding a Default Method to an Interface</t>
-  </si>
-  <si>
-    <t>Java Fundamentals</t>
-  </si>
-  <si>
-    <t>Hands On Exercises - Java Fundamentals</t>
   </si>
   <si>
     <t>Day 5</t>
@@ -1406,8 +1406,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="35">
     <font>
@@ -1521,20 +1521,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1553,14 +1545,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1591,25 +1575,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1628,15 +1603,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1651,7 +1651,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1697,19 +1697,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1721,13 +1715,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1739,61 +1751,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1811,7 +1781,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1823,13 +1823,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1847,19 +1847,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1871,13 +1859,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1971,17 +1971,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1993,6 +1982,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2021,21 +2025,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -2047,9 +2036,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2068,151 +2059,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2253,11 +2253,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2651,7 +2651,7 @@
   <sheetPr/>
   <dimension ref="A7:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -2908,37 +2908,37 @@
     </row>
     <row r="9" ht="15" spans="1:3">
       <c r="A9" s="12"/>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" ht="15" spans="1:3">
       <c r="A10" s="12"/>
-      <c r="B10" s="15"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" ht="15" spans="1:3">
       <c r="A11" s="12"/>
-      <c r="B11" s="15"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" ht="52" customHeight="1" spans="1:3">
       <c r="A12" s="12"/>
-      <c r="B12" s="15"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="23" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" ht="12" customHeight="1" spans="1:3">
       <c r="A13" s="12"/>
-      <c r="B13" s="15"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="5"/>
     </row>
     <row r="14" ht="15.75" spans="1:3">
@@ -2959,24 +2959,24 @@
     </row>
     <row r="16" ht="15" spans="1:3">
       <c r="A16" s="12"/>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" ht="15" spans="1:3">
       <c r="A17" s="12"/>
-      <c r="B17" s="15"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" ht="8" customHeight="1" spans="1:3">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
     </row>
     <row r="19" ht="33" customHeight="1" spans="1:3">
       <c r="A19" s="24" t="s">
@@ -3003,30 +3003,30 @@
     </row>
     <row r="22" ht="15" spans="1:3">
       <c r="A22" s="12"/>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="23" ht="15" spans="1:3">
       <c r="A23" s="12"/>
-      <c r="B23" s="15"/>
+      <c r="B23" s="14"/>
       <c r="C23" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="24" ht="69" customHeight="1" spans="1:3">
       <c r="A24" s="12"/>
-      <c r="B24" s="15"/>
+      <c r="B24" s="14"/>
       <c r="C24" s="23" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="25" ht="9" customHeight="1" spans="1:3">
       <c r="A25" s="12"/>
-      <c r="B25" s="15"/>
+      <c r="B25" s="14"/>
       <c r="C25" s="5"/>
     </row>
     <row r="26" ht="38" customHeight="1" spans="1:3">
@@ -3047,16 +3047,16 @@
     </row>
     <row r="28" ht="15" spans="1:3">
       <c r="A28" s="12"/>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="29" ht="100" customHeight="1" spans="1:3">
       <c r="A29" s="12"/>
-      <c r="B29" s="15"/>
+      <c r="B29" s="14"/>
       <c r="C29" s="23" t="s">
         <v>42</v>
       </c>
@@ -3084,24 +3084,24 @@
     </row>
     <row r="33" ht="13" customHeight="1" spans="1:3">
       <c r="A33" s="12"/>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C33" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="34" ht="89" customHeight="1" spans="1:3">
       <c r="A34" s="12"/>
-      <c r="B34" s="15"/>
+      <c r="B34" s="14"/>
       <c r="C34" s="23" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
+      <c r="A35" s="16"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
     </row>
     <row r="37" ht="18.75" spans="1:2">
       <c r="A37" s="22" t="s">
@@ -3142,12 +3142,12 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C224"/>
+  <dimension ref="A1:C227"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B224" sqref="B224"/>
+      <selection pane="bottomLeft" activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -3465,191 +3465,191 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" ht="9" customHeight="1" spans="1:3">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-    </row>
-    <row r="44" ht="24.75" spans="1:3">
-      <c r="A44" s="2" t="s">
+    <row r="43" ht="10" customHeight="1" spans="1:3">
+      <c r="A43" s="12"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="5"/>
+    </row>
+    <row r="44" ht="15" spans="1:3">
+      <c r="A44" s="12"/>
+      <c r="B44" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C44" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-    </row>
-    <row r="45" ht="15" spans="1:3">
-      <c r="A45" s="12" t="s">
+    </row>
+    <row r="45" ht="18.75" spans="1:3">
+      <c r="A45" s="12"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B45" s="6" t="s">
+    </row>
+    <row r="46" ht="9" customHeight="1" spans="1:3">
+      <c r="A46" s="16"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+    </row>
+    <row r="47" ht="24.75" spans="1:3">
+      <c r="A47" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+    </row>
+    <row r="48" ht="15" spans="1:3">
+      <c r="A48" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="46" ht="15" spans="1:3">
-      <c r="A46" s="12"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="47" ht="15" spans="1:3">
-      <c r="A47" s="12"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="48" ht="15" spans="1:3">
-      <c r="A48" s="12"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="5" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="49" ht="15" spans="1:3">
       <c r="A49" s="12"/>
       <c r="B49" s="6"/>
       <c r="C49" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" ht="15" spans="1:3">
       <c r="A50" s="12"/>
       <c r="B50" s="6"/>
       <c r="C50" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" ht="15" spans="1:3">
       <c r="A51" s="12"/>
       <c r="B51" s="6"/>
       <c r="C51" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" ht="15" spans="1:3">
       <c r="A52" s="12"/>
       <c r="B52" s="6"/>
       <c r="C52" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" ht="15" spans="1:3">
       <c r="A53" s="12"/>
       <c r="B53" s="6"/>
       <c r="C53" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" ht="15" spans="1:3">
       <c r="A54" s="12"/>
       <c r="B54" s="6"/>
       <c r="C54" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="55" ht="15" spans="1:3">
+      <c r="A55" s="12"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="55" ht="9" customHeight="1"/>
     <row r="56" ht="15" spans="1:3">
-      <c r="A56" s="12" t="s">
+      <c r="A56" s="12"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="57" ht="15" spans="1:3">
       <c r="A57" s="12"/>
       <c r="B57" s="6"/>
-      <c r="C57" s="5"/>
-    </row>
-    <row r="58" ht="15" spans="1:3">
-      <c r="A58" s="12"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
+      <c r="C57" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="58" ht="9" customHeight="1"/>
     <row r="59" ht="15" spans="1:3">
-      <c r="A59" s="12"/>
-      <c r="B59" s="6"/>
+      <c r="A59" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>106</v>
+      </c>
       <c r="C59" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="60" ht="15" spans="1:3">
       <c r="A60" s="12"/>
       <c r="B60" s="6"/>
-      <c r="C60" s="5" t="s">
-        <v>107</v>
-      </c>
+      <c r="C60" s="5"/>
     </row>
     <row r="61" ht="15" spans="1:3">
       <c r="A61" s="12"/>
       <c r="B61" s="6"/>
       <c r="C61" s="5" t="s">
-        <v>108</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" ht="15" spans="1:3">
       <c r="A62" s="12"/>
       <c r="B62" s="6"/>
       <c r="C62" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="63" ht="15" spans="1:3">
       <c r="A63" s="12"/>
       <c r="B63" s="6"/>
       <c r="C63" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="64" ht="15" spans="1:3">
       <c r="A64" s="12"/>
       <c r="B64" s="6"/>
       <c r="C64" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="65" ht="15" spans="1:3">
       <c r="A65" s="12"/>
       <c r="B65" s="6"/>
       <c r="C65" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="66" ht="15" spans="1:3">
       <c r="A66" s="12"/>
       <c r="B66" s="6"/>
       <c r="C66" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="67" ht="15" spans="1:3">
       <c r="A67" s="12"/>
       <c r="B67" s="6"/>
       <c r="C67" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="68" ht="15.75" spans="1:3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="68" ht="15" spans="1:3">
       <c r="A68" s="12"/>
       <c r="B68" s="6"/>
-      <c r="C68" s="5"/>
+      <c r="C68" s="5" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="69" ht="15" spans="1:3">
       <c r="A69" s="12"/>
-      <c r="B69" s="6" t="s">
+      <c r="B69" s="6"/>
+      <c r="C69" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="70" ht="15" spans="1:3">
@@ -3659,1137 +3659,1160 @@
         <v>116</v>
       </c>
     </row>
-    <row r="71" ht="15" spans="1:3">
+    <row r="71" ht="15.75" spans="1:3">
       <c r="A71" s="12"/>
       <c r="B71" s="6"/>
-      <c r="C71" s="5" t="s">
-        <v>117</v>
-      </c>
+      <c r="C71" s="5"/>
     </row>
     <row r="72" ht="15" spans="1:3">
       <c r="A72" s="12"/>
-      <c r="B72" s="6"/>
+      <c r="B72" s="6" t="s">
+        <v>117</v>
+      </c>
       <c r="C72" s="5" t="s">
-        <v>118</v>
+        <v>59</v>
       </c>
     </row>
     <row r="73" ht="15" spans="1:3">
       <c r="A73" s="12"/>
       <c r="B73" s="6"/>
       <c r="C73" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="74" ht="15" spans="1:3">
       <c r="A74" s="12"/>
       <c r="B74" s="6"/>
       <c r="C74" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="75" ht="15" spans="1:3">
       <c r="A75" s="12"/>
       <c r="B75" s="6"/>
       <c r="C75" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="76" ht="15" spans="1:3">
       <c r="A76" s="12"/>
       <c r="B76" s="6"/>
       <c r="C76" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="77" ht="15" spans="1:3">
       <c r="A77" s="12"/>
       <c r="B77" s="6"/>
       <c r="C77" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="78" ht="15" spans="1:3">
       <c r="A78" s="12"/>
       <c r="B78" s="6"/>
       <c r="C78" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="79" ht="15" spans="1:3">
       <c r="A79" s="12"/>
       <c r="B79" s="6"/>
       <c r="C79" s="5" t="s">
-        <v>69</v>
+        <v>124</v>
       </c>
     </row>
     <row r="80" ht="15" spans="1:3">
       <c r="A80" s="12"/>
-      <c r="B80" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C80" s="16" t="s">
+      <c r="B80" s="6"/>
+      <c r="C80" s="5" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="81" ht="15" spans="1:3">
       <c r="A81" s="12"/>
-      <c r="B81" s="15"/>
+      <c r="B81" s="6"/>
       <c r="C81" s="5" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="82" ht="9" customHeight="1" spans="1:3">
-      <c r="A82" s="14"/>
-      <c r="B82" s="14"/>
-      <c r="C82" s="14"/>
-    </row>
-    <row r="83" ht="24.75" spans="1:3">
-      <c r="A83" s="2" t="s">
+    <row r="82" ht="15" spans="1:3">
+      <c r="A82" s="12"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="83" ht="15" spans="1:3">
+      <c r="A83" s="12"/>
+      <c r="B83" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C83" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="84" ht="15" spans="1:3">
+      <c r="A84" s="12"/>
+      <c r="B84" s="14"/>
+      <c r="C84" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="85" ht="9" customHeight="1" spans="1:3">
+      <c r="A85" s="16"/>
+      <c r="B85" s="16"/>
+      <c r="C85" s="16"/>
+    </row>
+    <row r="86" ht="24.75" spans="1:3">
+      <c r="A86" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-    </row>
-    <row r="84" ht="15" spans="1:3">
-      <c r="A84" s="12" t="s">
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
+    </row>
+    <row r="87" ht="15" spans="1:3">
+      <c r="A87" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B84" s="6" t="s">
+      <c r="B87" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="C84" s="5" t="s">
+      <c r="C87" s="5" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="85" ht="15" spans="1:3">
-      <c r="A85" s="12"/>
-      <c r="B85" s="6"/>
-      <c r="C85" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="86" ht="15" spans="1:3">
-      <c r="A86" s="12"/>
-      <c r="B86" s="6"/>
-      <c r="C86" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="87" ht="15" spans="1:3">
-      <c r="A87" s="12"/>
-      <c r="B87" s="6"/>
-      <c r="C87" s="5" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="88" ht="15" spans="1:3">
       <c r="A88" s="12"/>
       <c r="B88" s="6"/>
       <c r="C88" s="5" t="s">
-        <v>132</v>
+        <v>59</v>
       </c>
     </row>
     <row r="89" ht="15" spans="1:3">
       <c r="A89" s="12"/>
       <c r="B89" s="6"/>
       <c r="C89" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="90" ht="15" spans="1:3">
       <c r="A90" s="12"/>
       <c r="B90" s="6"/>
       <c r="C90" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="91" ht="15" spans="1:3">
       <c r="A91" s="12"/>
       <c r="B91" s="6"/>
       <c r="C91" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="92" ht="15" spans="1:3">
       <c r="A92" s="12"/>
       <c r="B92" s="6"/>
-      <c r="C92" s="5"/>
+      <c r="C92" s="5" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="93" ht="15" spans="1:3">
       <c r="A93" s="12"/>
-      <c r="B93" s="6" t="s">
-        <v>136</v>
-      </c>
+      <c r="B93" s="6"/>
       <c r="C93" s="5" t="s">
-        <v>59</v>
+        <v>134</v>
       </c>
     </row>
     <row r="94" ht="15" spans="1:3">
       <c r="A94" s="12"/>
       <c r="B94" s="6"/>
       <c r="C94" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="95" ht="15" spans="1:3">
       <c r="A95" s="12"/>
       <c r="B95" s="6"/>
-      <c r="C95" s="5" t="s">
-        <v>138</v>
-      </c>
+      <c r="C95" s="5"/>
     </row>
     <row r="96" ht="15" spans="1:3">
       <c r="A96" s="12"/>
-      <c r="B96" s="6"/>
+      <c r="B96" s="6" t="s">
+        <v>136</v>
+      </c>
       <c r="C96" s="5" t="s">
-        <v>139</v>
+        <v>59</v>
       </c>
     </row>
     <row r="97" ht="15" spans="1:3">
       <c r="A97" s="12"/>
       <c r="B97" s="6"/>
       <c r="C97" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="98" ht="15" spans="1:3">
       <c r="A98" s="12"/>
       <c r="B98" s="6"/>
       <c r="C98" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="99" ht="15" spans="1:3">
       <c r="A99" s="12"/>
       <c r="B99" s="6"/>
       <c r="C99" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="100" ht="15" spans="1:3">
       <c r="A100" s="12"/>
       <c r="B100" s="6"/>
       <c r="C100" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="101" ht="9" customHeight="1"/>
-    <row r="102" ht="22" customHeight="1" spans="1:3">
-      <c r="A102" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>144</v>
-      </c>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="101" ht="15" spans="1:3">
+      <c r="A101" s="12"/>
+      <c r="B101" s="6"/>
+      <c r="C101" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="102" ht="15" spans="1:3">
+      <c r="A102" s="12"/>
+      <c r="B102" s="6"/>
       <c r="C102" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="103" ht="15" hidden="1" spans="1:3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="103" ht="15" spans="1:3">
       <c r="A103" s="12"/>
       <c r="B103" s="6"/>
       <c r="C103" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="104" ht="15" spans="1:3">
-      <c r="A104" s="12"/>
-      <c r="B104" s="6"/>
-      <c r="C104" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="105" ht="15" spans="1:3">
-      <c r="A105" s="12"/>
-      <c r="B105" s="6"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="104" ht="9" customHeight="1"/>
+    <row r="105" ht="22" customHeight="1" spans="1:3">
+      <c r="A105" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B105" s="6" t="s">
+        <v>144</v>
+      </c>
       <c r="C105" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="106" ht="15" spans="1:3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="106" ht="15" hidden="1" spans="1:3">
       <c r="A106" s="12"/>
       <c r="B106" s="6"/>
       <c r="C106" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="107" ht="15" spans="1:3">
       <c r="A107" s="12"/>
       <c r="B107" s="6"/>
       <c r="C107" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="108" ht="15" spans="1:3">
       <c r="A108" s="12"/>
       <c r="B108" s="6"/>
       <c r="C108" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="109" ht="15" spans="1:3">
       <c r="A109" s="12"/>
       <c r="B109" s="6"/>
       <c r="C109" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="110" ht="15" spans="1:3">
       <c r="A110" s="12"/>
       <c r="B110" s="6"/>
       <c r="C110" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="111" ht="15" spans="1:3">
       <c r="A111" s="12"/>
       <c r="B111" s="6"/>
       <c r="C111" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="112" ht="15" spans="1:3">
       <c r="A112" s="12"/>
       <c r="B112" s="6"/>
       <c r="C112" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="113" ht="15" spans="1:3">
       <c r="A113" s="12"/>
       <c r="B113" s="6"/>
       <c r="C113" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="114" ht="15" spans="1:3">
       <c r="A114" s="12"/>
       <c r="B114" s="6"/>
       <c r="C114" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="115" ht="15" spans="1:3">
       <c r="A115" s="12"/>
       <c r="B115" s="6"/>
       <c r="C115" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="116" ht="15" spans="1:3">
       <c r="A116" s="12"/>
       <c r="B116" s="6"/>
       <c r="C116" s="5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="117" ht="15.75" spans="1:3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="117" ht="15" spans="1:3">
       <c r="A117" s="12"/>
       <c r="B117" s="6"/>
-      <c r="C117" s="5"/>
+      <c r="C117" s="5" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="118" ht="15" spans="1:3">
       <c r="A118" s="12"/>
-      <c r="B118" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C118" s="16" t="s">
-        <v>158</v>
+      <c r="B118" s="6"/>
+      <c r="C118" s="5" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="119" ht="15" spans="1:3">
       <c r="A119" s="12"/>
-      <c r="B119" s="15"/>
+      <c r="B119" s="6"/>
       <c r="C119" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="120" ht="15" spans="1:3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="120" ht="15.75" spans="1:3">
       <c r="A120" s="12"/>
-      <c r="B120" s="15"/>
-      <c r="C120" s="5" t="s">
-        <v>160</v>
-      </c>
+      <c r="B120" s="6"/>
+      <c r="C120" s="5"/>
     </row>
     <row r="121" ht="15" spans="1:3">
       <c r="A121" s="12"/>
-      <c r="B121" s="15"/>
-      <c r="C121" s="5" t="s">
+      <c r="B121" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C121" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="122" ht="15" spans="1:3">
+      <c r="A122" s="12"/>
+      <c r="B122" s="14"/>
+      <c r="C122" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="123" ht="15" spans="1:3">
+      <c r="A123" s="12"/>
+      <c r="B123" s="14"/>
+      <c r="C123" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="124" ht="15" spans="1:3">
+      <c r="A124" s="12"/>
+      <c r="B124" s="14"/>
+      <c r="C124" s="5" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="122" ht="9" customHeight="1" spans="1:3">
-      <c r="A122" s="14"/>
-      <c r="B122" s="14"/>
-      <c r="C122" s="14"/>
-    </row>
-    <row r="123" ht="24" customHeight="1" spans="1:3">
-      <c r="A123" s="2" t="s">
+    <row r="125" ht="9" customHeight="1" spans="1:3">
+      <c r="A125" s="16"/>
+      <c r="B125" s="16"/>
+      <c r="C125" s="16"/>
+    </row>
+    <row r="126" ht="24" customHeight="1" spans="1:3">
+      <c r="A126" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B123" s="2"/>
-      <c r="C123" s="2"/>
-    </row>
-    <row r="124" ht="15" spans="1:3">
-      <c r="A124" s="12" t="s">
+      <c r="B126" s="2"/>
+      <c r="C126" s="2"/>
+    </row>
+    <row r="127" ht="15" spans="1:3">
+      <c r="A127" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="B124" s="6" t="s">
+      <c r="B127" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="C124" s="5" t="s">
+      <c r="C127" s="5" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="125" ht="15" spans="1:3">
-      <c r="A125" s="12"/>
-      <c r="B125" s="6"/>
-      <c r="C125" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="126" ht="15" spans="1:3">
-      <c r="A126" s="12"/>
-      <c r="B126" s="6"/>
-      <c r="C126" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="127" ht="15" spans="1:3">
-      <c r="A127" s="12"/>
-      <c r="B127" s="6"/>
-      <c r="C127" s="5" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="128" ht="15" spans="1:3">
       <c r="A128" s="12"/>
       <c r="B128" s="6"/>
       <c r="C128" s="5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="129" ht="15" spans="1:3">
       <c r="A129" s="12"/>
       <c r="B129" s="6"/>
       <c r="C129" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="130" ht="15" spans="1:3">
       <c r="A130" s="12"/>
       <c r="B130" s="6"/>
       <c r="C130" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="131" ht="15" spans="1:3">
       <c r="A131" s="12"/>
       <c r="B131" s="6"/>
       <c r="C131" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="132" ht="15" spans="1:3">
       <c r="A132" s="12"/>
       <c r="B132" s="6"/>
       <c r="C132" s="5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="133" ht="15" spans="1:3">
       <c r="A133" s="12"/>
       <c r="B133" s="6"/>
       <c r="C133" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="134" ht="15" spans="1:3">
       <c r="A134" s="12"/>
       <c r="B134" s="6"/>
       <c r="C134" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="135" ht="11" customHeight="1" spans="1:3">
-      <c r="A135" s="17"/>
-      <c r="B135" s="18"/>
-      <c r="C135" s="5"/>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="135" ht="15" spans="1:3">
+      <c r="A135" s="12"/>
+      <c r="B135" s="6"/>
+      <c r="C135" s="5" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="136" ht="15" spans="1:3">
-      <c r="A136" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="B136" s="6" t="s">
-        <v>175</v>
-      </c>
+      <c r="A136" s="12"/>
+      <c r="B136" s="6"/>
       <c r="C136" s="5" t="s">
-        <v>59</v>
+        <v>173</v>
       </c>
     </row>
     <row r="137" ht="15" spans="1:3">
       <c r="A137" s="12"/>
       <c r="B137" s="6"/>
       <c r="C137" s="5" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="138" ht="15" spans="1:3">
-      <c r="A138" s="12"/>
-      <c r="B138" s="6"/>
-      <c r="C138" s="5" t="s">
-        <v>177</v>
-      </c>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="138" ht="11" customHeight="1" spans="1:3">
+      <c r="A138" s="17"/>
+      <c r="B138" s="18"/>
+      <c r="C138" s="5"/>
     </row>
     <row r="139" ht="15" spans="1:3">
-      <c r="A139" s="12"/>
-      <c r="B139" s="6"/>
+      <c r="A139" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="B139" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="C139" s="5" t="s">
-        <v>178</v>
+        <v>59</v>
       </c>
     </row>
     <row r="140" ht="15" spans="1:3">
       <c r="A140" s="12"/>
       <c r="B140" s="6"/>
       <c r="C140" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="141" ht="15" spans="1:3">
       <c r="A141" s="12"/>
       <c r="B141" s="6"/>
-      <c r="C141" s="19" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="142" ht="21" customHeight="1" spans="1:3">
+      <c r="C141" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="142" ht="15" spans="1:3">
       <c r="A142" s="12"/>
       <c r="B142" s="6"/>
-      <c r="C142" s="19" t="s">
-        <v>181</v>
+      <c r="C142" s="5" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="143" ht="15" spans="1:3">
       <c r="A143" s="12"/>
       <c r="B143" s="6"/>
-      <c r="C143" s="19" t="s">
-        <v>182</v>
+      <c r="C143" s="5" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="144" ht="15" spans="1:3">
       <c r="A144" s="12"/>
       <c r="B144" s="6"/>
       <c r="C144" s="19" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="145" ht="15" spans="1:3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="145" ht="21" customHeight="1" spans="1:3">
       <c r="A145" s="12"/>
       <c r="B145" s="6"/>
       <c r="C145" s="19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="146" ht="15" spans="1:3">
       <c r="A146" s="12"/>
       <c r="B146" s="6"/>
       <c r="C146" s="19" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="147" ht="15" spans="1:3">
       <c r="A147" s="12"/>
       <c r="B147" s="6"/>
       <c r="C147" s="19" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="148" ht="15" spans="1:3">
       <c r="A148" s="12"/>
       <c r="B148" s="6"/>
       <c r="C148" s="19" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="149" ht="15" spans="1:3">
       <c r="A149" s="12"/>
       <c r="B149" s="6"/>
       <c r="C149" s="19" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="150" ht="15" spans="1:3">
       <c r="A150" s="12"/>
       <c r="B150" s="6"/>
       <c r="C150" s="19" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="151" ht="15" spans="1:3">
       <c r="A151" s="12"/>
       <c r="B151" s="6"/>
       <c r="C151" s="19" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="152" ht="15" spans="1:3">
       <c r="A152" s="12"/>
       <c r="B152" s="6"/>
       <c r="C152" s="19" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="153" ht="15" spans="1:3">
       <c r="A153" s="12"/>
       <c r="B153" s="6"/>
       <c r="C153" s="19" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="154" ht="15" spans="1:3">
       <c r="A154" s="12"/>
       <c r="B154" s="6"/>
       <c r="C154" s="19" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="155" ht="15" spans="1:3">
       <c r="A155" s="12"/>
       <c r="B155" s="6"/>
       <c r="C155" s="19" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="156" ht="15" spans="1:3">
       <c r="A156" s="12"/>
       <c r="B156" s="6"/>
       <c r="C156" s="19" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="157" ht="15.75" spans="1:3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="157" ht="15" spans="1:3">
       <c r="A157" s="12"/>
-      <c r="B157" s="4"/>
-      <c r="C157" s="19"/>
+      <c r="B157" s="6"/>
+      <c r="C157" s="19" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="158" ht="15" spans="1:3">
       <c r="A158" s="12"/>
-      <c r="B158" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C158" s="16" t="s">
-        <v>196</v>
+      <c r="B158" s="6"/>
+      <c r="C158" s="19" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="159" ht="15" spans="1:3">
       <c r="A159" s="12"/>
-      <c r="B159" s="15"/>
-      <c r="C159" s="5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="160" ht="15" spans="1:3">
+      <c r="B159" s="6"/>
+      <c r="C159" s="19" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="160" ht="15.75" spans="1:3">
       <c r="A160" s="12"/>
-      <c r="B160" s="15"/>
-      <c r="C160" s="5" t="s">
-        <v>198</v>
-      </c>
+      <c r="B160" s="4"/>
+      <c r="C160" s="19"/>
     </row>
     <row r="161" ht="15" spans="1:3">
       <c r="A161" s="12"/>
-      <c r="B161" s="15"/>
-      <c r="C161" s="5" t="s">
-        <v>199</v>
+      <c r="B161" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C161" s="15" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="162" ht="15" spans="1:3">
       <c r="A162" s="12"/>
-      <c r="B162" s="15"/>
-      <c r="C162" s="16" t="s">
-        <v>200</v>
+      <c r="B162" s="14"/>
+      <c r="C162" s="5" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="163" ht="15" spans="1:3">
       <c r="A163" s="12"/>
-      <c r="B163" s="15"/>
+      <c r="B163" s="14"/>
       <c r="C163" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="164" ht="15" spans="1:3">
       <c r="A164" s="12"/>
-      <c r="B164" s="15"/>
+      <c r="B164" s="14"/>
       <c r="C164" s="5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="165" ht="15" spans="1:3">
       <c r="A165" s="12"/>
-      <c r="B165" s="15"/>
-      <c r="C165" s="5" t="s">
-        <v>203</v>
+      <c r="B165" s="14"/>
+      <c r="C165" s="15" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="166" ht="15" spans="1:3">
       <c r="A166" s="12"/>
-      <c r="B166" s="15"/>
+      <c r="B166" s="14"/>
       <c r="C166" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="167" ht="15" spans="1:3">
       <c r="A167" s="12"/>
-      <c r="B167" s="15"/>
+      <c r="B167" s="14"/>
       <c r="C167" s="5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="168" ht="15" spans="1:3">
       <c r="A168" s="12"/>
-      <c r="B168" s="15"/>
+      <c r="B168" s="14"/>
       <c r="C168" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="169" ht="15" spans="1:3">
+      <c r="A169" s="12"/>
+      <c r="B169" s="14"/>
+      <c r="C169" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="170" ht="15" spans="1:3">
+      <c r="A170" s="12"/>
+      <c r="B170" s="14"/>
+      <c r="C170" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="171" ht="15" spans="1:3">
+      <c r="A171" s="12"/>
+      <c r="B171" s="14"/>
+      <c r="C171" s="5" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="169" ht="9" customHeight="1" spans="1:3">
-      <c r="A169" s="14"/>
-      <c r="B169" s="14"/>
-      <c r="C169" s="14"/>
-    </row>
-    <row r="170" ht="27" customHeight="1" spans="1:3">
-      <c r="A170" s="2" t="s">
+    <row r="172" ht="9" customHeight="1" spans="1:3">
+      <c r="A172" s="16"/>
+      <c r="B172" s="16"/>
+      <c r="C172" s="16"/>
+    </row>
+    <row r="173" ht="27" customHeight="1" spans="1:3">
+      <c r="A173" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B170" s="2"/>
-      <c r="C170" s="2"/>
-    </row>
-    <row r="171" ht="27" customHeight="1" spans="1:3">
-      <c r="A171" s="12" t="s">
+      <c r="B173" s="2"/>
+      <c r="C173" s="2"/>
+    </row>
+    <row r="174" ht="27" customHeight="1" spans="1:3">
+      <c r="A174" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="B171" s="6" t="s">
+      <c r="B174" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="C171" s="5" t="s">
+      <c r="C174" s="5" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="172" ht="27" customHeight="1" spans="1:3">
-      <c r="A172" s="12"/>
-      <c r="B172" s="6"/>
-      <c r="C172" s="5" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="173" ht="27" customHeight="1" spans="1:3">
-      <c r="A173" s="12"/>
-      <c r="B173" s="6"/>
-      <c r="C173" s="5" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="174" ht="27" customHeight="1" spans="1:3">
-      <c r="A174" s="12"/>
-      <c r="B174" s="6"/>
-      <c r="C174" s="5" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="175" ht="27" customHeight="1" spans="1:3">
       <c r="A175" s="12"/>
       <c r="B175" s="6"/>
       <c r="C175" s="5" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="176" ht="18" spans="1:3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="176" ht="27" customHeight="1" spans="1:3">
       <c r="A176" s="12"/>
-      <c r="B176" s="20"/>
-      <c r="C176" s="7"/>
-    </row>
-    <row r="177" ht="15" spans="1:3">
+      <c r="B176" s="6"/>
+      <c r="C176" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="177" ht="27" customHeight="1" spans="1:3">
       <c r="A177" s="12"/>
-      <c r="B177" s="6" t="s">
-        <v>214</v>
-      </c>
+      <c r="B177" s="6"/>
       <c r="C177" s="5" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="178" ht="27" customHeight="1" spans="1:3">
       <c r="A178" s="12"/>
       <c r="B178" s="6"/>
-      <c r="C178" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="179" ht="15" spans="1:3">
+      <c r="C178" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="179" ht="18" spans="1:3">
       <c r="A179" s="12"/>
-      <c r="B179" s="6"/>
-      <c r="C179" s="5" t="s">
-        <v>217</v>
-      </c>
+      <c r="B179" s="20"/>
+      <c r="C179" s="7"/>
     </row>
     <row r="180" ht="15" spans="1:3">
       <c r="A180" s="12"/>
-      <c r="B180" s="6"/>
-      <c r="C180" s="21" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="181" ht="15" spans="1:3">
+      <c r="B180" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C180" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
       <c r="A181" s="12"/>
       <c r="B181" s="6"/>
-      <c r="C181" s="5" t="s">
-        <v>219</v>
+      <c r="C181" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="182" ht="15" spans="1:3">
       <c r="A182" s="12"/>
       <c r="B182" s="6"/>
       <c r="C182" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="183" ht="15" spans="1:3">
       <c r="A183" s="12"/>
       <c r="B183" s="6"/>
-      <c r="C183" s="5" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="184" ht="18.75" spans="1:3">
-      <c r="A184" s="17"/>
-      <c r="B184" s="20"/>
-      <c r="C184" s="5"/>
+      <c r="C183" s="21" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="184" ht="15" spans="1:3">
+      <c r="A184" s="12"/>
+      <c r="B184" s="6"/>
+      <c r="C184" s="5" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="185" ht="15" spans="1:3">
-      <c r="A185" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="B185" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="C185" s="21" t="s">
-        <v>224</v>
+      <c r="A185" s="12"/>
+      <c r="B185" s="6"/>
+      <c r="C185" s="5" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="186" ht="15" spans="1:3">
       <c r="A186" s="12"/>
       <c r="B186" s="6"/>
-      <c r="C186" s="21" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="187" ht="15" spans="1:3">
-      <c r="A187" s="12"/>
-      <c r="B187" s="6"/>
-      <c r="C187" s="21" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="188" ht="18" spans="1:3">
-      <c r="A188" s="12"/>
-      <c r="B188" s="20"/>
-      <c r="C188" s="21"/>
+      <c r="C186" s="5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="187" ht="18.75" spans="1:3">
+      <c r="A187" s="17"/>
+      <c r="B187" s="20"/>
+      <c r="C187" s="5"/>
+    </row>
+    <row r="188" ht="15" spans="1:3">
+      <c r="A188" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="B188" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="C188" s="21" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="189" ht="15" spans="1:3">
       <c r="A189" s="12"/>
-      <c r="B189" s="6" t="s">
-        <v>227</v>
-      </c>
+      <c r="B189" s="6"/>
       <c r="C189" s="21" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="190" ht="15" spans="1:3">
       <c r="A190" s="12"/>
       <c r="B190" s="6"/>
       <c r="C190" s="21" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="191" ht="15" spans="1:3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="191" ht="18" spans="1:3">
       <c r="A191" s="12"/>
-      <c r="B191" s="6"/>
-      <c r="C191" s="21" t="s">
-        <v>230</v>
-      </c>
+      <c r="B191" s="20"/>
+      <c r="C191" s="21"/>
     </row>
     <row r="192" ht="15" spans="1:3">
       <c r="A192" s="12"/>
-      <c r="B192" s="7"/>
-      <c r="C192" s="21"/>
+      <c r="B192" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C192" s="21" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="193" ht="15" spans="1:3">
       <c r="A193" s="12"/>
-      <c r="B193" s="6" t="s">
-        <v>231</v>
-      </c>
+      <c r="B193" s="6"/>
       <c r="C193" s="21" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="194" ht="15" spans="1:3">
       <c r="A194" s="12"/>
       <c r="B194" s="6"/>
       <c r="C194" s="21" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="195" ht="15" spans="1:3">
       <c r="A195" s="12"/>
-      <c r="B195" s="6"/>
-      <c r="C195" s="21" t="s">
-        <v>234</v>
-      </c>
+      <c r="B195" s="7"/>
+      <c r="C195" s="21"/>
     </row>
     <row r="196" ht="15" spans="1:3">
       <c r="A196" s="12"/>
-      <c r="B196" s="6"/>
+      <c r="B196" s="6" t="s">
+        <v>231</v>
+      </c>
       <c r="C196" s="21" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="197" ht="15" spans="1:3">
       <c r="A197" s="12"/>
       <c r="B197" s="6"/>
       <c r="C197" s="21" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="198" ht="15" spans="1:3">
       <c r="A198" s="12"/>
       <c r="B198" s="6"/>
       <c r="C198" s="21" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="199" ht="15" spans="1:3">
       <c r="A199" s="12"/>
       <c r="B199" s="6"/>
       <c r="C199" s="21" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="200" ht="15" spans="1:3">
       <c r="A200" s="12"/>
       <c r="B200" s="6"/>
       <c r="C200" s="21" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="201" ht="15" spans="1:3">
       <c r="A201" s="12"/>
       <c r="B201" s="6"/>
       <c r="C201" s="21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="202" ht="18.75" spans="1:3">
-      <c r="A202" s="17"/>
+        <v>237</v>
+      </c>
+    </row>
+    <row r="202" ht="15" spans="1:3">
+      <c r="A202" s="12"/>
       <c r="B202" s="6"/>
-      <c r="C202" s="21"/>
+      <c r="C202" s="21" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="203" ht="15" spans="1:3">
-      <c r="A203" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="B203" s="6" t="s">
-        <v>242</v>
-      </c>
+      <c r="A203" s="12"/>
+      <c r="B203" s="6"/>
       <c r="C203" s="21" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="204" ht="15" spans="1:3">
       <c r="A204" s="12"/>
       <c r="B204" s="6"/>
       <c r="C204" s="21" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="205" ht="15" spans="1:3">
-      <c r="A205" s="12"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="205" ht="18.75" spans="1:3">
+      <c r="A205" s="17"/>
       <c r="B205" s="6"/>
-      <c r="C205" s="21" t="s">
-        <v>245</v>
-      </c>
+      <c r="C205" s="21"/>
     </row>
     <row r="206" ht="15" spans="1:3">
-      <c r="A206" s="12"/>
-      <c r="B206" s="6"/>
+      <c r="A206" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="B206" s="6" t="s">
+        <v>242</v>
+      </c>
       <c r="C206" s="21" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="207" ht="15" spans="1:3">
       <c r="A207" s="12"/>
       <c r="B207" s="6"/>
       <c r="C207" s="21" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="208" ht="18.75" spans="1:3">
-      <c r="A208" s="17"/>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="208" ht="15" spans="1:3">
+      <c r="A208" s="12"/>
       <c r="B208" s="6"/>
-      <c r="C208" s="21"/>
+      <c r="C208" s="21" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="209" ht="15" spans="1:3">
-      <c r="A209" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="B209" s="15" t="s">
-        <v>249</v>
-      </c>
-      <c r="C209" s="5" t="s">
-        <v>50</v>
+      <c r="A209" s="12"/>
+      <c r="B209" s="6"/>
+      <c r="C209" s="21" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="210" ht="15" spans="1:3">
       <c r="A210" s="12"/>
-      <c r="B210" s="15"/>
-      <c r="C210" s="5" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="211" ht="15" spans="1:3">
-      <c r="A211" s="12"/>
-      <c r="B211" s="15"/>
-      <c r="C211" s="5" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="212" ht="15" customHeight="1" spans="1:3">
-      <c r="A212" s="12"/>
-      <c r="B212" s="15"/>
+      <c r="B210" s="6"/>
+      <c r="C210" s="21" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="211" ht="18.75" spans="1:3">
+      <c r="A211" s="17"/>
+      <c r="B211" s="6"/>
+      <c r="C211" s="21"/>
+    </row>
+    <row r="212" ht="15" spans="1:3">
+      <c r="A212" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="B212" s="14" t="s">
+        <v>249</v>
+      </c>
       <c r="C212" s="5" t="s">
-        <v>252</v>
+        <v>50</v>
       </c>
     </row>
     <row r="213" ht="15" spans="1:3">
       <c r="A213" s="12"/>
-      <c r="B213" s="15"/>
+      <c r="B213" s="14"/>
       <c r="C213" s="5" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="214" ht="15" spans="1:3">
       <c r="A214" s="12"/>
-      <c r="B214" s="15"/>
+      <c r="B214" s="14"/>
       <c r="C214" s="5" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="215" ht="18.75" spans="1:3">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="215" ht="15" customHeight="1" spans="1:3">
       <c r="A215" s="12"/>
-      <c r="B215" s="6"/>
-      <c r="C215" s="5"/>
+      <c r="B215" s="14"/>
+      <c r="C215" s="5" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="216" ht="15" spans="1:3">
       <c r="A216" s="12"/>
-      <c r="B216" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C216" s="16" t="s">
-        <v>255</v>
+      <c r="B216" s="14"/>
+      <c r="C216" s="5" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="217" ht="15" spans="1:3">
       <c r="A217" s="12"/>
-      <c r="B217" s="15"/>
+      <c r="B217" s="14"/>
       <c r="C217" s="5" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="218" ht="15" spans="1:3">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="218" ht="18.75" spans="1:3">
       <c r="A218" s="12"/>
-      <c r="B218" s="15"/>
-      <c r="C218" s="5" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3">
+      <c r="B218" s="6"/>
+      <c r="C218" s="5"/>
+    </row>
+    <row r="219" ht="15" spans="1:3">
       <c r="A219" s="12"/>
-      <c r="B219" s="15"/>
-      <c r="C219" s="7" t="s">
-        <v>258</v>
+      <c r="B219" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C219" s="15" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="220" ht="15" spans="1:3">
       <c r="A220" s="12"/>
-      <c r="B220" s="15"/>
-      <c r="C220" s="21" t="s">
+      <c r="B220" s="14"/>
+      <c r="C220" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="221" ht="15" spans="1:3">
+      <c r="A221" s="12"/>
+      <c r="B221" s="14"/>
+      <c r="C221" s="5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3">
+      <c r="A222" s="12"/>
+      <c r="B222" s="14"/>
+      <c r="C222" s="7" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="223" ht="15" spans="1:3">
+      <c r="A223" s="12"/>
+      <c r="B223" s="14"/>
+      <c r="C223" s="21" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="221" spans="1:3">
-      <c r="A221" s="14"/>
-      <c r="B221" s="14"/>
-      <c r="C221" s="14"/>
-    </row>
-    <row r="222" s="7" customFormat="1"/>
-    <row r="223" s="7" customFormat="1" ht="18.75" spans="1:2">
-      <c r="A223" s="22" t="s">
+    <row r="224" spans="1:3">
+      <c r="A224" s="16"/>
+      <c r="B224" s="16"/>
+      <c r="C224" s="16"/>
+    </row>
+    <row r="225" s="7" customFormat="1"/>
+    <row r="226" s="7" customFormat="1" ht="18.75" spans="1:2">
+      <c r="A226" s="22" t="s">
         <v>260</v>
       </c>
-      <c r="B223" s="11">
+      <c r="B226" s="11">
         <v>5</v>
       </c>
     </row>
-    <row r="224" ht="18.75" spans="1:2">
-      <c r="A224" s="22" t="s">
+    <row r="227" ht="18.75" spans="1:2">
+      <c r="A227" s="22" t="s">
         <v>261</v>
       </c>
-      <c r="B224" s="11">
+      <c r="B227" s="11">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="43">
+  <mergeCells count="45">
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A83:C83"/>
-    <mergeCell ref="A123:C123"/>
-    <mergeCell ref="A170:C170"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A86:C86"/>
+    <mergeCell ref="A126:C126"/>
+    <mergeCell ref="A173:C173"/>
     <mergeCell ref="A3:A9"/>
     <mergeCell ref="A11:A21"/>
     <mergeCell ref="A23:A33"/>
     <mergeCell ref="A35:A42"/>
-    <mergeCell ref="A45:A54"/>
-    <mergeCell ref="A56:A81"/>
-    <mergeCell ref="A84:A100"/>
-    <mergeCell ref="A102:A121"/>
-    <mergeCell ref="A124:A134"/>
-    <mergeCell ref="A136:A168"/>
-    <mergeCell ref="A171:A183"/>
-    <mergeCell ref="A185:A201"/>
-    <mergeCell ref="A203:A207"/>
-    <mergeCell ref="A209:A214"/>
-    <mergeCell ref="A216:A220"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A48:A57"/>
+    <mergeCell ref="A59:A84"/>
+    <mergeCell ref="A87:A103"/>
+    <mergeCell ref="A105:A124"/>
+    <mergeCell ref="A127:A137"/>
+    <mergeCell ref="A139:A171"/>
+    <mergeCell ref="A174:A186"/>
+    <mergeCell ref="A188:A204"/>
+    <mergeCell ref="A206:A210"/>
+    <mergeCell ref="A212:A217"/>
+    <mergeCell ref="A219:A223"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B11:B21"/>
     <mergeCell ref="B23:B33"/>
     <mergeCell ref="B35:B42"/>
-    <mergeCell ref="B45:B54"/>
-    <mergeCell ref="B56:B67"/>
-    <mergeCell ref="B69:B79"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="B84:B92"/>
-    <mergeCell ref="B93:B100"/>
-    <mergeCell ref="B102:B116"/>
-    <mergeCell ref="B118:B121"/>
-    <mergeCell ref="B124:B134"/>
-    <mergeCell ref="B136:B156"/>
-    <mergeCell ref="B158:B168"/>
-    <mergeCell ref="B171:B175"/>
-    <mergeCell ref="B177:B183"/>
-    <mergeCell ref="B185:B187"/>
-    <mergeCell ref="B189:B191"/>
-    <mergeCell ref="B193:B201"/>
-    <mergeCell ref="B203:B207"/>
-    <mergeCell ref="B209:B214"/>
-    <mergeCell ref="B216:B220"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B48:B57"/>
+    <mergeCell ref="B59:B70"/>
+    <mergeCell ref="B72:B82"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="B87:B95"/>
+    <mergeCell ref="B96:B103"/>
+    <mergeCell ref="B105:B119"/>
+    <mergeCell ref="B121:B124"/>
+    <mergeCell ref="B127:B137"/>
+    <mergeCell ref="B139:B159"/>
+    <mergeCell ref="B161:B171"/>
+    <mergeCell ref="B174:B178"/>
+    <mergeCell ref="B180:B186"/>
+    <mergeCell ref="B188:B190"/>
+    <mergeCell ref="B192:B194"/>
+    <mergeCell ref="B196:B204"/>
+    <mergeCell ref="B206:B210"/>
+    <mergeCell ref="B212:B217"/>
+    <mergeCell ref="B219:B223"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -5594,7 +5617,7 @@
       <c r="A45" s="3"/>
       <c r="B45" s="6"/>
       <c r="C45" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" ht="15.75" spans="1:3">

</xml_diff>

<commit_message>
Added Course Materials - Day 7
</commit_message>
<xml_diff>
--- a/Java Apps @ DXC - Domain - TOC.xlsx
+++ b/Java Apps @ DXC - Domain - TOC.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="449">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -680,28 +680,22 @@
     <t>5. Summary</t>
   </si>
   <si>
-    <t>16. Generics on Methods</t>
-  </si>
-  <si>
-    <t>1. Generic Methods</t>
-  </si>
-  <si>
-    <t>2. Bounded Generics</t>
-  </si>
-  <si>
-    <t>3. Multiple Bounds</t>
-  </si>
-  <si>
-    <t>4. Using Wildcards With Generics</t>
-  </si>
-  <si>
-    <t>5. Type Erasure</t>
-  </si>
-  <si>
-    <t>6. Generics and Primitive Data Types</t>
-  </si>
-  <si>
-    <t>7. Conclusion</t>
+    <t>16. Java's Generic Collections</t>
+  </si>
+  <si>
+    <t>2. The Problem with Arrays</t>
+  </si>
+  <si>
+    <t>3. Lists</t>
+  </si>
+  <si>
+    <t>4. Sets</t>
+  </si>
+  <si>
+    <t>5. Maps</t>
+  </si>
+  <si>
+    <t>6. Conclusions</t>
   </si>
   <si>
     <t>JUnit 4</t>
@@ -812,10 +806,10 @@
     <t>Hands On Exercises - JUnit with Eclipse</t>
   </si>
   <si>
-    <t>Hands On Exercises - Unit test of Counter Class</t>
-  </si>
-  <si>
     <t>Hands On Exercises - Test Suite</t>
+  </si>
+  <si>
+    <t>Hands On Lab 1 - Test Cases and Test Fixtures</t>
   </si>
   <si>
     <t xml:space="preserve">Total # of Days for Core Java </t>
@@ -1515,9 +1509,16 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1531,7 +1532,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1545,26 +1569,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1583,14 +1592,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -1601,9 +1602,25 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1623,15 +1640,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1639,21 +1648,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1692,13 +1686,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1716,37 +1704,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1764,25 +1764,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1800,13 +1806,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1818,37 +1848,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1860,19 +1860,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2005,6 +1999,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -2029,17 +2038,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2052,166 +2057,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="29" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="29" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2264,6 +2258,11 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2660,149 +2659,149 @@
   <sheetData>
     <row r="7" ht="13.5"/>
     <row r="8" ht="13.5" spans="6:9">
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="27" t="s">
+      <c r="I8" s="30" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="6:9">
-      <c r="F9" s="28">
+      <c r="F9" s="31">
         <v>1</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="30">
+      <c r="H9" s="33">
         <v>2</v>
       </c>
-      <c r="I9" s="30">
+      <c r="I9" s="33">
         <v>16</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="6:9">
-      <c r="F10" s="31">
+      <c r="F10" s="34">
         <v>2</v>
       </c>
-      <c r="G10" s="32" t="s">
+      <c r="G10" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="33">
         <v>5</v>
       </c>
-      <c r="I10" s="30">
+      <c r="I10" s="33">
         <v>40</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="6:9">
-      <c r="F11" s="33">
+      <c r="F11" s="36">
         <v>3</v>
       </c>
-      <c r="G11" s="32" t="s">
+      <c r="G11" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="30">
+      <c r="H11" s="33">
         <v>1</v>
       </c>
-      <c r="I11" s="30">
+      <c r="I11" s="33">
         <v>8</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="6:9">
-      <c r="F12" s="31">
+      <c r="F12" s="34">
         <v>4</v>
       </c>
-      <c r="G12" s="29" t="s">
+      <c r="G12" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="30">
+      <c r="H12" s="33">
         <v>1</v>
       </c>
-      <c r="I12" s="30">
+      <c r="I12" s="33">
         <v>8</v>
       </c>
     </row>
     <row r="13" ht="15.75" spans="6:9">
-      <c r="F13" s="31">
+      <c r="F13" s="34">
         <v>5</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="G13" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="30">
+      <c r="H13" s="33">
         <v>1</v>
       </c>
-      <c r="I13" s="30">
+      <c r="I13" s="33">
         <v>8</v>
       </c>
     </row>
     <row r="14" ht="15.75" spans="6:9">
-      <c r="F14" s="34"/>
-      <c r="G14" s="35" t="s">
+      <c r="F14" s="37"/>
+      <c r="G14" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="36" t="s">
+      <c r="H14" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="36" t="s">
+      <c r="I14" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="40" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="38">
+      <c r="A20" s="41">
         <v>1</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="38"/>
-      <c r="B21" s="40" t="s">
+      <c r="A21" s="41"/>
+      <c r="B21" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
     </row>
     <row r="22" ht="26" customHeight="1" spans="1:6">
-      <c r="A22" s="38"/>
-      <c r="B22" s="41" t="s">
+      <c r="A22" s="41"/>
+      <c r="B22" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="42">
+      <c r="A23" s="45">
         <v>2</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2860,14 +2859,14 @@
       <c r="B3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="26" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" ht="10" customHeight="1" spans="1:3">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
     </row>
     <row r="5" ht="56.25" spans="1:3">
       <c r="A5" s="12" t="s">
@@ -2882,7 +2881,7 @@
     </row>
     <row r="6" ht="18.75" spans="1:3">
       <c r="A6" s="12"/>
-      <c r="B6" s="25"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="7"/>
     </row>
     <row r="7" ht="31.5" spans="1:3">
@@ -2892,14 +2891,14 @@
       <c r="B7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="26" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" ht="12" customHeight="1" spans="1:3">
       <c r="A8" s="12"/>
       <c r="B8" s="6"/>
-      <c r="C8" s="23"/>
+      <c r="C8" s="26"/>
     </row>
     <row r="9" ht="15" spans="1:3">
       <c r="A9" s="12"/>
@@ -2927,7 +2926,7 @@
     <row r="12" ht="52" customHeight="1" spans="1:3">
       <c r="A12" s="12"/>
       <c r="B12" s="14"/>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="26" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2974,11 +2973,11 @@
       <c r="C18" s="16"/>
     </row>
     <row r="19" ht="33" customHeight="1" spans="1:3">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
     </row>
     <row r="20" ht="31.5" spans="1:3">
       <c r="A20" s="12" t="s">
@@ -2987,7 +2986,7 @@
       <c r="B20" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="26" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3015,7 +3014,7 @@
     <row r="24" ht="69" customHeight="1" spans="1:3">
       <c r="A24" s="12"/>
       <c r="B24" s="14"/>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="26" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3031,7 +3030,7 @@
       <c r="B26" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="26" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3052,7 +3051,7 @@
     <row r="29" ht="100" customHeight="1" spans="1:3">
       <c r="A29" s="12"/>
       <c r="B29" s="14"/>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="26" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3068,7 +3067,7 @@
       <c r="B31" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="23" t="s">
+      <c r="C31" s="26" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3089,7 +3088,7 @@
     <row r="34" ht="89" customHeight="1" spans="1:3">
       <c r="A34" s="12"/>
       <c r="B34" s="14"/>
-      <c r="C34" s="23" t="s">
+      <c r="C34" s="26" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3099,7 +3098,7 @@
       <c r="C35" s="16"/>
     </row>
     <row r="37" ht="18.75" spans="1:2">
-      <c r="A37" s="22" t="s">
+      <c r="A37" s="25" t="s">
         <v>46</v>
       </c>
       <c r="B37" s="11">
@@ -3107,7 +3106,7 @@
       </c>
     </row>
     <row r="38" ht="18.75" spans="1:2">
-      <c r="A38" s="22" t="s">
+      <c r="A38" s="25" t="s">
         <v>47</v>
       </c>
       <c r="B38" s="11">
@@ -3137,12 +3136,12 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C224"/>
+  <dimension ref="A1:C223"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A136" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C157" sqref="C157"/>
+      <selection pane="bottomLeft" activeCell="E190" sqref="E190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -4407,336 +4406,329 @@
       <c r="B177" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="C177" s="5" t="s">
-        <v>214</v>
+      <c r="C177" s="21" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" s="12"/>
       <c r="B178" s="6"/>
-      <c r="C178" t="s">
-        <v>215</v>
+      <c r="C178" s="22" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="179" ht="15" spans="1:3">
       <c r="A179" s="12"/>
       <c r="B179" s="6"/>
-      <c r="C179" s="5" t="s">
-        <v>216</v>
+      <c r="C179" s="21" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="180" ht="15" spans="1:3">
       <c r="A180" s="12"/>
       <c r="B180" s="6"/>
-      <c r="C180" s="21" t="s">
-        <v>217</v>
+      <c r="C180" s="23" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="181" ht="15" spans="1:3">
       <c r="A181" s="12"/>
       <c r="B181" s="6"/>
-      <c r="C181" s="5" t="s">
-        <v>218</v>
+      <c r="C181" s="21" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="182" ht="15" spans="1:3">
       <c r="A182" s="12"/>
       <c r="B182" s="6"/>
-      <c r="C182" s="5" t="s">
+      <c r="C182" s="21" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="183" ht="18.75" spans="1:3">
+      <c r="A183" s="17"/>
+      <c r="B183" s="20"/>
+      <c r="C183" s="5"/>
+    </row>
+    <row r="184" ht="15" spans="1:3">
+      <c r="A184" s="12" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="183" ht="15" spans="1:3">
-      <c r="A183" s="12"/>
-      <c r="B183" s="6"/>
-      <c r="C183" s="5" t="s">
+      <c r="B184" s="6" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="184" ht="18.75" spans="1:3">
-      <c r="A184" s="17"/>
-      <c r="B184" s="20"/>
-      <c r="C184" s="5"/>
+      <c r="C184" s="24" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="185" ht="15" spans="1:3">
-      <c r="A185" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="B185" s="6" t="s">
+      <c r="A185" s="12"/>
+      <c r="B185" s="6"/>
+      <c r="C185" s="24" t="s">
         <v>222</v>
-      </c>
-      <c r="C185" s="21" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="186" ht="15" spans="1:3">
       <c r="A186" s="12"/>
       <c r="B186" s="6"/>
-      <c r="C186" s="21" t="s">
+      <c r="C186" s="24" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="187" ht="18" spans="1:3">
+      <c r="A187" s="12"/>
+      <c r="B187" s="20"/>
+      <c r="C187" s="24"/>
+    </row>
+    <row r="188" ht="15" spans="1:3">
+      <c r="A188" s="12"/>
+      <c r="B188" s="6" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="187" ht="15" spans="1:3">
-      <c r="A187" s="12"/>
-      <c r="B187" s="6"/>
-      <c r="C187" s="21" t="s">
+      <c r="C188" s="24" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="188" ht="18" spans="1:3">
-      <c r="A188" s="12"/>
-      <c r="B188" s="20"/>
-      <c r="C188" s="21"/>
     </row>
     <row r="189" ht="15" spans="1:3">
       <c r="A189" s="12"/>
-      <c r="B189" s="6" t="s">
+      <c r="B189" s="6"/>
+      <c r="C189" s="24" t="s">
         <v>226</v>
-      </c>
-      <c r="C189" s="21" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="190" ht="15" spans="1:3">
       <c r="A190" s="12"/>
       <c r="B190" s="6"/>
-      <c r="C190" s="21" t="s">
-        <v>228</v>
+      <c r="C190" s="24" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="191" ht="15" spans="1:3">
       <c r="A191" s="12"/>
-      <c r="B191" s="6"/>
-      <c r="C191" s="21" t="s">
-        <v>229</v>
-      </c>
+      <c r="B191" s="7"/>
+      <c r="C191" s="24"/>
     </row>
     <row r="192" ht="15" spans="1:3">
       <c r="A192" s="12"/>
-      <c r="B192" s="7"/>
-      <c r="C192" s="21"/>
+      <c r="B192" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="C192" s="24" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="193" ht="15" spans="1:3">
       <c r="A193" s="12"/>
-      <c r="B193" s="6" t="s">
+      <c r="B193" s="6"/>
+      <c r="C193" s="24" t="s">
         <v>230</v>
-      </c>
-      <c r="C193" s="21" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="194" ht="15" spans="1:3">
       <c r="A194" s="12"/>
       <c r="B194" s="6"/>
-      <c r="C194" s="21" t="s">
-        <v>232</v>
+      <c r="C194" s="24" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="195" ht="15" spans="1:3">
       <c r="A195" s="12"/>
       <c r="B195" s="6"/>
-      <c r="C195" s="21" t="s">
-        <v>233</v>
+      <c r="C195" s="24" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="196" ht="15" spans="1:3">
       <c r="A196" s="12"/>
       <c r="B196" s="6"/>
-      <c r="C196" s="21" t="s">
-        <v>234</v>
+      <c r="C196" s="24" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="197" ht="15" spans="1:3">
       <c r="A197" s="12"/>
       <c r="B197" s="6"/>
-      <c r="C197" s="21" t="s">
-        <v>235</v>
+      <c r="C197" s="24" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="198" ht="15" spans="1:3">
       <c r="A198" s="12"/>
       <c r="B198" s="6"/>
-      <c r="C198" s="21" t="s">
-        <v>236</v>
+      <c r="C198" s="24" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="199" ht="15" spans="1:3">
       <c r="A199" s="12"/>
       <c r="B199" s="6"/>
-      <c r="C199" s="21" t="s">
-        <v>237</v>
+      <c r="C199" s="24" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="200" ht="15" spans="1:3">
       <c r="A200" s="12"/>
       <c r="B200" s="6"/>
-      <c r="C200" s="21" t="s">
+      <c r="C200" s="24" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="201" ht="18.75" spans="1:3">
+      <c r="A201" s="17"/>
+      <c r="B201" s="6"/>
+      <c r="C201" s="24"/>
+    </row>
+    <row r="202" ht="15" spans="1:3">
+      <c r="A202" s="12" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="201" ht="15" spans="1:3">
-      <c r="A201" s="12"/>
-      <c r="B201" s="6"/>
-      <c r="C201" s="21" t="s">
+      <c r="B202" s="6" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="202" ht="18.75" spans="1:3">
-      <c r="A202" s="17"/>
-      <c r="B202" s="6"/>
-      <c r="C202" s="21"/>
+      <c r="C202" s="24" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="203" ht="15" spans="1:3">
-      <c r="A203" s="12" t="s">
-        <v>240</v>
-      </c>
-      <c r="B203" s="6" t="s">
+      <c r="A203" s="12"/>
+      <c r="B203" s="6"/>
+      <c r="C203" s="24" t="s">
         <v>241</v>
-      </c>
-      <c r="C203" s="21" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="204" ht="15" spans="1:3">
       <c r="A204" s="12"/>
       <c r="B204" s="6"/>
-      <c r="C204" s="21" t="s">
-        <v>243</v>
+      <c r="C204" s="24" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="205" ht="15" spans="1:3">
       <c r="A205" s="12"/>
       <c r="B205" s="6"/>
-      <c r="C205" s="21" t="s">
-        <v>244</v>
+      <c r="C205" s="24" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="206" ht="15" spans="1:3">
       <c r="A206" s="12"/>
       <c r="B206" s="6"/>
-      <c r="C206" s="21" t="s">
+      <c r="C206" s="24" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="207" ht="18.75" spans="1:3">
+      <c r="A207" s="17"/>
+      <c r="B207" s="6"/>
+      <c r="C207" s="24"/>
+    </row>
+    <row r="208" ht="15" spans="1:3">
+      <c r="A208" s="12" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="207" ht="15" spans="1:3">
-      <c r="A207" s="12"/>
-      <c r="B207" s="6"/>
-      <c r="C207" s="21" t="s">
+      <c r="B208" s="14" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="208" ht="18.75" spans="1:3">
-      <c r="A208" s="17"/>
-      <c r="B208" s="6"/>
-      <c r="C208" s="21"/>
+      <c r="C208" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="209" ht="15" spans="1:3">
-      <c r="A209" s="12" t="s">
+      <c r="A209" s="12"/>
+      <c r="B209" s="14"/>
+      <c r="C209" s="5" t="s">
         <v>247</v>
-      </c>
-      <c r="B209" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="C209" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="210" ht="15" spans="1:3">
       <c r="A210" s="12"/>
       <c r="B210" s="14"/>
       <c r="C210" s="5" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="211" ht="15" spans="1:3">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="211" ht="15" customHeight="1" spans="1:3">
       <c r="A211" s="12"/>
       <c r="B211" s="14"/>
       <c r="C211" s="5" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="212" ht="15" customHeight="1" spans="1:3">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="212" ht="15" spans="1:3">
       <c r="A212" s="12"/>
       <c r="B212" s="14"/>
       <c r="C212" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="213" ht="15" spans="1:3">
       <c r="A213" s="12"/>
       <c r="B213" s="14"/>
       <c r="C213" s="5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="214" ht="18.75" spans="1:3">
+      <c r="A214" s="12"/>
+      <c r="B214" s="6"/>
+      <c r="C214" s="5"/>
+    </row>
+    <row r="215" ht="15" spans="1:3">
+      <c r="A215" s="12"/>
+      <c r="B215" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C215" s="15" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="214" ht="15" spans="1:3">
-      <c r="A214" s="12"/>
-      <c r="B214" s="14"/>
-      <c r="C214" s="5" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="215" ht="18.75" spans="1:3">
-      <c r="A215" s="12"/>
-      <c r="B215" s="6"/>
-      <c r="C215" s="5"/>
     </row>
     <row r="216" ht="15" spans="1:3">
       <c r="A216" s="12"/>
-      <c r="B216" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C216" s="15" t="s">
-        <v>254</v>
+      <c r="B216" s="14"/>
+      <c r="C216" s="5" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="217" ht="15" spans="1:3">
       <c r="A217" s="12"/>
       <c r="B217" s="14"/>
       <c r="C217" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="218" ht="15" spans="1:3">
       <c r="A218" s="12"/>
       <c r="B218" s="14"/>
       <c r="C218" s="5" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="219" ht="15" spans="1:3">
       <c r="A219" s="12"/>
       <c r="B219" s="14"/>
-      <c r="C219" s="7" t="s">
+      <c r="C219" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="A220" s="16"/>
+      <c r="B220" s="16"/>
+      <c r="C220" s="16"/>
+    </row>
+    <row r="221" s="7" customFormat="1"/>
+    <row r="222" s="7" customFormat="1" ht="18.75" spans="1:2">
+      <c r="A222" s="25" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="220" ht="15" spans="1:3">
-      <c r="A220" s="12"/>
-      <c r="B220" s="14"/>
-      <c r="C220" s="21" t="s">
+      <c r="B222" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="223" ht="18.75" spans="1:2">
+      <c r="A223" s="25" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="221" spans="1:3">
-      <c r="A221" s="16"/>
-      <c r="B221" s="16"/>
-      <c r="C221" s="16"/>
-    </row>
-    <row r="222" s="7" customFormat="1"/>
-    <row r="223" s="7" customFormat="1" ht="18.75" spans="1:2">
-      <c r="A223" s="22" t="s">
-        <v>259</v>
-      </c>
       <c r="B223" s="11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="224" ht="18.75" spans="1:2">
-      <c r="A224" s="22" t="s">
-        <v>260</v>
-      </c>
-      <c r="B224" s="11">
         <v>40</v>
       </c>
     </row>
@@ -4758,11 +4750,11 @@
     <mergeCell ref="A105:A124"/>
     <mergeCell ref="A127:A137"/>
     <mergeCell ref="A139:A168"/>
-    <mergeCell ref="A171:A183"/>
-    <mergeCell ref="A185:A201"/>
-    <mergeCell ref="A203:A207"/>
-    <mergeCell ref="A209:A214"/>
-    <mergeCell ref="A216:A220"/>
+    <mergeCell ref="A171:A182"/>
+    <mergeCell ref="A184:A200"/>
+    <mergeCell ref="A202:A206"/>
+    <mergeCell ref="A208:A213"/>
+    <mergeCell ref="A215:A219"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B11:B21"/>
     <mergeCell ref="B23:B33"/>
@@ -4780,13 +4772,13 @@
     <mergeCell ref="B139:B156"/>
     <mergeCell ref="B158:B168"/>
     <mergeCell ref="B171:B175"/>
-    <mergeCell ref="B177:B183"/>
-    <mergeCell ref="B185:B187"/>
-    <mergeCell ref="B189:B191"/>
-    <mergeCell ref="B193:B201"/>
-    <mergeCell ref="B203:B207"/>
-    <mergeCell ref="B209:B214"/>
-    <mergeCell ref="B216:B220"/>
+    <mergeCell ref="B177:B182"/>
+    <mergeCell ref="B184:B186"/>
+    <mergeCell ref="B188:B190"/>
+    <mergeCell ref="B192:B200"/>
+    <mergeCell ref="B202:B206"/>
+    <mergeCell ref="B208:B213"/>
+    <mergeCell ref="B215:B219"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -4799,7 +4791,7 @@
   <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="B47" sqref="B47:B57"/>
     </sheetView>
@@ -4824,20 +4816,20 @@
     </row>
     <row r="2" ht="24.75" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" ht="15.75" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:3">
@@ -4848,38 +4840,38 @@
     <row r="5" ht="15" spans="1:3">
       <c r="A5" s="3"/>
       <c r="B5" s="6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" ht="15" spans="1:3">
       <c r="A6" s="3"/>
       <c r="B6" s="6"/>
       <c r="C6" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" ht="15" spans="1:3">
       <c r="A7" s="3"/>
       <c r="B7" s="6"/>
       <c r="C7" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:3">
       <c r="A8" s="3"/>
       <c r="B8" s="6"/>
       <c r="C8" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:3">
       <c r="A9" s="3"/>
       <c r="B9" s="6"/>
       <c r="C9" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -4889,17 +4881,17 @@
     <row r="11" ht="15" spans="1:3">
       <c r="A11" s="3"/>
       <c r="B11" s="6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:3">
       <c r="A12" s="3"/>
       <c r="B12" s="6"/>
       <c r="C12" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -4909,45 +4901,45 @@
     <row r="14" ht="15" spans="1:3">
       <c r="A14" s="3"/>
       <c r="B14" s="6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="15" ht="15" spans="1:3">
       <c r="A15" s="3"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" ht="15" spans="1:3">
       <c r="A16" s="3"/>
       <c r="B16" s="6"/>
       <c r="C16" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="17" ht="15" spans="1:3">
       <c r="A17" s="3"/>
       <c r="B17" s="6"/>
       <c r="C17" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="18" ht="15" spans="1:3">
       <c r="A18" s="3"/>
       <c r="B18" s="6"/>
       <c r="C18" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="19" ht="15" spans="1:3">
       <c r="A19" s="3"/>
       <c r="B19" s="6"/>
       <c r="C19" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" ht="15.75" spans="1:3">
@@ -4958,24 +4950,24 @@
     <row r="21" ht="15" spans="1:3">
       <c r="A21" s="3"/>
       <c r="B21" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="22" ht="15" spans="1:3">
       <c r="A22" s="3"/>
       <c r="B22" s="6"/>
       <c r="C22" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="23" ht="15" spans="1:3">
       <c r="A23" s="3"/>
       <c r="B23" s="6"/>
       <c r="C23" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" ht="15.75" spans="1:3">
@@ -4986,17 +4978,17 @@
     <row r="25" ht="15" spans="1:3">
       <c r="A25" s="3"/>
       <c r="B25" s="6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="26" ht="15" spans="1:3">
       <c r="A26" s="3"/>
       <c r="B26" s="6"/>
       <c r="C26" s="5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="27" ht="15.75" spans="1:3">
@@ -5007,38 +4999,38 @@
     <row r="28" ht="15" spans="1:3">
       <c r="A28" s="3"/>
       <c r="B28" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="29" ht="15" spans="1:3">
       <c r="A29" s="3"/>
       <c r="B29" s="6"/>
       <c r="C29" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="30" ht="15" spans="1:3">
       <c r="A30" s="3"/>
       <c r="B30" s="6"/>
       <c r="C30" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="31" ht="15" spans="1:3">
       <c r="A31" s="3"/>
       <c r="B31" s="6"/>
       <c r="C31" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="32" ht="15" spans="1:3">
       <c r="A32" s="3"/>
       <c r="B32" s="6"/>
       <c r="C32" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="33" ht="15.75" spans="1:3">
@@ -5049,84 +5041,84 @@
     <row r="34" ht="15" spans="1:3">
       <c r="A34" s="3"/>
       <c r="B34" s="6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="35" ht="15" spans="1:3">
       <c r="A35" s="3"/>
       <c r="B35" s="6"/>
       <c r="C35" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="36" ht="15" spans="1:3">
       <c r="A36" s="3"/>
       <c r="B36" s="6"/>
       <c r="C36" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="38" ht="15" spans="1:3">
       <c r="A38" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>296</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="39" ht="15" spans="1:3">
       <c r="A39" s="12"/>
       <c r="B39" s="6"/>
       <c r="C39" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="40" ht="15" spans="1:3">
       <c r="A40" s="12"/>
       <c r="B40" s="6"/>
       <c r="C40" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="41" ht="15" spans="1:3">
       <c r="A41" s="12"/>
       <c r="B41" s="6"/>
       <c r="C41" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="42" ht="15" spans="1:3">
       <c r="A42" s="12"/>
       <c r="B42" s="6"/>
       <c r="C42" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="43" ht="15" spans="1:3">
       <c r="A43" s="12"/>
       <c r="B43" s="6"/>
       <c r="C43" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="12"/>
       <c r="B44" s="6"/>
       <c r="C44" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="12"/>
       <c r="B45" s="6"/>
       <c r="C45" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="46" ht="18.75" spans="1:1">
@@ -5134,83 +5126,83 @@
     </row>
     <row r="47" ht="15" spans="1:3">
       <c r="A47" s="12" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="48" ht="15" spans="1:3">
       <c r="A48" s="12"/>
       <c r="B48" s="6"/>
       <c r="C48" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="49" ht="15" spans="1:3">
       <c r="A49" s="12"/>
       <c r="B49" s="6"/>
       <c r="C49" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="50" ht="15" spans="1:3">
       <c r="A50" s="12"/>
       <c r="B50" s="6"/>
       <c r="C50" s="5" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="51" ht="15" spans="1:3">
       <c r="A51" s="12"/>
       <c r="B51" s="6"/>
       <c r="C51" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="52" ht="15" spans="1:3">
       <c r="A52" s="12"/>
       <c r="B52" s="6"/>
       <c r="C52" s="5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="53" ht="15" spans="1:3">
       <c r="A53" s="12"/>
       <c r="B53" s="6"/>
       <c r="C53" s="5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="54" ht="15" spans="1:3">
       <c r="A54" s="12"/>
       <c r="B54" s="6"/>
       <c r="C54" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="55" ht="15" spans="1:3">
       <c r="A55" s="12"/>
       <c r="B55" s="6"/>
       <c r="C55" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="12"/>
       <c r="B56" s="6"/>
       <c r="C56" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="12"/>
       <c r="B57" s="6"/>
       <c r="C57" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="58" ht="7" customHeight="1" spans="1:3">
@@ -5220,7 +5212,7 @@
     </row>
     <row r="60" ht="37.5" spans="1:2">
       <c r="A60" s="10" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B60" s="11">
         <v>1</v>
@@ -5228,7 +5220,7 @@
     </row>
     <row r="61" ht="37.5" spans="1:2">
       <c r="A61" s="10" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B61" s="11">
         <v>8</v>
@@ -5286,20 +5278,20 @@
     </row>
     <row r="2" ht="24.75" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" ht="15.75" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:3">
@@ -5310,10 +5302,10 @@
     <row r="5" ht="15" spans="1:3">
       <c r="A5" s="3"/>
       <c r="B5" s="6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="6" ht="15" spans="1:3">
@@ -5327,49 +5319,49 @@
       <c r="A7" s="3"/>
       <c r="B7" s="6"/>
       <c r="C7" s="5" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:3">
       <c r="A8" s="3"/>
       <c r="B8" s="6"/>
       <c r="C8" s="5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:3">
       <c r="A9" s="3"/>
       <c r="B9" s="6"/>
       <c r="C9" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="10" ht="15" spans="1:3">
       <c r="A10" s="3"/>
       <c r="B10" s="6"/>
       <c r="C10" s="5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="11" ht="15" spans="1:3">
       <c r="A11" s="3"/>
       <c r="B11" s="6"/>
       <c r="C11" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:3">
       <c r="A12" s="3"/>
       <c r="B12" s="6"/>
       <c r="C12" s="5" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:3">
       <c r="A13" s="3"/>
       <c r="B13" s="6"/>
       <c r="C13" s="5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -5379,7 +5371,7 @@
     <row r="15" ht="15" spans="1:3">
       <c r="A15" s="3"/>
       <c r="B15" s="6" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>59</v>
@@ -5389,77 +5381,77 @@
       <c r="A16" s="3"/>
       <c r="B16" s="6"/>
       <c r="C16" s="5" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="17" ht="15" spans="1:3">
       <c r="A17" s="3"/>
       <c r="B17" s="6"/>
       <c r="C17" s="5" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="18" ht="15" spans="1:3">
       <c r="A18" s="3"/>
       <c r="B18" s="6"/>
       <c r="C18" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="19" ht="15" spans="1:3">
       <c r="A19" s="3"/>
       <c r="B19" s="6"/>
       <c r="C19" s="5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="20" ht="15" spans="1:3">
       <c r="A20" s="3"/>
       <c r="B20" s="6"/>
       <c r="C20" s="5" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="21" ht="15" spans="1:3">
       <c r="A21" s="3"/>
       <c r="B21" s="6"/>
       <c r="C21" s="5" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="22" ht="15" spans="1:3">
       <c r="A22" s="3"/>
       <c r="B22" s="6"/>
       <c r="C22" s="5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="23" ht="15" spans="1:3">
       <c r="A23" s="3"/>
       <c r="B23" s="6"/>
       <c r="C23" s="5" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="24" ht="15" spans="1:3">
       <c r="A24" s="3"/>
       <c r="B24" s="6"/>
       <c r="C24" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="25" ht="15" spans="1:3">
       <c r="A25" s="3"/>
       <c r="B25" s="6"/>
       <c r="C25" s="5" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="26" ht="15" spans="1:3">
       <c r="A26" s="3"/>
       <c r="B26" s="6"/>
       <c r="C26" s="5" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="27" ht="15" spans="1:3">
@@ -5469,7 +5461,7 @@
     <row r="28" ht="15" spans="1:3">
       <c r="A28" s="3"/>
       <c r="B28" s="6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>59</v>
@@ -5479,56 +5471,56 @@
       <c r="A29" s="3"/>
       <c r="B29" s="6"/>
       <c r="C29" s="5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="30" ht="15" spans="1:3">
       <c r="A30" s="3"/>
       <c r="B30" s="6"/>
       <c r="C30" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="31" ht="15" spans="1:3">
       <c r="A31" s="3"/>
       <c r="B31" s="6"/>
       <c r="C31" s="5" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="32" ht="15" spans="1:3">
       <c r="A32" s="3"/>
       <c r="B32" s="6"/>
       <c r="C32" s="5" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="33" ht="15" spans="1:3">
       <c r="A33" s="3"/>
       <c r="B33" s="6"/>
       <c r="C33" s="5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="34" ht="15" spans="1:3">
       <c r="A34" s="3"/>
       <c r="B34" s="6"/>
       <c r="C34" s="5" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="35" ht="15" spans="1:3">
       <c r="A35" s="3"/>
       <c r="B35" s="6"/>
       <c r="C35" s="5" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="36" ht="15" spans="1:3">
       <c r="A36" s="3"/>
       <c r="B36" s="6"/>
       <c r="C36" s="5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="37" ht="15.75" spans="1:3">
@@ -5539,7 +5531,7 @@
     <row r="38" ht="15" spans="1:3">
       <c r="A38" s="3"/>
       <c r="B38" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>59</v>
@@ -5549,42 +5541,42 @@
       <c r="A39" s="3"/>
       <c r="B39" s="6"/>
       <c r="C39" s="5" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="40" ht="15" spans="1:3">
       <c r="A40" s="3"/>
       <c r="B40" s="6"/>
       <c r="C40" s="5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="41" ht="15" spans="1:3">
       <c r="A41" s="3"/>
       <c r="B41" s="6"/>
       <c r="C41" s="5" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="42" ht="15" spans="1:3">
       <c r="A42" s="3"/>
       <c r="B42" s="6"/>
       <c r="C42" s="5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="43" ht="15" spans="1:3">
       <c r="A43" s="3"/>
       <c r="B43" s="6"/>
       <c r="C43" s="5" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="44" ht="15" spans="1:3">
       <c r="A44" s="3"/>
       <c r="B44" s="6"/>
       <c r="C44" s="5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="45" ht="15" spans="1:3">
@@ -5602,7 +5594,7 @@
     <row r="47" ht="15" spans="1:3">
       <c r="A47" s="3"/>
       <c r="B47" s="6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>59</v>
@@ -5612,77 +5604,77 @@
       <c r="A48" s="3"/>
       <c r="B48" s="6"/>
       <c r="C48" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="49" ht="15" spans="1:3">
       <c r="A49" s="3"/>
       <c r="B49" s="6"/>
       <c r="C49" s="5" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="50" ht="15" spans="1:3">
       <c r="A50" s="3"/>
       <c r="B50" s="6"/>
       <c r="C50" s="5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="51" ht="15" spans="1:3">
       <c r="A51" s="3"/>
       <c r="B51" s="6"/>
       <c r="C51" s="5" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="52" ht="15" spans="1:3">
       <c r="A52" s="3"/>
       <c r="B52" s="6"/>
       <c r="C52" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="53" ht="15" spans="1:3">
       <c r="A53" s="3"/>
       <c r="B53" s="6"/>
       <c r="C53" s="5" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="54" ht="15" spans="1:3">
       <c r="A54" s="3"/>
       <c r="B54" s="6"/>
       <c r="C54" s="5" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="55" ht="15" spans="1:3">
       <c r="A55" s="3"/>
       <c r="B55" s="6"/>
       <c r="C55" s="5" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="56" ht="15" spans="1:3">
       <c r="A56" s="3"/>
       <c r="B56" s="6"/>
       <c r="C56" s="5" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="57" ht="15" spans="1:3">
       <c r="A57" s="3"/>
       <c r="B57" s="6"/>
       <c r="C57" s="5" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="58" ht="15" spans="1:3">
       <c r="A58" s="3"/>
       <c r="B58" s="6"/>
       <c r="C58" s="5" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="59" ht="15.75" spans="1:3">
@@ -5693,7 +5685,7 @@
     <row r="60" ht="15" spans="1:3">
       <c r="A60" s="3"/>
       <c r="B60" s="6" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>59</v>
@@ -5703,105 +5695,105 @@
       <c r="A61" s="3"/>
       <c r="B61" s="6"/>
       <c r="C61" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="62" ht="15" spans="1:3">
       <c r="A62" s="3"/>
       <c r="B62" s="6"/>
       <c r="C62" s="5" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="63" ht="15" spans="1:3">
       <c r="A63" s="3"/>
       <c r="B63" s="6"/>
       <c r="C63" s="5" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="64" ht="15" spans="1:3">
       <c r="A64" s="3"/>
       <c r="B64" s="6"/>
       <c r="C64" s="5" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="65" ht="15" spans="1:3">
       <c r="A65" s="3"/>
       <c r="B65" s="6"/>
       <c r="C65" s="5" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="66" ht="15" spans="1:3">
       <c r="A66" s="3"/>
       <c r="B66" s="6"/>
       <c r="C66" s="5" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="67" ht="15" spans="1:3">
       <c r="A67" s="3"/>
       <c r="B67" s="6"/>
       <c r="C67" s="5" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="68" ht="15" spans="1:3">
       <c r="A68" s="3"/>
       <c r="B68" s="6"/>
       <c r="C68" s="5" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="69" ht="15" spans="1:3">
       <c r="A69" s="3"/>
       <c r="B69" s="6"/>
       <c r="C69" s="5" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="70" ht="15" spans="1:3">
       <c r="A70" s="3"/>
       <c r="B70" s="6"/>
       <c r="C70" s="5" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="71" ht="15" spans="1:3">
       <c r="A71" s="3"/>
       <c r="B71" s="6"/>
       <c r="C71" s="5" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="72" ht="15" spans="1:3">
       <c r="A72" s="3"/>
       <c r="B72" s="6"/>
       <c r="C72" s="5" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="73" ht="15" spans="1:3">
       <c r="A73" s="3"/>
       <c r="B73" s="6"/>
       <c r="C73" s="5" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="74" ht="15" spans="1:3">
       <c r="A74" s="3"/>
       <c r="B74" s="6"/>
       <c r="C74" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="75" ht="15" spans="1:3">
       <c r="A75" s="3"/>
       <c r="B75" s="6"/>
       <c r="C75" s="5" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="76" ht="7" customHeight="1" spans="1:3">
@@ -5811,7 +5803,7 @@
     </row>
     <row r="78" ht="18.75" spans="1:2">
       <c r="A78" s="10" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B78" s="11">
         <v>1</v>
@@ -5819,7 +5811,7 @@
     </row>
     <row r="79" ht="18.75" spans="1:2">
       <c r="A79" s="10" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B79" s="11">
         <v>8</v>
@@ -5872,20 +5864,20 @@
     </row>
     <row r="2" ht="24.75" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" ht="15.75" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:3">
@@ -5896,52 +5888,52 @@
     <row r="5" ht="15" spans="1:3">
       <c r="A5" s="3"/>
       <c r="B5" s="6" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="6" ht="15" spans="1:3">
       <c r="A6" s="3"/>
       <c r="B6" s="6"/>
       <c r="C6" s="5" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="7" ht="15" spans="1:3">
       <c r="A7" s="3"/>
       <c r="B7" s="6"/>
       <c r="C7" s="5" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:3">
       <c r="A8" s="3"/>
       <c r="B8" s="6"/>
       <c r="C8" s="5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:3">
       <c r="A9" s="3"/>
       <c r="B9" s="6"/>
       <c r="C9" s="5" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="10" ht="15" spans="1:3">
       <c r="A10" s="3"/>
       <c r="B10" s="6"/>
       <c r="C10" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="11" ht="15" spans="1:3">
       <c r="A11" s="3"/>
       <c r="B11" s="6"/>
       <c r="C11" s="5" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -5951,66 +5943,66 @@
     <row r="13" ht="15" spans="1:3">
       <c r="A13" s="3"/>
       <c r="B13" s="6" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="14" ht="15" spans="1:3">
       <c r="A14" s="3"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="15" ht="15" spans="1:3">
       <c r="A15" s="3"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="16" ht="15" spans="1:3">
       <c r="A16" s="3"/>
       <c r="B16" s="6"/>
       <c r="C16" s="5" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="17" ht="15" spans="1:3">
       <c r="A17" s="3"/>
       <c r="B17" s="6"/>
       <c r="C17" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="18" ht="15" spans="1:3">
       <c r="A18" s="3"/>
       <c r="B18" s="6"/>
       <c r="C18" s="5" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="19" ht="15" spans="1:3">
       <c r="A19" s="3"/>
       <c r="B19" s="6"/>
       <c r="C19" s="5" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="20" ht="15" spans="1:3">
       <c r="A20" s="3"/>
       <c r="B20" s="6"/>
       <c r="C20" s="5" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="21" ht="15" spans="1:3">
       <c r="A21" s="3"/>
       <c r="B21" s="6"/>
       <c r="C21" s="5" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="22" ht="15" spans="1:3">
@@ -6020,73 +6012,73 @@
     <row r="23" ht="15" spans="1:3">
       <c r="A23" s="3"/>
       <c r="B23" s="6" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="24" ht="15" spans="1:3">
       <c r="A24" s="3"/>
       <c r="B24" s="6"/>
       <c r="C24" s="5" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="25" ht="15" spans="1:3">
       <c r="A25" s="3"/>
       <c r="B25" s="6"/>
       <c r="C25" s="5" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="26" ht="15" spans="1:3">
       <c r="A26" s="3"/>
       <c r="B26" s="6"/>
       <c r="C26" s="5" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="27" ht="15" spans="1:3">
       <c r="A27" s="3"/>
       <c r="B27" s="6"/>
       <c r="C27" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="28" ht="15" spans="1:3">
       <c r="A28" s="3"/>
       <c r="B28" s="6"/>
       <c r="C28" s="5" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="29" ht="15" spans="1:3">
       <c r="A29" s="3"/>
       <c r="B29" s="6"/>
       <c r="C29" s="5" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="30" ht="15" spans="1:3">
       <c r="A30" s="3"/>
       <c r="B30" s="6"/>
       <c r="C30" s="5" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="31" ht="15" spans="1:3">
       <c r="A31" s="3"/>
       <c r="B31" s="6"/>
       <c r="C31" s="5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="32" ht="15" spans="1:3">
       <c r="A32" s="3"/>
       <c r="B32" s="6"/>
       <c r="C32" s="5" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="33" ht="15.75" spans="1:3">
@@ -6097,45 +6089,45 @@
     <row r="34" ht="15" spans="1:3">
       <c r="A34" s="3"/>
       <c r="B34" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="35" ht="15" spans="1:3">
       <c r="A35" s="3"/>
       <c r="B35" s="6"/>
       <c r="C35" s="5" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="36" ht="15" spans="1:3">
       <c r="A36" s="3"/>
       <c r="B36" s="6"/>
       <c r="C36" s="5" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="37" ht="15" spans="1:3">
       <c r="A37" s="3"/>
       <c r="B37" s="6"/>
       <c r="C37" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="38" ht="15" spans="1:3">
       <c r="A38" s="3"/>
       <c r="B38" s="6"/>
       <c r="C38" s="5" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="39" ht="15" spans="1:3">
       <c r="A39" s="3"/>
       <c r="B39" s="6"/>
       <c r="C39" s="5" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="40" ht="15.75" spans="1:3">
@@ -6146,31 +6138,31 @@
     <row r="41" ht="15" spans="1:3">
       <c r="A41" s="3"/>
       <c r="B41" s="6" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="42" ht="15" spans="1:3">
       <c r="A42" s="3"/>
       <c r="B42" s="6"/>
       <c r="C42" s="5" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="43" ht="15" spans="1:3">
       <c r="A43" s="3"/>
       <c r="B43" s="6"/>
       <c r="C43" s="5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="44" ht="15" spans="1:3">
       <c r="A44" s="3"/>
       <c r="B44" s="6"/>
       <c r="C44" s="5" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="45" ht="15.75" spans="1:3">
@@ -6181,31 +6173,31 @@
     <row r="46" ht="15" spans="1:3">
       <c r="A46" s="3"/>
       <c r="B46" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="47" ht="15" spans="1:3">
       <c r="A47" s="3"/>
       <c r="B47" s="6"/>
       <c r="C47" s="5" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="48" ht="15" spans="1:3">
       <c r="A48" s="3"/>
       <c r="B48" s="6"/>
       <c r="C48" s="5" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="49" ht="15" spans="1:3">
       <c r="A49" s="3"/>
       <c r="B49" s="6"/>
       <c r="C49" s="5" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="50" ht="15.75" spans="1:3">
@@ -6216,52 +6208,52 @@
     <row r="51" ht="15" spans="1:3">
       <c r="A51" s="3"/>
       <c r="B51" s="6" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="52" ht="15" spans="1:3">
       <c r="A52" s="3"/>
       <c r="B52" s="6"/>
       <c r="C52" s="5" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="53" ht="15" spans="1:3">
       <c r="A53" s="3"/>
       <c r="B53" s="6"/>
       <c r="C53" s="5" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="54" ht="15" spans="1:3">
       <c r="A54" s="3"/>
       <c r="B54" s="6"/>
       <c r="C54" s="5" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="55" ht="15" spans="1:3">
       <c r="A55" s="3"/>
       <c r="B55" s="6"/>
       <c r="C55" s="5" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="56" ht="15" spans="1:3">
       <c r="A56" s="3"/>
       <c r="B56" s="6"/>
       <c r="C56" s="5" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="57" ht="15" spans="1:3">
       <c r="A57" s="3"/>
       <c r="B57" s="6"/>
       <c r="C57" s="5" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="58" ht="15.75" spans="1:3">
@@ -6272,38 +6264,38 @@
     <row r="59" ht="15" spans="1:3">
       <c r="A59" s="3"/>
       <c r="B59" s="6" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="60" ht="15" spans="1:3">
       <c r="A60" s="3"/>
       <c r="B60" s="6"/>
       <c r="C60" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="61" ht="15" spans="1:3">
       <c r="A61" s="3"/>
       <c r="B61" s="6"/>
       <c r="C61" s="5" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="62" ht="15" spans="1:3">
       <c r="A62" s="3"/>
       <c r="B62" s="6"/>
       <c r="C62" s="5" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="63" ht="15" spans="1:3">
       <c r="A63" s="3"/>
       <c r="B63" s="6"/>
       <c r="C63" s="5" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="64" ht="7" customHeight="1" spans="1:3">
@@ -6313,7 +6305,7 @@
     </row>
     <row r="66" ht="37.5" spans="1:2">
       <c r="A66" s="10" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B66" s="11">
         <v>1</v>
@@ -6321,7 +6313,7 @@
     </row>
     <row r="67" ht="37.5" spans="1:2">
       <c r="A67" s="10" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B67" s="11">
         <v>8</v>

</xml_diff>

<commit_message>
Added Course Materials - Day 9
</commit_message>
<xml_diff>
--- a/Java Apps @ DXC - Domain - TOC.xlsx
+++ b/Java Apps @ DXC - Domain - TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" activeTab="2"/>
+    <workbookView windowWidth="20490" windowHeight="7815" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="7" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="449">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -932,25 +932,22 @@
     <t>1. Introduction to SOAP</t>
   </si>
   <si>
-    <t>2. Demo : SOAP Web Service Setup</t>
-  </si>
-  <si>
-    <t>3. Contract last or Bottom up approach</t>
-  </si>
-  <si>
-    <t>4. Contract first or Top Down Approach</t>
-  </si>
-  <si>
-    <t>5.  Demo : SOAP Web Service</t>
-  </si>
-  <si>
-    <t>6.  Demo : SOAP Web Service Client</t>
-  </si>
-  <si>
-    <t>7. SOAP Web Service Test</t>
-  </si>
-  <si>
-    <t>8. SOAP Web Service WSDL and Configs</t>
+    <t>2. Features of SOAP</t>
+  </si>
+  <si>
+    <t>3. SOAP Schema</t>
+  </si>
+  <si>
+    <t>4. SOAP Request and Response</t>
+  </si>
+  <si>
+    <t>5.  Fault Code</t>
+  </si>
+  <si>
+    <t>6.  UDDI</t>
+  </si>
+  <si>
+    <t>7. SOAP Service Styles</t>
   </si>
   <si>
     <t>Restful  Webservices in Java</t>
@@ -959,34 +956,37 @@
     <t>10. Restful Webservices in Java</t>
   </si>
   <si>
-    <t>2. Java RESTful Web Services API</t>
-  </si>
-  <si>
-    <t>3. Restful Web Services Annotations</t>
+    <t>1. Introduction to REST</t>
+  </si>
+  <si>
+    <t>2. Java RESTful Architectural Style</t>
+  </si>
+  <si>
+    <t>3. Resources</t>
   </si>
   <si>
     <t>4. Restful Web Services and SOAP</t>
   </si>
   <si>
-    <t>5.  REST API Implementations</t>
-  </si>
-  <si>
-    <t>6.  Demo : Jersey Restful Web Services</t>
-  </si>
-  <si>
-    <t>7. REST Demo Model Classes</t>
-  </si>
-  <si>
-    <t>8. REST Demo Services</t>
-  </si>
-  <si>
-    <t>9. Restful Web Services Test</t>
-  </si>
-  <si>
-    <t>10. Demo : RESTEasy RESTful Web Services</t>
-  </si>
-  <si>
-    <t>11. RESTEasy Web Services Test</t>
+    <t>5.  Request and Responses</t>
+  </si>
+  <si>
+    <t>6.  URI Examples</t>
+  </si>
+  <si>
+    <t>7. REST  Characteristics</t>
+  </si>
+  <si>
+    <t>8. HTTP Methods</t>
+  </si>
+  <si>
+    <t>9. CRUD Operations MApped To HTTP Methods In RESTful  Web Services</t>
+  </si>
+  <si>
+    <t>10. Status Codes</t>
+  </si>
+  <si>
+    <t>11. Constraints or Principles</t>
   </si>
   <si>
     <t>Total # of Days for Servlets, JSPs and Web Services</t>
@@ -1393,9 +1393,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="35">
@@ -1510,21 +1510,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1532,7 +1517,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1546,16 +1547,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1592,6 +1593,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -1602,25 +1611,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1638,16 +1631,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1686,13 +1686,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1704,13 +1698,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1734,13 +1740,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1758,61 +1854,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1824,49 +1866,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1960,6 +1960,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1999,21 +2029,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -2023,17 +2038,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2048,27 +2057,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -2081,131 +2081,131 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="20" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="19" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2238,6 +2238,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2258,14 +2261,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2659,149 +2654,149 @@
   <sheetData>
     <row r="7" ht="13.5"/>
     <row r="8" ht="13.5" spans="6:9">
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="30" t="s">
+      <c r="I8" s="27" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="6:9">
-      <c r="F9" s="31">
+      <c r="F9" s="28">
         <v>1</v>
       </c>
-      <c r="G9" s="32" t="s">
+      <c r="G9" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="33">
+      <c r="H9" s="30">
         <v>2</v>
       </c>
-      <c r="I9" s="33">
+      <c r="I9" s="30">
         <v>16</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="6:9">
-      <c r="F10" s="34">
+      <c r="F10" s="31">
         <v>2</v>
       </c>
-      <c r="G10" s="35" t="s">
+      <c r="G10" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="33">
+      <c r="H10" s="30">
         <v>5</v>
       </c>
-      <c r="I10" s="33">
+      <c r="I10" s="30">
         <v>40</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="6:9">
-      <c r="F11" s="36">
+      <c r="F11" s="33">
         <v>3</v>
       </c>
-      <c r="G11" s="35" t="s">
+      <c r="G11" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="33">
+      <c r="H11" s="30">
         <v>1</v>
       </c>
-      <c r="I11" s="33">
+      <c r="I11" s="30">
         <v>8</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="6:9">
-      <c r="F12" s="34">
+      <c r="F12" s="31">
         <v>4</v>
       </c>
-      <c r="G12" s="32" t="s">
+      <c r="G12" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="33">
+      <c r="H12" s="30">
         <v>1</v>
       </c>
-      <c r="I12" s="33">
+      <c r="I12" s="30">
         <v>8</v>
       </c>
     </row>
     <row r="13" ht="15.75" spans="6:9">
-      <c r="F13" s="34">
+      <c r="F13" s="31">
         <v>5</v>
       </c>
-      <c r="G13" s="32" t="s">
+      <c r="G13" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="33">
+      <c r="H13" s="30">
         <v>1</v>
       </c>
-      <c r="I13" s="33">
+      <c r="I13" s="30">
         <v>8</v>
       </c>
     </row>
     <row r="14" ht="15.75" spans="6:9">
-      <c r="F14" s="37"/>
-      <c r="G14" s="38" t="s">
+      <c r="F14" s="34"/>
+      <c r="G14" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="39" t="s">
+      <c r="H14" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="39" t="s">
+      <c r="I14" s="36" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="37" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="41">
+      <c r="A20" s="38">
         <v>1</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="41"/>
-      <c r="B21" s="43" t="s">
+      <c r="A21" s="38"/>
+      <c r="B21" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
     </row>
     <row r="22" ht="26" customHeight="1" spans="1:6">
-      <c r="A22" s="41"/>
-      <c r="B22" s="44" t="s">
+      <c r="A22" s="38"/>
+      <c r="B22" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="44"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="45">
+      <c r="A23" s="42">
         <v>2</v>
       </c>
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2859,14 +2854,14 @@
       <c r="B3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="23" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" ht="10" customHeight="1" spans="1:3">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
     </row>
     <row r="5" ht="56.25" spans="1:3">
       <c r="A5" s="12" t="s">
@@ -2875,13 +2870,13 @@
       <c r="B5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" ht="18.75" spans="1:3">
       <c r="A6" s="12"/>
-      <c r="B6" s="28"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="7"/>
     </row>
     <row r="7" ht="31.5" spans="1:3">
@@ -2891,48 +2886,48 @@
       <c r="B7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="23" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" ht="12" customHeight="1" spans="1:3">
       <c r="A8" s="12"/>
       <c r="B8" s="6"/>
-      <c r="C8" s="26"/>
+      <c r="C8" s="23"/>
     </row>
     <row r="9" ht="15" spans="1:3">
       <c r="A9" s="12"/>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="16" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" ht="15" spans="1:3">
       <c r="A10" s="12"/>
-      <c r="B10" s="14"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" ht="15" spans="1:3">
       <c r="A11" s="12"/>
-      <c r="B11" s="14"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" ht="52" customHeight="1" spans="1:3">
       <c r="A12" s="12"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="26" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="23" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" ht="12" customHeight="1" spans="1:3">
       <c r="A13" s="12"/>
-      <c r="B13" s="14"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="5"/>
     </row>
     <row r="14" ht="15.75" spans="1:3">
@@ -2953,31 +2948,31 @@
     </row>
     <row r="16" ht="15" spans="1:3">
       <c r="A16" s="12"/>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="16" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" ht="15" spans="1:3">
       <c r="A17" s="12"/>
-      <c r="B17" s="14"/>
+      <c r="B17" s="15"/>
       <c r="C17" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" ht="8" customHeight="1" spans="1:3">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
     </row>
     <row r="19" ht="33" customHeight="1" spans="1:3">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
     </row>
     <row r="20" ht="31.5" spans="1:3">
       <c r="A20" s="12" t="s">
@@ -2986,7 +2981,7 @@
       <c r="B20" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="23" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2997,30 +2992,30 @@
     </row>
     <row r="22" ht="15" spans="1:3">
       <c r="A22" s="12"/>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="16" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="23" ht="15" spans="1:3">
       <c r="A23" s="12"/>
-      <c r="B23" s="14"/>
+      <c r="B23" s="15"/>
       <c r="C23" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="24" ht="69" customHeight="1" spans="1:3">
       <c r="A24" s="12"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="26" t="s">
+      <c r="B24" s="15"/>
+      <c r="C24" s="23" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="25" ht="9" customHeight="1" spans="1:3">
       <c r="A25" s="12"/>
-      <c r="B25" s="14"/>
+      <c r="B25" s="15"/>
       <c r="C25" s="5"/>
     </row>
     <row r="26" ht="38" customHeight="1" spans="1:3">
@@ -3030,7 +3025,7 @@
       <c r="B26" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="23" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3041,17 +3036,17 @@
     </row>
     <row r="28" ht="15" spans="1:3">
       <c r="A28" s="12"/>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="16" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="29" ht="100" customHeight="1" spans="1:3">
       <c r="A29" s="12"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="26" t="s">
+      <c r="B29" s="15"/>
+      <c r="C29" s="23" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3067,7 +3062,7 @@
       <c r="B31" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="26" t="s">
+      <c r="C31" s="23" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3078,27 +3073,27 @@
     </row>
     <row r="33" ht="13" customHeight="1" spans="1:3">
       <c r="A33" s="12"/>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="16" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="34" ht="89" customHeight="1" spans="1:3">
       <c r="A34" s="12"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="26" t="s">
+      <c r="B34" s="15"/>
+      <c r="C34" s="23" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="16"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="16"/>
+      <c r="A35" s="17"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
     </row>
     <row r="37" ht="18.75" spans="1:2">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="22" t="s">
         <v>46</v>
       </c>
       <c r="B37" s="11">
@@ -3106,7 +3101,7 @@
       </c>
     </row>
     <row r="38" ht="18.75" spans="1:2">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="22" t="s">
         <v>47</v>
       </c>
       <c r="B38" s="11">
@@ -3138,8 +3133,8 @@
   <sheetPr/>
   <dimension ref="A1:C223"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A181" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="E190" sqref="E190"/>
     </sheetView>
@@ -3176,14 +3171,14 @@
       <c r="B3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" ht="18.75" spans="1:3">
       <c r="A4" s="12"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="13"/>
+      <c r="C4" s="14"/>
     </row>
     <row r="5" ht="15.75" spans="1:3">
       <c r="A5" s="12"/>
@@ -3466,24 +3461,24 @@
     </row>
     <row r="44" ht="15" spans="1:3">
       <c r="A44" s="12"/>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C44" s="16" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="45" ht="15" spans="1:3">
       <c r="A45" s="12"/>
-      <c r="B45" s="14"/>
+      <c r="B45" s="15"/>
       <c r="C45" s="5" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="46" ht="9" customHeight="1" spans="1:3">
-      <c r="A46" s="16"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="16"/>
+      <c r="A46" s="17"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
     </row>
     <row r="47" ht="24.75" spans="1:3">
       <c r="A47" s="2" t="s">
@@ -3739,24 +3734,24 @@
     </row>
     <row r="83" ht="15" spans="1:3">
       <c r="A83" s="12"/>
-      <c r="B83" s="14" t="s">
+      <c r="B83" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C83" s="15" t="s">
+      <c r="C83" s="16" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="84" ht="15" spans="1:3">
       <c r="A84" s="12"/>
-      <c r="B84" s="14"/>
+      <c r="B84" s="15"/>
       <c r="C84" s="5" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="85" ht="9" customHeight="1" spans="1:3">
-      <c r="A85" s="16"/>
-      <c r="B85" s="16"/>
-      <c r="C85" s="16"/>
+      <c r="A85" s="17"/>
+      <c r="B85" s="17"/>
+      <c r="C85" s="17"/>
     </row>
     <row r="86" ht="24.75" spans="1:3">
       <c r="A86" s="2" t="s">
@@ -4005,38 +4000,38 @@
     </row>
     <row r="121" ht="15" spans="1:3">
       <c r="A121" s="12"/>
-      <c r="B121" s="14" t="s">
+      <c r="B121" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C121" s="15" t="s">
+      <c r="C121" s="16" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="122" ht="15" spans="1:3">
       <c r="A122" s="12"/>
-      <c r="B122" s="14"/>
+      <c r="B122" s="15"/>
       <c r="C122" s="5" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="123" ht="15" spans="1:3">
       <c r="A123" s="12"/>
-      <c r="B123" s="14"/>
+      <c r="B123" s="15"/>
       <c r="C123" s="5" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="124" ht="15" spans="1:3">
       <c r="A124" s="12"/>
-      <c r="B124" s="14"/>
+      <c r="B124" s="15"/>
       <c r="C124" s="5" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="125" ht="9" customHeight="1" spans="1:3">
-      <c r="A125" s="16"/>
-      <c r="B125" s="16"/>
-      <c r="C125" s="16"/>
+      <c r="A125" s="17"/>
+      <c r="B125" s="17"/>
+      <c r="C125" s="17"/>
     </row>
     <row r="126" ht="24" customHeight="1" spans="1:3">
       <c r="A126" s="2" t="s">
@@ -4127,8 +4122,8 @@
       </c>
     </row>
     <row r="138" ht="11" customHeight="1" spans="1:3">
-      <c r="A138" s="17"/>
-      <c r="B138" s="18"/>
+      <c r="A138" s="18"/>
+      <c r="B138" s="19"/>
       <c r="C138" s="5"/>
     </row>
     <row r="139" ht="15" spans="1:3">
@@ -4173,182 +4168,182 @@
     <row r="144" ht="15" spans="1:3">
       <c r="A144" s="12"/>
       <c r="B144" s="6"/>
-      <c r="C144" s="19" t="s">
+      <c r="C144" s="20" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="145" ht="21" customHeight="1" spans="1:3">
       <c r="A145" s="12"/>
       <c r="B145" s="6"/>
-      <c r="C145" s="19" t="s">
+      <c r="C145" s="20" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="146" ht="15" spans="1:3">
       <c r="A146" s="12"/>
       <c r="B146" s="6"/>
-      <c r="C146" s="19" t="s">
+      <c r="C146" s="20" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="147" ht="15" spans="1:3">
       <c r="A147" s="12"/>
       <c r="B147" s="6"/>
-      <c r="C147" s="19" t="s">
+      <c r="C147" s="20" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="148" ht="15" spans="1:3">
       <c r="A148" s="12"/>
       <c r="B148" s="6"/>
-      <c r="C148" s="19" t="s">
+      <c r="C148" s="20" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="149" ht="15" spans="1:3">
       <c r="A149" s="12"/>
       <c r="B149" s="6"/>
-      <c r="C149" s="19" t="s">
+      <c r="C149" s="20" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="150" ht="15" spans="1:3">
       <c r="A150" s="12"/>
       <c r="B150" s="6"/>
-      <c r="C150" s="19" t="s">
+      <c r="C150" s="20" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="151" ht="15" spans="1:3">
       <c r="A151" s="12"/>
       <c r="B151" s="6"/>
-      <c r="C151" s="19" t="s">
+      <c r="C151" s="20" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="152" ht="15" spans="1:3">
       <c r="A152" s="12"/>
       <c r="B152" s="6"/>
-      <c r="C152" s="19" t="s">
+      <c r="C152" s="20" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="153" ht="15" spans="1:3">
       <c r="A153" s="12"/>
       <c r="B153" s="6"/>
-      <c r="C153" s="19" t="s">
+      <c r="C153" s="20" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="154" ht="15" spans="1:3">
       <c r="A154" s="12"/>
       <c r="B154" s="6"/>
-      <c r="C154" s="19" t="s">
+      <c r="C154" s="20" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="155" ht="15" spans="1:3">
       <c r="A155" s="12"/>
       <c r="B155" s="6"/>
-      <c r="C155" s="19" t="s">
+      <c r="C155" s="20" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="156" ht="15" spans="1:3">
       <c r="A156" s="12"/>
       <c r="B156" s="6"/>
-      <c r="C156" s="19" t="s">
+      <c r="C156" s="20" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="157" ht="15.75" spans="1:3">
       <c r="A157" s="12"/>
       <c r="B157" s="4"/>
-      <c r="C157" s="19"/>
+      <c r="C157" s="20"/>
     </row>
     <row r="158" ht="15" spans="1:3">
       <c r="A158" s="12"/>
-      <c r="B158" s="14" t="s">
+      <c r="B158" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C158" s="15" t="s">
+      <c r="C158" s="16" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="159" ht="15" spans="1:3">
       <c r="A159" s="12"/>
-      <c r="B159" s="14"/>
+      <c r="B159" s="15"/>
       <c r="C159" s="5" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="160" ht="15" spans="1:3">
       <c r="A160" s="12"/>
-      <c r="B160" s="14"/>
+      <c r="B160" s="15"/>
       <c r="C160" s="5" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="161" ht="15" spans="1:3">
       <c r="A161" s="12"/>
-      <c r="B161" s="14"/>
+      <c r="B161" s="15"/>
       <c r="C161" s="5" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="162" ht="15" spans="1:3">
       <c r="A162" s="12"/>
-      <c r="B162" s="14"/>
-      <c r="C162" s="15" t="s">
+      <c r="B162" s="15"/>
+      <c r="C162" s="16" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="163" ht="15" spans="1:3">
       <c r="A163" s="12"/>
-      <c r="B163" s="14"/>
+      <c r="B163" s="15"/>
       <c r="C163" s="5" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="164" ht="15" spans="1:3">
       <c r="A164" s="12"/>
-      <c r="B164" s="14"/>
+      <c r="B164" s="15"/>
       <c r="C164" s="5" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="165" ht="15" spans="1:3">
       <c r="A165" s="12"/>
-      <c r="B165" s="14"/>
+      <c r="B165" s="15"/>
       <c r="C165" s="5" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="166" ht="15" spans="1:3">
       <c r="A166" s="12"/>
-      <c r="B166" s="14"/>
+      <c r="B166" s="15"/>
       <c r="C166" s="5" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="167" ht="15" spans="1:3">
       <c r="A167" s="12"/>
-      <c r="B167" s="14"/>
+      <c r="B167" s="15"/>
       <c r="C167" s="5" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="168" ht="15" spans="1:3">
       <c r="A168" s="12"/>
-      <c r="B168" s="14"/>
+      <c r="B168" s="15"/>
       <c r="C168" s="5" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="169" ht="9" customHeight="1" spans="1:3">
-      <c r="A169" s="16"/>
-      <c r="B169" s="16"/>
-      <c r="C169" s="16"/>
+      <c r="A169" s="17"/>
+      <c r="B169" s="17"/>
+      <c r="C169" s="17"/>
     </row>
     <row r="170" ht="27" customHeight="1" spans="1:3">
       <c r="A170" s="2" t="s">
@@ -4398,7 +4393,7 @@
     </row>
     <row r="176" ht="18" spans="1:3">
       <c r="A176" s="12"/>
-      <c r="B176" s="20"/>
+      <c r="B176" s="21"/>
       <c r="C176" s="7"/>
     </row>
     <row r="177" ht="15" spans="1:3">
@@ -4406,48 +4401,48 @@
       <c r="B177" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="C177" s="21" t="s">
+      <c r="C177" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" s="12"/>
       <c r="B178" s="6"/>
-      <c r="C178" s="22" t="s">
+      <c r="C178" s="7" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="179" ht="15" spans="1:3">
       <c r="A179" s="12"/>
       <c r="B179" s="6"/>
-      <c r="C179" s="21" t="s">
+      <c r="C179" s="5" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="180" ht="15" spans="1:3">
       <c r="A180" s="12"/>
       <c r="B180" s="6"/>
-      <c r="C180" s="23" t="s">
+      <c r="C180" s="13" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="181" ht="15" spans="1:3">
       <c r="A181" s="12"/>
       <c r="B181" s="6"/>
-      <c r="C181" s="21" t="s">
+      <c r="C181" s="5" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="182" ht="15" spans="1:3">
       <c r="A182" s="12"/>
       <c r="B182" s="6"/>
-      <c r="C182" s="21" t="s">
+      <c r="C182" s="5" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="183" ht="18.75" spans="1:3">
-      <c r="A183" s="17"/>
-      <c r="B183" s="20"/>
+      <c r="A183" s="18"/>
+      <c r="B183" s="21"/>
       <c r="C183" s="5"/>
     </row>
     <row r="184" ht="15" spans="1:3">
@@ -4457,126 +4452,126 @@
       <c r="B184" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="C184" s="24" t="s">
+      <c r="C184" s="13" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="185" ht="15" spans="1:3">
       <c r="A185" s="12"/>
       <c r="B185" s="6"/>
-      <c r="C185" s="24" t="s">
+      <c r="C185" s="13" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="186" ht="15" spans="1:3">
       <c r="A186" s="12"/>
       <c r="B186" s="6"/>
-      <c r="C186" s="24" t="s">
+      <c r="C186" s="13" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="187" ht="18" spans="1:3">
       <c r="A187" s="12"/>
-      <c r="B187" s="20"/>
-      <c r="C187" s="24"/>
+      <c r="B187" s="21"/>
+      <c r="C187" s="13"/>
     </row>
     <row r="188" ht="15" spans="1:3">
       <c r="A188" s="12"/>
       <c r="B188" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="C188" s="24" t="s">
+      <c r="C188" s="13" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="189" ht="15" spans="1:3">
       <c r="A189" s="12"/>
       <c r="B189" s="6"/>
-      <c r="C189" s="24" t="s">
+      <c r="C189" s="13" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="190" ht="15" spans="1:3">
       <c r="A190" s="12"/>
       <c r="B190" s="6"/>
-      <c r="C190" s="24" t="s">
+      <c r="C190" s="13" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="191" ht="15" spans="1:3">
       <c r="A191" s="12"/>
       <c r="B191" s="7"/>
-      <c r="C191" s="24"/>
+      <c r="C191" s="13"/>
     </row>
     <row r="192" ht="15" spans="1:3">
       <c r="A192" s="12"/>
       <c r="B192" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="C192" s="24" t="s">
+      <c r="C192" s="13" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="193" ht="15" spans="1:3">
       <c r="A193" s="12"/>
       <c r="B193" s="6"/>
-      <c r="C193" s="24" t="s">
+      <c r="C193" s="13" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="194" ht="15" spans="1:3">
       <c r="A194" s="12"/>
       <c r="B194" s="6"/>
-      <c r="C194" s="24" t="s">
+      <c r="C194" s="13" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="195" ht="15" spans="1:3">
       <c r="A195" s="12"/>
       <c r="B195" s="6"/>
-      <c r="C195" s="24" t="s">
+      <c r="C195" s="13" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="196" ht="15" spans="1:3">
       <c r="A196" s="12"/>
       <c r="B196" s="6"/>
-      <c r="C196" s="24" t="s">
+      <c r="C196" s="13" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="197" ht="15" spans="1:3">
       <c r="A197" s="12"/>
       <c r="B197" s="6"/>
-      <c r="C197" s="24" t="s">
+      <c r="C197" s="13" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="198" ht="15" spans="1:3">
       <c r="A198" s="12"/>
       <c r="B198" s="6"/>
-      <c r="C198" s="24" t="s">
+      <c r="C198" s="13" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="199" ht="15" spans="1:3">
       <c r="A199" s="12"/>
       <c r="B199" s="6"/>
-      <c r="C199" s="24" t="s">
+      <c r="C199" s="13" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="200" ht="15" spans="1:3">
       <c r="A200" s="12"/>
       <c r="B200" s="6"/>
-      <c r="C200" s="24" t="s">
+      <c r="C200" s="13" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="201" ht="18.75" spans="1:3">
-      <c r="A201" s="17"/>
+      <c r="A201" s="18"/>
       <c r="B201" s="6"/>
-      <c r="C201" s="24"/>
+      <c r="C201" s="13"/>
     </row>
     <row r="202" ht="15" spans="1:3">
       <c r="A202" s="12" t="s">
@@ -4585,48 +4580,48 @@
       <c r="B202" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="C202" s="24" t="s">
+      <c r="C202" s="13" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="203" ht="15" spans="1:3">
       <c r="A203" s="12"/>
       <c r="B203" s="6"/>
-      <c r="C203" s="24" t="s">
+      <c r="C203" s="13" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="204" ht="15" spans="1:3">
       <c r="A204" s="12"/>
       <c r="B204" s="6"/>
-      <c r="C204" s="24" t="s">
+      <c r="C204" s="13" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="205" ht="15" spans="1:3">
       <c r="A205" s="12"/>
       <c r="B205" s="6"/>
-      <c r="C205" s="24" t="s">
+      <c r="C205" s="13" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="206" ht="15" spans="1:3">
       <c r="A206" s="12"/>
       <c r="B206" s="6"/>
-      <c r="C206" s="24" t="s">
+      <c r="C206" s="13" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="207" ht="18.75" spans="1:3">
-      <c r="A207" s="17"/>
+      <c r="A207" s="18"/>
       <c r="B207" s="6"/>
-      <c r="C207" s="24"/>
+      <c r="C207" s="13"/>
     </row>
     <row r="208" ht="15" spans="1:3">
       <c r="A208" s="12" t="s">
         <v>245</v>
       </c>
-      <c r="B208" s="14" t="s">
+      <c r="B208" s="15" t="s">
         <v>246</v>
       </c>
       <c r="C208" s="5" t="s">
@@ -4635,35 +4630,35 @@
     </row>
     <row r="209" ht="15" spans="1:3">
       <c r="A209" s="12"/>
-      <c r="B209" s="14"/>
+      <c r="B209" s="15"/>
       <c r="C209" s="5" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="210" ht="15" spans="1:3">
       <c r="A210" s="12"/>
-      <c r="B210" s="14"/>
+      <c r="B210" s="15"/>
       <c r="C210" s="5" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="211" ht="15" customHeight="1" spans="1:3">
       <c r="A211" s="12"/>
-      <c r="B211" s="14"/>
+      <c r="B211" s="15"/>
       <c r="C211" s="5" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="212" ht="15" spans="1:3">
       <c r="A212" s="12"/>
-      <c r="B212" s="14"/>
+      <c r="B212" s="15"/>
       <c r="C212" s="5" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="213" ht="15" spans="1:3">
       <c r="A213" s="12"/>
-      <c r="B213" s="14"/>
+      <c r="B213" s="15"/>
       <c r="C213" s="5" t="s">
         <v>251</v>
       </c>
@@ -4675,49 +4670,49 @@
     </row>
     <row r="215" ht="15" spans="1:3">
       <c r="A215" s="12"/>
-      <c r="B215" s="14" t="s">
+      <c r="B215" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C215" s="15" t="s">
+      <c r="C215" s="16" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="216" ht="15" spans="1:3">
       <c r="A216" s="12"/>
-      <c r="B216" s="14"/>
+      <c r="B216" s="15"/>
       <c r="C216" s="5" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="217" ht="15" spans="1:3">
       <c r="A217" s="12"/>
-      <c r="B217" s="14"/>
+      <c r="B217" s="15"/>
       <c r="C217" s="5" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="218" ht="15" spans="1:3">
       <c r="A218" s="12"/>
-      <c r="B218" s="14"/>
+      <c r="B218" s="15"/>
       <c r="C218" s="5" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="219" ht="15" spans="1:3">
       <c r="A219" s="12"/>
-      <c r="B219" s="14"/>
+      <c r="B219" s="15"/>
       <c r="C219" s="5" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="220" spans="1:3">
-      <c r="A220" s="16"/>
-      <c r="B220" s="16"/>
-      <c r="C220" s="16"/>
+      <c r="A220" s="17"/>
+      <c r="B220" s="17"/>
+      <c r="C220" s="17"/>
     </row>
     <row r="221" s="7" customFormat="1"/>
     <row r="222" s="7" customFormat="1" ht="18.75" spans="1:2">
-      <c r="A222" s="25" t="s">
+      <c r="A222" s="22" t="s">
         <v>257</v>
       </c>
       <c r="B222" s="11">
@@ -4725,7 +4720,7 @@
       </c>
     </row>
     <row r="223" ht="18.75" spans="1:2">
-      <c r="A223" s="25" t="s">
+      <c r="A223" s="22" t="s">
         <v>258</v>
       </c>
       <c r="B223" s="11">
@@ -4788,12 +4783,12 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B47" sqref="B47:B57"/>
+      <selection pane="bottomLeft" activeCell="C46" sqref="C46:C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -5114,115 +5109,108 @@
         <v>302</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" ht="16" customHeight="1" spans="1:1">
       <c r="A45" s="12"/>
-      <c r="B45" s="6"/>
-      <c r="C45" t="s">
+    </row>
+    <row r="46" ht="15" spans="1:3">
+      <c r="A46" s="12" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="46" ht="18.75" spans="1:1">
-      <c r="A46" s="12"/>
+      <c r="B46" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="47" ht="15" spans="1:3">
-      <c r="A47" s="12" t="s">
-        <v>304</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>305</v>
-      </c>
+      <c r="A47" s="12"/>
+      <c r="B47" s="6"/>
       <c r="C47" s="5" t="s">
-        <v>296</v>
+        <v>306</v>
       </c>
     </row>
     <row r="48" ht="15" spans="1:3">
       <c r="A48" s="12"/>
       <c r="B48" s="6"/>
       <c r="C48" s="5" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="49" ht="15" spans="1:3">
       <c r="A49" s="12"/>
       <c r="B49" s="6"/>
       <c r="C49" s="5" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="50" ht="15" spans="1:3">
       <c r="A50" s="12"/>
       <c r="B50" s="6"/>
       <c r="C50" s="5" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="51" ht="15" spans="1:3">
       <c r="A51" s="12"/>
       <c r="B51" s="6"/>
       <c r="C51" s="5" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="52" ht="15" spans="1:3">
       <c r="A52" s="12"/>
       <c r="B52" s="6"/>
       <c r="C52" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="53" ht="15" spans="1:3">
       <c r="A53" s="12"/>
       <c r="B53" s="6"/>
       <c r="C53" s="5" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="54" ht="15" spans="1:3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="54" ht="30" spans="1:3">
       <c r="A54" s="12"/>
       <c r="B54" s="6"/>
-      <c r="C54" s="5" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="55" ht="15" spans="1:3">
+      <c r="C54" s="13" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" s="12"/>
       <c r="B55" s="6"/>
-      <c r="C55" s="5" t="s">
-        <v>313</v>
+      <c r="C55" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="12"/>
       <c r="B56" s="6"/>
       <c r="C56" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="12"/>
-      <c r="B57" s="6"/>
-      <c r="C57" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="58" ht="7" customHeight="1" spans="1:3">
-      <c r="A58" s="8"/>
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
+    <row r="57" ht="7" customHeight="1" spans="1:3">
+      <c r="A57" s="8"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+    </row>
+    <row r="59" ht="37.5" spans="1:2">
+      <c r="A59" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="B59" s="11">
+        <v>1</v>
+      </c>
     </row>
     <row r="60" ht="37.5" spans="1:2">
       <c r="A60" s="10" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B60" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" ht="37.5" spans="1:2">
-      <c r="A61" s="10" t="s">
-        <v>317</v>
-      </c>
-      <c r="B61" s="11">
         <v>8</v>
       </c>
     </row>
@@ -5230,8 +5218,8 @@
   <mergeCells count="13">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:A36"/>
-    <mergeCell ref="A38:A45"/>
-    <mergeCell ref="A47:A57"/>
+    <mergeCell ref="A38:A44"/>
+    <mergeCell ref="A46:A56"/>
     <mergeCell ref="B5:B9"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B14:B19"/>
@@ -5239,8 +5227,8 @@
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="B28:B32"/>
     <mergeCell ref="B34:B36"/>
-    <mergeCell ref="B38:B45"/>
-    <mergeCell ref="B47:B57"/>
+    <mergeCell ref="B38:B44"/>
+    <mergeCell ref="B46:B56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Added Course Materials - Day 11
</commit_message>
<xml_diff>
--- a/Java Apps @ DXC - Domain - TOC.xlsx
+++ b/Java Apps @ DXC - Domain - TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="1" activeTab="5"/>
+    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="7" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="458">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -1199,7 +1199,8 @@
     <t>Day 10</t>
   </si>
   <si>
-    <t>Interacting with Data Using jQuery and Ajax</t>
+    <t xml:space="preserve">
+jQuery: Getting Started</t>
   </si>
   <si>
     <t>2.  CoursePreview</t>
@@ -1347,6 +1348,66 @@
   </si>
   <si>
     <t>5. Demo: Radio Buttons</t>
+  </si>
+  <si>
+    <t>8. The Big Picture</t>
+  </si>
+  <si>
+    <t>2. Different jQuery Versions</t>
+  </si>
+  <si>
+    <t>3. jQuery in Context of Other Libraries</t>
+  </si>
+  <si>
+    <t>4. Demo: JavaScript Function Scope</t>
+  </si>
+  <si>
+    <t>5. Demo: Naming Conventions</t>
+  </si>
+  <si>
+    <t>9. jQuery and AJAX</t>
+  </si>
+  <si>
+    <t>1. jQuery AJAX Introduction</t>
+  </si>
+  <si>
+    <t>2. Ajax methods of jQuery</t>
+  </si>
+  <si>
+    <t>3. jQuery Ajax Events</t>
+  </si>
+  <si>
+    <t>4. jQuery ajax() Method</t>
+  </si>
+  <si>
+    <t>5. jQuery ajax() Demo on JSFiddle</t>
+  </si>
+  <si>
+    <t>6. jQuery Ajax Load</t>
+  </si>
+  <si>
+    <t>7. jQuery Ajax Load Example</t>
+  </si>
+  <si>
+    <t>8. jQuery Ajax Load Demo</t>
+  </si>
+  <si>
+    <t>9. jQuery get() Method</t>
+  </si>
+  <si>
+    <t>10. jQuery get() Example</t>
+  </si>
+  <si>
+    <t>11. jQuery Ajax Get Demo</t>
+  </si>
+  <si>
+    <t>12. jQuery Ajax Post Method</t>
+  </si>
+  <si>
+    <t>13. jQuery Ajax Post Example</t>
+  </si>
+  <si>
+    <t>14. jQuery Ajax Post Demo</t>
   </si>
   <si>
     <t>Total # of Days for jQuery and Ajax</t>
@@ -1361,8 +1422,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="36">
@@ -1483,16 +1544,9 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1505,17 +1559,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1531,9 +1600,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1554,6 +1623,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1568,38 +1651,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1612,16 +1673,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1660,13 +1721,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1678,7 +1745,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1690,31 +1769,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1732,73 +1793,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1822,7 +1823,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1834,13 +1883,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1934,11 +1995,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1973,6 +2049,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1991,23 +2076,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2022,19 +2092,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2052,130 +2113,130 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="12" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -5799,12 +5860,12 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B55" sqref="B55:B60"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -5832,7 +5893,7 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" ht="15.75" spans="1:3">
+    <row r="3" ht="15" spans="1:3">
       <c r="A3" s="3" t="s">
         <v>386</v>
       </c>
@@ -5843,42 +5904,42 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" ht="15.75" spans="1:3">
+    <row r="4" ht="15" spans="1:3">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="5" ht="15.75" spans="1:3">
+    <row r="5" ht="15" spans="1:3">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="6" ht="15.75" spans="1:3">
+    <row r="6" ht="15" spans="1:3">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="7" ht="15.75" spans="1:3">
+    <row r="7" ht="15" spans="1:3">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="8" ht="15.75" spans="1:3">
+    <row r="8" ht="15" spans="1:3">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="9" ht="15.75" spans="1:3">
+    <row r="9" ht="15" spans="1:3">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
@@ -6003,14 +6064,14 @@
         <v>407</v>
       </c>
     </row>
-    <row r="27" ht="15.75" spans="1:3">
+    <row r="27" ht="15" spans="1:3">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="5" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="28" ht="15.75" spans="1:3">
+    <row r="28" ht="15" spans="1:3">
       <c r="A28" s="3"/>
       <c r="B28" s="4"/>
       <c r="C28" s="5" t="s">
@@ -6240,31 +6301,185 @@
         <v>398</v>
       </c>
     </row>
-    <row r="61" ht="7" customHeight="1" spans="1:3">
-      <c r="A61" s="9"/>
-      <c r="B61" s="10"/>
-      <c r="C61" s="10"/>
-    </row>
-    <row r="63" ht="37.5" spans="1:2">
-      <c r="A63" s="11" t="s">
+    <row r="61" customFormat="1" ht="18.75" spans="1:3">
+      <c r="A61" s="3"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="5"/>
+    </row>
+    <row r="62" customFormat="1" ht="18.75" spans="1:3">
+      <c r="A62" s="3"/>
+      <c r="B62" s="4" t="s">
         <v>436</v>
       </c>
-      <c r="B63" s="12">
+      <c r="C62" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" customFormat="1" ht="18.75" spans="1:3">
+      <c r="A63" s="3"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="5" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="64" customFormat="1" ht="18.75" spans="1:3">
+      <c r="A64" s="3"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="5" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="65" customFormat="1" ht="18.75" spans="1:3">
+      <c r="A65" s="3"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="5" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="66" customFormat="1" ht="18.75" spans="1:3">
+      <c r="A66" s="3"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="67" customFormat="1" ht="18.75" spans="1:3">
+      <c r="A67" s="3"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="5" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="68" customFormat="1" ht="18.75" spans="1:3">
+      <c r="A68" s="3"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="5"/>
+    </row>
+    <row r="69" customFormat="1" ht="18.75" spans="1:3">
+      <c r="A69" s="3"/>
+      <c r="B69" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="70" customFormat="1" ht="18.75" spans="1:3">
+      <c r="A70" s="3"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="71" customFormat="1" ht="18.75" spans="1:3">
+      <c r="A71" s="3"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="5" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="72" customFormat="1" ht="18.75" spans="1:3">
+      <c r="A72" s="3"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="73" customFormat="1" ht="18.75" spans="1:3">
+      <c r="A73" s="3"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="5" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="74" customFormat="1" ht="18.75" spans="1:3">
+      <c r="A74" s="3"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="5" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="75" customFormat="1" ht="18.75" spans="1:3">
+      <c r="A75" s="3"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="5" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="76" customFormat="1" ht="18.75" spans="1:3">
+      <c r="A76" s="3"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="5" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="77" customFormat="1" ht="18.75" spans="1:3">
+      <c r="A77" s="3"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="5" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="78" customFormat="1" ht="18.75" spans="1:3">
+      <c r="A78" s="3"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="5" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="79" customFormat="1" ht="18.75" spans="1:3">
+      <c r="A79" s="3"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="5" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="80" customFormat="1" ht="18.75" spans="1:3">
+      <c r="A80" s="3"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="5" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="81" customFormat="1" ht="18.75" spans="1:3">
+      <c r="A81" s="3"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="5" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="82" customFormat="1" ht="18.75" spans="1:3">
+      <c r="A82" s="3"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="5" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="83" ht="7" customHeight="1" spans="1:3">
+      <c r="A83" s="9"/>
+      <c r="B83" s="10"/>
+      <c r="C83" s="10"/>
+    </row>
+    <row r="85" ht="37.5" spans="1:2">
+      <c r="A85" s="11" t="s">
+        <v>456</v>
+      </c>
+      <c r="B85" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="64" ht="37.5" spans="1:2">
-      <c r="A64" s="11" t="s">
-        <v>437</v>
-      </c>
-      <c r="B64" s="12">
+    <row r="86" ht="37.5" spans="1:2">
+      <c r="A86" s="11" t="s">
+        <v>457</v>
+      </c>
+      <c r="B86" s="12">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:A60"/>
+    <mergeCell ref="A3:A82"/>
     <mergeCell ref="B3:B9"/>
     <mergeCell ref="B11:B16"/>
     <mergeCell ref="B18:B28"/>
@@ -6272,6 +6487,8 @@
     <mergeCell ref="B38:B46"/>
     <mergeCell ref="B48:B53"/>
     <mergeCell ref="B55:B60"/>
+    <mergeCell ref="B62:B67"/>
+    <mergeCell ref="B69:B82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Added Course Materials - Day 14
</commit_message>
<xml_diff>
--- a/Java Apps @ DXC - Domain - TOC.xlsx
+++ b/Java Apps @ DXC - Domain - TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="2" activeTab="5"/>
+    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="7" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="463">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -989,6 +989,15 @@
     <t>11. Constraints or Principles</t>
   </si>
   <si>
+    <t xml:space="preserve">Servlets and  JSPs </t>
+  </si>
+  <si>
+    <t>Hands On Exercises - JSPs</t>
+  </si>
+  <si>
+    <t>Hands On Exercises - Servlets</t>
+  </si>
+  <si>
     <t>Total # of Days for Servlets, JSPs and Web Services</t>
   </si>
   <si>
@@ -1188,6 +1197,9 @@
   </si>
   <si>
     <t>16. Summary</t>
+  </si>
+  <si>
+    <t>Maven Workshop</t>
   </si>
   <si>
     <t>Total # of Days for Maven</t>
@@ -1408,6 +1420,9 @@
   </si>
   <si>
     <t>14. jQuery Ajax Post Demo</t>
+  </si>
+  <si>
+    <t>Hands On Exercises - jQuery</t>
   </si>
   <si>
     <t>Total # of Days for jQuery and Ajax</t>
@@ -1422,8 +1437,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="36">
@@ -1476,18 +1491,26 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="14.05"/>
-      <color rgb="FFEFEFEF"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14.05"/>
+      <color rgb="FFEFEFEF"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1497,14 +1520,6 @@
     </font>
     <font>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1544,14 +1559,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1559,9 +1566,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1577,14 +1583,29 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1599,40 +1620,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1651,6 +1642,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -1659,22 +1658,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1721,7 +1736,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1733,175 +1910,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2010,30 +2025,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2045,6 +2036,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2076,8 +2076,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2095,7 +2110,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2113,130 +2128,130 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2260,33 +2275,33 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2298,7 +2313,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2852,8 +2867,8 @@
   <sheetPr/>
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
@@ -2884,7 +2899,7 @@
       <c r="C2" s="2"/>
     </row>
     <row r="3" ht="37.5" spans="1:3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -2900,7 +2915,7 @@
       <c r="C4" s="25"/>
     </row>
     <row r="5" ht="56.25" spans="1:3">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -2911,12 +2926,12 @@
       </c>
     </row>
     <row r="6" ht="18.75" spans="1:3">
-      <c r="A6" s="13"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="26"/>
       <c r="C6" s="8"/>
     </row>
     <row r="7" ht="31.5" spans="1:3">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -2927,47 +2942,47 @@
       </c>
     </row>
     <row r="8" ht="12" customHeight="1" spans="1:3">
-      <c r="A8" s="13"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="4"/>
       <c r="C8" s="24"/>
     </row>
     <row r="9" ht="15" spans="1:3">
-      <c r="A9" s="13"/>
-      <c r="B9" s="16" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" ht="15" spans="1:3">
-      <c r="A10" s="13"/>
-      <c r="B10" s="16"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" ht="15" spans="1:3">
-      <c r="A11" s="13"/>
-      <c r="B11" s="16"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" ht="52" customHeight="1" spans="1:3">
-      <c r="A12" s="13"/>
-      <c r="B12" s="16"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="24" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" ht="12" customHeight="1" spans="1:3">
-      <c r="A13" s="13"/>
-      <c r="B13" s="16"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="5"/>
     </row>
     <row r="14" ht="15.75" spans="1:3">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -2978,22 +2993,22 @@
       </c>
     </row>
     <row r="15" ht="15.75" spans="1:3">
-      <c r="A15" s="13"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
     </row>
     <row r="16" ht="15" spans="1:3">
-      <c r="A16" s="13"/>
-      <c r="B16" s="16" t="s">
+      <c r="A16" s="9"/>
+      <c r="B16" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" ht="15" spans="1:3">
-      <c r="A17" s="13"/>
-      <c r="B17" s="16"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="5" t="s">
         <v>34</v>
       </c>
@@ -3011,7 +3026,7 @@
       <c r="C19" s="25"/>
     </row>
     <row r="20" ht="31.5" spans="1:3">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -3022,40 +3037,40 @@
       </c>
     </row>
     <row r="21" ht="12" customHeight="1" spans="1:3">
-      <c r="A21" s="13"/>
+      <c r="A21" s="9"/>
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
     </row>
     <row r="22" ht="15" spans="1:3">
-      <c r="A22" s="13"/>
-      <c r="B22" s="16" t="s">
+      <c r="A22" s="9"/>
+      <c r="B22" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="23" ht="15" spans="1:3">
-      <c r="A23" s="13"/>
-      <c r="B23" s="16"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="24" ht="69" customHeight="1" spans="1:3">
-      <c r="A24" s="13"/>
-      <c r="B24" s="16"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="24" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="25" ht="9" customHeight="1" spans="1:3">
-      <c r="A25" s="13"/>
-      <c r="B25" s="16"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="5"/>
     </row>
     <row r="26" ht="38" customHeight="1" spans="1:3">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="9" t="s">
         <v>40</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -3066,22 +3081,22 @@
       </c>
     </row>
     <row r="27" ht="15" spans="1:3">
-      <c r="A27" s="13"/>
+      <c r="A27" s="9"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
     <row r="28" ht="15" spans="1:3">
-      <c r="A28" s="13"/>
-      <c r="B28" s="16" t="s">
+      <c r="A28" s="9"/>
+      <c r="B28" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="29" ht="100" customHeight="1" spans="1:3">
-      <c r="A29" s="13"/>
-      <c r="B29" s="16"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="10"/>
       <c r="C29" s="24" t="s">
         <v>42</v>
       </c>
@@ -3092,7 +3107,7 @@
       <c r="C30" s="8"/>
     </row>
     <row r="31" ht="15.75" spans="1:3">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -3103,22 +3118,22 @@
       </c>
     </row>
     <row r="32" ht="15" spans="1:3">
-      <c r="A32" s="13"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
     </row>
     <row r="33" ht="13" customHeight="1" spans="1:3">
-      <c r="A33" s="13"/>
-      <c r="B33" s="16" t="s">
+      <c r="A33" s="9"/>
+      <c r="B33" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C33" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="34" ht="89" customHeight="1" spans="1:3">
-      <c r="A34" s="13"/>
-      <c r="B34" s="16"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="10"/>
       <c r="C34" s="24" t="s">
         <v>45</v>
       </c>
@@ -3132,7 +3147,7 @@
       <c r="A37" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="12">
+      <c r="B37" s="15">
         <v>2</v>
       </c>
     </row>
@@ -3140,7 +3155,7 @@
       <c r="A38" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="12">
+      <c r="B38" s="15">
         <v>16</v>
       </c>
     </row>
@@ -3170,9 +3185,9 @@
   <dimension ref="A1:C223"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A181" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E190" sqref="E190"/>
+      <selection pane="bottomLeft" activeCell="C215" sqref="$A215:$XFD219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -3201,23 +3216,23 @@
       <c r="C2" s="2"/>
     </row>
     <row r="3" ht="18.75" spans="1:3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="9" t="s">
         <v>49</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="17" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" ht="18.75" spans="1:3">
-      <c r="A4" s="13"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="15"/>
+      <c r="C4" s="17"/>
     </row>
     <row r="5" ht="15.75" spans="1:3">
-      <c r="A5" s="13"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="4" t="s">
         <v>51</v>
       </c>
@@ -3226,12 +3241,12 @@
       </c>
     </row>
     <row r="6" ht="24.75" spans="1:3">
-      <c r="A6" s="13"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
     <row r="7" ht="15" spans="1:3">
-      <c r="A7" s="13"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="4" t="s">
         <v>53</v>
       </c>
@@ -3240,14 +3255,14 @@
       </c>
     </row>
     <row r="8" ht="15" spans="1:3">
-      <c r="A8" s="13"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:3">
-      <c r="A9" s="13"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
         <v>56</v>
@@ -3259,7 +3274,7 @@
       <c r="C10" s="5"/>
     </row>
     <row r="11" ht="15" spans="1:3">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="9" t="s">
         <v>57</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -3270,70 +3285,70 @@
       </c>
     </row>
     <row r="12" ht="15" spans="1:3">
-      <c r="A12" s="13"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:3">
-      <c r="A13" s="13"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="4"/>
       <c r="C13" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="14" ht="15" spans="1:3">
-      <c r="A14" s="13"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="15" ht="15" spans="1:3">
-      <c r="A15" s="13"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="16" ht="15" spans="1:3">
-      <c r="A16" s="13"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="17" ht="15" spans="1:3">
-      <c r="A17" s="13"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="18" ht="15" spans="1:3">
-      <c r="A18" s="13"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="19" ht="15" spans="1:3">
-      <c r="A19" s="13"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="4"/>
       <c r="C19" s="5" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="20" ht="15" spans="1:3">
-      <c r="A20" s="13"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="21" ht="15" spans="1:3">
-      <c r="A21" s="13"/>
+      <c r="A21" s="9"/>
       <c r="B21" s="4"/>
       <c r="C21" s="5" t="s">
         <v>69</v>
@@ -3345,7 +3360,7 @@
       <c r="C22" s="5"/>
     </row>
     <row r="23" ht="15" spans="1:3">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="9" t="s">
         <v>70</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -3356,82 +3371,82 @@
       </c>
     </row>
     <row r="24" ht="15" spans="1:3">
-      <c r="A24" s="13"/>
+      <c r="A24" s="9"/>
       <c r="B24" s="4"/>
       <c r="C24" s="5" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="25" ht="15" spans="1:3">
-      <c r="A25" s="13"/>
+      <c r="A25" s="9"/>
       <c r="B25" s="4"/>
       <c r="C25" s="5" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="26" ht="15" spans="1:3">
-      <c r="A26" s="13"/>
+      <c r="A26" s="9"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="27" ht="15" spans="1:3">
-      <c r="A27" s="13"/>
+      <c r="A27" s="9"/>
       <c r="B27" s="4"/>
       <c r="C27" s="5" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="28" ht="15" spans="1:3">
-      <c r="A28" s="13"/>
+      <c r="A28" s="9"/>
       <c r="B28" s="4"/>
       <c r="C28" s="5" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="29" ht="15" spans="1:3">
-      <c r="A29" s="13"/>
+      <c r="A29" s="9"/>
       <c r="B29" s="4"/>
       <c r="C29" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="30" ht="15" spans="1:3">
-      <c r="A30" s="13"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="4"/>
       <c r="C30" s="5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="31" ht="15" spans="1:3">
-      <c r="A31" s="13"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="4"/>
       <c r="C31" s="5" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="32" ht="15" spans="1:3">
-      <c r="A32" s="13"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="4"/>
       <c r="C32" s="5" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="33" ht="15" spans="1:3">
-      <c r="A33" s="13"/>
+      <c r="A33" s="9"/>
       <c r="B33" s="4"/>
       <c r="C33" s="5" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="34" ht="10" customHeight="1" spans="1:3">
-      <c r="A34" s="13"/>
+      <c r="A34" s="9"/>
       <c r="B34" s="4"/>
       <c r="C34" s="5"/>
     </row>
     <row r="35" ht="15" spans="1:3">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="9" t="s">
         <v>82</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -3442,71 +3457,71 @@
       </c>
     </row>
     <row r="36" ht="15" spans="1:3">
-      <c r="A36" s="13"/>
+      <c r="A36" s="9"/>
       <c r="B36" s="4"/>
       <c r="C36" s="5" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="37" ht="15" spans="1:3">
-      <c r="A37" s="13"/>
+      <c r="A37" s="9"/>
       <c r="B37" s="4"/>
       <c r="C37" s="5" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="38" ht="15" spans="1:3">
-      <c r="A38" s="13"/>
+      <c r="A38" s="9"/>
       <c r="B38" s="4"/>
       <c r="C38" s="5" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="39" ht="15" spans="1:3">
-      <c r="A39" s="13"/>
+      <c r="A39" s="9"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="40" ht="15" spans="1:3">
-      <c r="A40" s="13"/>
+      <c r="A40" s="9"/>
       <c r="B40" s="4"/>
       <c r="C40" s="5" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="41" ht="15" spans="1:3">
-      <c r="A41" s="13"/>
+      <c r="A41" s="9"/>
       <c r="B41" s="4"/>
       <c r="C41" s="5" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="42" ht="15" spans="1:3">
-      <c r="A42" s="13"/>
+      <c r="A42" s="9"/>
       <c r="B42" s="4"/>
       <c r="C42" s="5" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="43" ht="10" customHeight="1" spans="1:3">
-      <c r="A43" s="13"/>
+      <c r="A43" s="9"/>
       <c r="B43" s="4"/>
       <c r="C43" s="5"/>
     </row>
     <row r="44" ht="15" spans="1:3">
-      <c r="A44" s="13"/>
-      <c r="B44" s="16" t="s">
+      <c r="A44" s="9"/>
+      <c r="B44" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C44" s="17" t="s">
+      <c r="C44" s="11" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="45" ht="15" spans="1:3">
-      <c r="A45" s="13"/>
-      <c r="B45" s="16"/>
+      <c r="A45" s="9"/>
+      <c r="B45" s="10"/>
       <c r="C45" s="5" t="s">
         <v>92</v>
       </c>
@@ -3524,7 +3539,7 @@
       <c r="C47" s="2"/>
     </row>
     <row r="48" ht="15" spans="1:3">
-      <c r="A48" s="13" t="s">
+      <c r="A48" s="9" t="s">
         <v>94</v>
       </c>
       <c r="B48" s="4" t="s">
@@ -3535,63 +3550,63 @@
       </c>
     </row>
     <row r="49" ht="15" spans="1:3">
-      <c r="A49" s="13"/>
+      <c r="A49" s="9"/>
       <c r="B49" s="4"/>
       <c r="C49" s="5" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="50" ht="15" spans="1:3">
-      <c r="A50" s="13"/>
+      <c r="A50" s="9"/>
       <c r="B50" s="4"/>
       <c r="C50" s="5" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="51" ht="15" spans="1:3">
-      <c r="A51" s="13"/>
+      <c r="A51" s="9"/>
       <c r="B51" s="4"/>
       <c r="C51" s="5" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="52" ht="15" spans="1:3">
-      <c r="A52" s="13"/>
+      <c r="A52" s="9"/>
       <c r="B52" s="4"/>
       <c r="C52" s="5" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="53" ht="15" spans="1:3">
-      <c r="A53" s="13"/>
+      <c r="A53" s="9"/>
       <c r="B53" s="4"/>
       <c r="C53" s="5" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="54" ht="15" spans="1:3">
-      <c r="A54" s="13"/>
+      <c r="A54" s="9"/>
       <c r="B54" s="4"/>
       <c r="C54" s="5" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="55" ht="15" spans="1:3">
-      <c r="A55" s="13"/>
+      <c r="A55" s="9"/>
       <c r="B55" s="4"/>
       <c r="C55" s="5" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="56" ht="15" spans="1:3">
-      <c r="A56" s="13"/>
+      <c r="A56" s="9"/>
       <c r="B56" s="4"/>
       <c r="C56" s="5" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="57" ht="15" spans="1:3">
-      <c r="A57" s="13"/>
+      <c r="A57" s="9"/>
       <c r="B57" s="4"/>
       <c r="C57" s="5" t="s">
         <v>104</v>
@@ -3599,7 +3614,7 @@
     </row>
     <row r="58" ht="9" customHeight="1"/>
     <row r="59" ht="15" spans="1:3">
-      <c r="A59" s="13" t="s">
+      <c r="A59" s="9" t="s">
         <v>105</v>
       </c>
       <c r="B59" s="4" t="s">
@@ -3610,87 +3625,87 @@
       </c>
     </row>
     <row r="60" ht="15" spans="1:3">
-      <c r="A60" s="13"/>
+      <c r="A60" s="9"/>
       <c r="B60" s="4"/>
       <c r="C60" s="5"/>
     </row>
     <row r="61" ht="15" spans="1:3">
-      <c r="A61" s="13"/>
+      <c r="A61" s="9"/>
       <c r="B61" s="4"/>
       <c r="C61" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="62" ht="15" spans="1:3">
-      <c r="A62" s="13"/>
+      <c r="A62" s="9"/>
       <c r="B62" s="4"/>
       <c r="C62" s="5" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="63" ht="15" spans="1:3">
-      <c r="A63" s="13"/>
+      <c r="A63" s="9"/>
       <c r="B63" s="4"/>
       <c r="C63" s="5" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="64" ht="15" spans="1:3">
-      <c r="A64" s="13"/>
+      <c r="A64" s="9"/>
       <c r="B64" s="4"/>
       <c r="C64" s="5" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="65" ht="15" spans="1:3">
-      <c r="A65" s="13"/>
+      <c r="A65" s="9"/>
       <c r="B65" s="4"/>
       <c r="C65" s="5" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="66" ht="15" spans="1:3">
-      <c r="A66" s="13"/>
+      <c r="A66" s="9"/>
       <c r="B66" s="4"/>
       <c r="C66" s="5" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="67" ht="15" spans="1:3">
-      <c r="A67" s="13"/>
+      <c r="A67" s="9"/>
       <c r="B67" s="4"/>
       <c r="C67" s="5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="68" ht="15" spans="1:3">
-      <c r="A68" s="13"/>
+      <c r="A68" s="9"/>
       <c r="B68" s="4"/>
       <c r="C68" s="5" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="69" ht="15" spans="1:3">
-      <c r="A69" s="13"/>
+      <c r="A69" s="9"/>
       <c r="B69" s="4"/>
       <c r="C69" s="5" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="70" ht="15" spans="1:3">
-      <c r="A70" s="13"/>
+      <c r="A70" s="9"/>
       <c r="B70" s="4"/>
       <c r="C70" s="5" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="71" ht="15.75" spans="1:3">
-      <c r="A71" s="13"/>
+      <c r="A71" s="9"/>
       <c r="B71" s="4"/>
       <c r="C71" s="5"/>
     </row>
     <row r="72" ht="15" spans="1:3">
-      <c r="A72" s="13"/>
+      <c r="A72" s="9"/>
       <c r="B72" s="4" t="s">
         <v>117</v>
       </c>
@@ -3699,87 +3714,87 @@
       </c>
     </row>
     <row r="73" ht="15" spans="1:3">
-      <c r="A73" s="13"/>
+      <c r="A73" s="9"/>
       <c r="B73" s="4"/>
       <c r="C73" s="5" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="74" ht="15" spans="1:3">
-      <c r="A74" s="13"/>
+      <c r="A74" s="9"/>
       <c r="B74" s="4"/>
       <c r="C74" s="5" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="75" ht="15" spans="1:3">
-      <c r="A75" s="13"/>
+      <c r="A75" s="9"/>
       <c r="B75" s="4"/>
       <c r="C75" s="5" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="76" ht="15" spans="1:3">
-      <c r="A76" s="13"/>
+      <c r="A76" s="9"/>
       <c r="B76" s="4"/>
       <c r="C76" s="5" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="77" ht="15" spans="1:3">
-      <c r="A77" s="13"/>
+      <c r="A77" s="9"/>
       <c r="B77" s="4"/>
       <c r="C77" s="5" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="78" ht="15" spans="1:3">
-      <c r="A78" s="13"/>
+      <c r="A78" s="9"/>
       <c r="B78" s="4"/>
       <c r="C78" s="5" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="79" ht="15" spans="1:3">
-      <c r="A79" s="13"/>
+      <c r="A79" s="9"/>
       <c r="B79" s="4"/>
       <c r="C79" s="5" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="80" ht="15" spans="1:3">
-      <c r="A80" s="13"/>
+      <c r="A80" s="9"/>
       <c r="B80" s="4"/>
       <c r="C80" s="5" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="81" ht="15" spans="1:3">
-      <c r="A81" s="13"/>
+      <c r="A81" s="9"/>
       <c r="B81" s="4"/>
       <c r="C81" s="5" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="82" ht="15" spans="1:3">
-      <c r="A82" s="13"/>
+      <c r="A82" s="9"/>
       <c r="B82" s="4"/>
       <c r="C82" s="5" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="83" ht="15" spans="1:3">
-      <c r="A83" s="13"/>
-      <c r="B83" s="16" t="s">
+      <c r="A83" s="9"/>
+      <c r="B83" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C83" s="17" t="s">
+      <c r="C83" s="11" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="84" ht="15" spans="1:3">
-      <c r="A84" s="13"/>
-      <c r="B84" s="16"/>
+      <c r="A84" s="9"/>
+      <c r="B84" s="10"/>
       <c r="C84" s="5" t="s">
         <v>128</v>
       </c>
@@ -3797,7 +3812,7 @@
       <c r="C86" s="2"/>
     </row>
     <row r="87" ht="15" spans="1:3">
-      <c r="A87" s="13" t="s">
+      <c r="A87" s="9" t="s">
         <v>130</v>
       </c>
       <c r="B87" s="4" t="s">
@@ -3808,61 +3823,61 @@
       </c>
     </row>
     <row r="88" ht="15" spans="1:3">
-      <c r="A88" s="13"/>
+      <c r="A88" s="9"/>
       <c r="B88" s="4"/>
       <c r="C88" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="89" ht="15" spans="1:3">
-      <c r="A89" s="13"/>
+      <c r="A89" s="9"/>
       <c r="B89" s="4"/>
       <c r="C89" s="5" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="90" ht="15" spans="1:3">
-      <c r="A90" s="13"/>
+      <c r="A90" s="9"/>
       <c r="B90" s="4"/>
       <c r="C90" s="5" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="91" ht="15" spans="1:3">
-      <c r="A91" s="13"/>
+      <c r="A91" s="9"/>
       <c r="B91" s="4"/>
       <c r="C91" s="5" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="92" ht="15" spans="1:3">
-      <c r="A92" s="13"/>
+      <c r="A92" s="9"/>
       <c r="B92" s="4"/>
       <c r="C92" s="5" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="93" ht="15" spans="1:3">
-      <c r="A93" s="13"/>
+      <c r="A93" s="9"/>
       <c r="B93" s="4"/>
       <c r="C93" s="5" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="94" ht="15" spans="1:3">
-      <c r="A94" s="13"/>
+      <c r="A94" s="9"/>
       <c r="B94" s="4"/>
       <c r="C94" s="5" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="95" ht="15" spans="1:3">
-      <c r="A95" s="13"/>
+      <c r="A95" s="9"/>
       <c r="B95" s="4"/>
       <c r="C95" s="5"/>
     </row>
     <row r="96" ht="15" spans="1:3">
-      <c r="A96" s="13"/>
+      <c r="A96" s="9"/>
       <c r="B96" s="4" t="s">
         <v>138</v>
       </c>
@@ -3871,49 +3886,49 @@
       </c>
     </row>
     <row r="97" ht="15" spans="1:3">
-      <c r="A97" s="13"/>
+      <c r="A97" s="9"/>
       <c r="B97" s="4"/>
       <c r="C97" s="5" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="98" ht="15" spans="1:3">
-      <c r="A98" s="13"/>
+      <c r="A98" s="9"/>
       <c r="B98" s="4"/>
       <c r="C98" s="5" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="99" ht="15" spans="1:3">
-      <c r="A99" s="13"/>
+      <c r="A99" s="9"/>
       <c r="B99" s="4"/>
       <c r="C99" s="5" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="100" ht="15" spans="1:3">
-      <c r="A100" s="13"/>
+      <c r="A100" s="9"/>
       <c r="B100" s="4"/>
       <c r="C100" s="5" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="101" ht="15" spans="1:3">
-      <c r="A101" s="13"/>
+      <c r="A101" s="9"/>
       <c r="B101" s="4"/>
       <c r="C101" s="5" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="102" ht="15" spans="1:3">
-      <c r="A102" s="13"/>
+      <c r="A102" s="9"/>
       <c r="B102" s="4"/>
       <c r="C102" s="5" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="103" ht="15" spans="1:3">
-      <c r="A103" s="13"/>
+      <c r="A103" s="9"/>
       <c r="B103" s="4"/>
       <c r="C103" s="5" t="s">
         <v>116</v>
@@ -3921,7 +3936,7 @@
     </row>
     <row r="104" ht="9" customHeight="1"/>
     <row r="105" ht="22" customHeight="1" spans="1:3">
-      <c r="A105" s="13" t="s">
+      <c r="A105" s="9" t="s">
         <v>145</v>
       </c>
       <c r="B105" s="4" t="s">
@@ -3932,134 +3947,134 @@
       </c>
     </row>
     <row r="106" ht="15" hidden="1" spans="1:3">
-      <c r="A106" s="13"/>
+      <c r="A106" s="9"/>
       <c r="B106" s="4"/>
       <c r="C106" s="5" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="107" ht="15" spans="1:3">
-      <c r="A107" s="13"/>
+      <c r="A107" s="9"/>
       <c r="B107" s="4"/>
       <c r="C107" s="5" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="108" ht="15" spans="1:3">
-      <c r="A108" s="13"/>
+      <c r="A108" s="9"/>
       <c r="B108" s="4"/>
       <c r="C108" s="5" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="109" ht="15" spans="1:3">
-      <c r="A109" s="13"/>
+      <c r="A109" s="9"/>
       <c r="B109" s="4"/>
       <c r="C109" s="5" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="110" ht="15" spans="1:3">
-      <c r="A110" s="13"/>
+      <c r="A110" s="9"/>
       <c r="B110" s="4"/>
       <c r="C110" s="5" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="111" ht="15" spans="1:3">
-      <c r="A111" s="13"/>
+      <c r="A111" s="9"/>
       <c r="B111" s="4"/>
       <c r="C111" s="5" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="112" ht="15" spans="1:3">
-      <c r="A112" s="13"/>
+      <c r="A112" s="9"/>
       <c r="B112" s="4"/>
       <c r="C112" s="5" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="113" ht="15" spans="1:3">
-      <c r="A113" s="13"/>
+      <c r="A113" s="9"/>
       <c r="B113" s="4"/>
       <c r="C113" s="5" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="114" ht="15" spans="1:3">
-      <c r="A114" s="13"/>
+      <c r="A114" s="9"/>
       <c r="B114" s="4"/>
       <c r="C114" s="5" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="115" ht="15" spans="1:3">
-      <c r="A115" s="13"/>
+      <c r="A115" s="9"/>
       <c r="B115" s="4"/>
       <c r="C115" s="5" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="116" ht="15" spans="1:3">
-      <c r="A116" s="13"/>
+      <c r="A116" s="9"/>
       <c r="B116" s="4"/>
       <c r="C116" s="5" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="117" ht="15" spans="1:3">
-      <c r="A117" s="13"/>
+      <c r="A117" s="9"/>
       <c r="B117" s="4"/>
       <c r="C117" s="5" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="118" ht="15" spans="1:3">
-      <c r="A118" s="13"/>
+      <c r="A118" s="9"/>
       <c r="B118" s="4"/>
       <c r="C118" s="5" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="119" ht="15" spans="1:3">
-      <c r="A119" s="13"/>
+      <c r="A119" s="9"/>
       <c r="B119" s="4"/>
       <c r="C119" s="5" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="120" ht="15.75" spans="1:3">
-      <c r="A120" s="13"/>
+      <c r="A120" s="9"/>
       <c r="B120" s="4"/>
       <c r="C120" s="5"/>
     </row>
     <row r="121" ht="15" spans="1:3">
-      <c r="A121" s="13"/>
-      <c r="B121" s="16" t="s">
+      <c r="A121" s="9"/>
+      <c r="B121" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C121" s="17" t="s">
+      <c r="C121" s="11" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="122" ht="15" spans="1:3">
-      <c r="A122" s="13"/>
-      <c r="B122" s="16"/>
+      <c r="A122" s="9"/>
+      <c r="B122" s="10"/>
       <c r="C122" s="5" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="123" ht="15" spans="1:3">
-      <c r="A123" s="13"/>
-      <c r="B123" s="16"/>
+      <c r="A123" s="9"/>
+      <c r="B123" s="10"/>
       <c r="C123" s="5" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="124" ht="15" spans="1:3">
-      <c r="A124" s="13"/>
-      <c r="B124" s="16"/>
+      <c r="A124" s="9"/>
+      <c r="B124" s="10"/>
       <c r="C124" s="5" t="s">
         <v>163</v>
       </c>
@@ -4077,7 +4092,7 @@
       <c r="C126" s="2"/>
     </row>
     <row r="127" ht="15" spans="1:3">
-      <c r="A127" s="13" t="s">
+      <c r="A127" s="9" t="s">
         <v>165</v>
       </c>
       <c r="B127" s="4" t="s">
@@ -4088,70 +4103,70 @@
       </c>
     </row>
     <row r="128" ht="15" spans="1:3">
-      <c r="A128" s="13"/>
+      <c r="A128" s="9"/>
       <c r="B128" s="4"/>
       <c r="C128" s="5" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="129" ht="15" spans="1:3">
-      <c r="A129" s="13"/>
+      <c r="A129" s="9"/>
       <c r="B129" s="4"/>
       <c r="C129" s="5" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="130" ht="15" spans="1:3">
-      <c r="A130" s="13"/>
+      <c r="A130" s="9"/>
       <c r="B130" s="4"/>
       <c r="C130" s="5" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="131" ht="15" spans="1:3">
-      <c r="A131" s="13"/>
+      <c r="A131" s="9"/>
       <c r="B131" s="4"/>
       <c r="C131" s="5" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="132" ht="15" spans="1:3">
-      <c r="A132" s="13"/>
+      <c r="A132" s="9"/>
       <c r="B132" s="4"/>
       <c r="C132" s="5" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="133" ht="15" spans="1:3">
-      <c r="A133" s="13"/>
+      <c r="A133" s="9"/>
       <c r="B133" s="4"/>
       <c r="C133" s="5" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="134" ht="15" spans="1:3">
-      <c r="A134" s="13"/>
+      <c r="A134" s="9"/>
       <c r="B134" s="4"/>
       <c r="C134" s="5" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="135" ht="15" spans="1:3">
-      <c r="A135" s="13"/>
+      <c r="A135" s="9"/>
       <c r="B135" s="4"/>
       <c r="C135" s="5" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="136" ht="15" spans="1:3">
-      <c r="A136" s="13"/>
+      <c r="A136" s="9"/>
       <c r="B136" s="4"/>
       <c r="C136" s="5" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="137" ht="15" spans="1:3">
-      <c r="A137" s="13"/>
+      <c r="A137" s="9"/>
       <c r="B137" s="4"/>
       <c r="C137" s="5" t="s">
         <v>69</v>
@@ -4163,7 +4178,7 @@
       <c r="C138" s="5"/>
     </row>
     <row r="139" ht="15" spans="1:3">
-      <c r="A139" s="13" t="s">
+      <c r="A139" s="9" t="s">
         <v>176</v>
       </c>
       <c r="B139" s="4" t="s">
@@ -4174,204 +4189,204 @@
       </c>
     </row>
     <row r="140" ht="15" spans="1:3">
-      <c r="A140" s="13"/>
+      <c r="A140" s="9"/>
       <c r="B140" s="4"/>
       <c r="C140" s="5" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="141" ht="15" spans="1:3">
-      <c r="A141" s="13"/>
+      <c r="A141" s="9"/>
       <c r="B141" s="4"/>
       <c r="C141" s="5" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="142" ht="15" spans="1:3">
-      <c r="A142" s="13"/>
+      <c r="A142" s="9"/>
       <c r="B142" s="4"/>
       <c r="C142" s="5" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="143" ht="15" spans="1:3">
-      <c r="A143" s="13"/>
+      <c r="A143" s="9"/>
       <c r="B143" s="4"/>
       <c r="C143" s="5" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="144" ht="15" spans="1:3">
-      <c r="A144" s="13"/>
+      <c r="A144" s="9"/>
       <c r="B144" s="4"/>
       <c r="C144" s="21" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="145" ht="21" customHeight="1" spans="1:3">
-      <c r="A145" s="13"/>
+      <c r="A145" s="9"/>
       <c r="B145" s="4"/>
       <c r="C145" s="21" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="146" ht="15" spans="1:3">
-      <c r="A146" s="13"/>
+      <c r="A146" s="9"/>
       <c r="B146" s="4"/>
       <c r="C146" s="21" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="147" ht="15" spans="1:3">
-      <c r="A147" s="13"/>
+      <c r="A147" s="9"/>
       <c r="B147" s="4"/>
       <c r="C147" s="21" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="148" ht="15" spans="1:3">
-      <c r="A148" s="13"/>
+      <c r="A148" s="9"/>
       <c r="B148" s="4"/>
       <c r="C148" s="21" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="149" ht="15" spans="1:3">
-      <c r="A149" s="13"/>
+      <c r="A149" s="9"/>
       <c r="B149" s="4"/>
       <c r="C149" s="21" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="150" ht="15" spans="1:3">
-      <c r="A150" s="13"/>
+      <c r="A150" s="9"/>
       <c r="B150" s="4"/>
       <c r="C150" s="21" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="151" ht="15" spans="1:3">
-      <c r="A151" s="13"/>
+      <c r="A151" s="9"/>
       <c r="B151" s="4"/>
       <c r="C151" s="21" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="152" ht="15" spans="1:3">
-      <c r="A152" s="13"/>
+      <c r="A152" s="9"/>
       <c r="B152" s="4"/>
       <c r="C152" s="21" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="153" ht="15" spans="1:3">
-      <c r="A153" s="13"/>
+      <c r="A153" s="9"/>
       <c r="B153" s="4"/>
       <c r="C153" s="21" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="154" ht="15" spans="1:3">
-      <c r="A154" s="13"/>
+      <c r="A154" s="9"/>
       <c r="B154" s="4"/>
       <c r="C154" s="21" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="155" ht="15" spans="1:3">
-      <c r="A155" s="13"/>
+      <c r="A155" s="9"/>
       <c r="B155" s="4"/>
       <c r="C155" s="21" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="156" ht="15" spans="1:3">
-      <c r="A156" s="13"/>
+      <c r="A156" s="9"/>
       <c r="B156" s="4"/>
       <c r="C156" s="21" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="157" ht="15.75" spans="1:3">
-      <c r="A157" s="13"/>
+      <c r="A157" s="9"/>
       <c r="B157" s="6"/>
       <c r="C157" s="21"/>
     </row>
     <row r="158" ht="15" spans="1:3">
-      <c r="A158" s="13"/>
-      <c r="B158" s="16" t="s">
+      <c r="A158" s="9"/>
+      <c r="B158" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C158" s="17" t="s">
+      <c r="C158" s="11" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="159" ht="15" spans="1:3">
-      <c r="A159" s="13"/>
-      <c r="B159" s="16"/>
+      <c r="A159" s="9"/>
+      <c r="B159" s="10"/>
       <c r="C159" s="5" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="160" ht="15" spans="1:3">
-      <c r="A160" s="13"/>
-      <c r="B160" s="16"/>
+      <c r="A160" s="9"/>
+      <c r="B160" s="10"/>
       <c r="C160" s="5" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="161" ht="15" spans="1:3">
-      <c r="A161" s="13"/>
-      <c r="B161" s="16"/>
+      <c r="A161" s="9"/>
+      <c r="B161" s="10"/>
       <c r="C161" s="5" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="162" ht="15" spans="1:3">
-      <c r="A162" s="13"/>
-      <c r="B162" s="16"/>
-      <c r="C162" s="17" t="s">
+      <c r="A162" s="9"/>
+      <c r="B162" s="10"/>
+      <c r="C162" s="11" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="163" ht="15" spans="1:3">
-      <c r="A163" s="13"/>
-      <c r="B163" s="16"/>
+      <c r="A163" s="9"/>
+      <c r="B163" s="10"/>
       <c r="C163" s="5" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="164" ht="15" spans="1:3">
-      <c r="A164" s="13"/>
-      <c r="B164" s="16"/>
+      <c r="A164" s="9"/>
+      <c r="B164" s="10"/>
       <c r="C164" s="5" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="165" ht="15" spans="1:3">
-      <c r="A165" s="13"/>
-      <c r="B165" s="16"/>
+      <c r="A165" s="9"/>
+      <c r="B165" s="10"/>
       <c r="C165" s="5" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="166" ht="15" spans="1:3">
-      <c r="A166" s="13"/>
-      <c r="B166" s="16"/>
+      <c r="A166" s="9"/>
+      <c r="B166" s="10"/>
       <c r="C166" s="5" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="167" ht="15" spans="1:3">
-      <c r="A167" s="13"/>
-      <c r="B167" s="16"/>
+      <c r="A167" s="9"/>
+      <c r="B167" s="10"/>
       <c r="C167" s="5" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="168" ht="15" spans="1:3">
-      <c r="A168" s="13"/>
-      <c r="B168" s="16"/>
+      <c r="A168" s="9"/>
+      <c r="B168" s="10"/>
       <c r="C168" s="5" t="s">
         <v>205</v>
       </c>
@@ -4389,7 +4404,7 @@
       <c r="C170" s="2"/>
     </row>
     <row r="171" ht="27" customHeight="1" spans="1:3">
-      <c r="A171" s="13" t="s">
+      <c r="A171" s="9" t="s">
         <v>207</v>
       </c>
       <c r="B171" s="4" t="s">
@@ -4400,40 +4415,40 @@
       </c>
     </row>
     <row r="172" ht="27" customHeight="1" spans="1:3">
-      <c r="A172" s="13"/>
+      <c r="A172" s="9"/>
       <c r="B172" s="4"/>
       <c r="C172" s="5" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="173" ht="27" customHeight="1" spans="1:3">
-      <c r="A173" s="13"/>
+      <c r="A173" s="9"/>
       <c r="B173" s="4"/>
       <c r="C173" s="5" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="174" ht="27" customHeight="1" spans="1:3">
-      <c r="A174" s="13"/>
+      <c r="A174" s="9"/>
       <c r="B174" s="4"/>
       <c r="C174" s="5" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="175" ht="27" customHeight="1" spans="1:3">
-      <c r="A175" s="13"/>
+      <c r="A175" s="9"/>
       <c r="B175" s="4"/>
       <c r="C175" s="5" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="176" ht="18" spans="1:3">
-      <c r="A176" s="13"/>
+      <c r="A176" s="9"/>
       <c r="B176" s="22"/>
       <c r="C176" s="8"/>
     </row>
     <row r="177" ht="15" spans="1:3">
-      <c r="A177" s="13"/>
+      <c r="A177" s="9"/>
       <c r="B177" s="4" t="s">
         <v>213</v>
       </c>
@@ -4442,35 +4457,35 @@
       </c>
     </row>
     <row r="178" spans="1:3">
-      <c r="A178" s="13"/>
+      <c r="A178" s="9"/>
       <c r="B178" s="4"/>
       <c r="C178" s="8" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="179" ht="15" spans="1:3">
-      <c r="A179" s="13"/>
+      <c r="A179" s="9"/>
       <c r="B179" s="4"/>
       <c r="C179" s="5" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="180" ht="15" spans="1:3">
-      <c r="A180" s="13"/>
+      <c r="A180" s="9"/>
       <c r="B180" s="4"/>
-      <c r="C180" s="14" t="s">
+      <c r="C180" s="16" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="181" ht="15" spans="1:3">
-      <c r="A181" s="13"/>
+      <c r="A181" s="9"/>
       <c r="B181" s="4"/>
       <c r="C181" s="5" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="182" ht="15" spans="1:3">
-      <c r="A182" s="13"/>
+      <c r="A182" s="9"/>
       <c r="B182" s="4"/>
       <c r="C182" s="5" t="s">
         <v>218</v>
@@ -4482,182 +4497,182 @@
       <c r="C183" s="5"/>
     </row>
     <row r="184" ht="15" spans="1:3">
-      <c r="A184" s="13" t="s">
+      <c r="A184" s="9" t="s">
         <v>219</v>
       </c>
       <c r="B184" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="C184" s="14" t="s">
+      <c r="C184" s="16" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="185" ht="15" spans="1:3">
-      <c r="A185" s="13"/>
+      <c r="A185" s="9"/>
       <c r="B185" s="4"/>
-      <c r="C185" s="14" t="s">
+      <c r="C185" s="16" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="186" ht="15" spans="1:3">
-      <c r="A186" s="13"/>
+      <c r="A186" s="9"/>
       <c r="B186" s="4"/>
-      <c r="C186" s="14" t="s">
+      <c r="C186" s="16" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="187" ht="18" spans="1:3">
-      <c r="A187" s="13"/>
+      <c r="A187" s="9"/>
       <c r="B187" s="22"/>
-      <c r="C187" s="14"/>
+      <c r="C187" s="16"/>
     </row>
     <row r="188" ht="15" spans="1:3">
-      <c r="A188" s="13"/>
+      <c r="A188" s="9"/>
       <c r="B188" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="C188" s="14" t="s">
+      <c r="C188" s="16" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="189" ht="15" spans="1:3">
-      <c r="A189" s="13"/>
+      <c r="A189" s="9"/>
       <c r="B189" s="4"/>
-      <c r="C189" s="14" t="s">
+      <c r="C189" s="16" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="190" ht="15" spans="1:3">
-      <c r="A190" s="13"/>
+      <c r="A190" s="9"/>
       <c r="B190" s="4"/>
-      <c r="C190" s="14" t="s">
+      <c r="C190" s="16" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="191" ht="15" spans="1:3">
-      <c r="A191" s="13"/>
+      <c r="A191" s="9"/>
       <c r="B191" s="8"/>
-      <c r="C191" s="14"/>
+      <c r="C191" s="16"/>
     </row>
     <row r="192" ht="15" spans="1:3">
-      <c r="A192" s="13"/>
+      <c r="A192" s="9"/>
       <c r="B192" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="C192" s="14" t="s">
+      <c r="C192" s="16" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="193" ht="15" spans="1:3">
-      <c r="A193" s="13"/>
+      <c r="A193" s="9"/>
       <c r="B193" s="4"/>
-      <c r="C193" s="14" t="s">
+      <c r="C193" s="16" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="194" ht="15" spans="1:3">
-      <c r="A194" s="13"/>
+      <c r="A194" s="9"/>
       <c r="B194" s="4"/>
-      <c r="C194" s="14" t="s">
+      <c r="C194" s="16" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="195" ht="15" spans="1:3">
-      <c r="A195" s="13"/>
+      <c r="A195" s="9"/>
       <c r="B195" s="4"/>
-      <c r="C195" s="14" t="s">
+      <c r="C195" s="16" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="196" ht="15" spans="1:3">
-      <c r="A196" s="13"/>
+      <c r="A196" s="9"/>
       <c r="B196" s="4"/>
-      <c r="C196" s="14" t="s">
+      <c r="C196" s="16" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="197" ht="15" spans="1:3">
-      <c r="A197" s="13"/>
+      <c r="A197" s="9"/>
       <c r="B197" s="4"/>
-      <c r="C197" s="14" t="s">
+      <c r="C197" s="16" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="198" ht="15" spans="1:3">
-      <c r="A198" s="13"/>
+      <c r="A198" s="9"/>
       <c r="B198" s="4"/>
-      <c r="C198" s="14" t="s">
+      <c r="C198" s="16" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="199" ht="15" spans="1:3">
-      <c r="A199" s="13"/>
+      <c r="A199" s="9"/>
       <c r="B199" s="4"/>
-      <c r="C199" s="14" t="s">
+      <c r="C199" s="16" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="200" ht="15" spans="1:3">
-      <c r="A200" s="13"/>
+      <c r="A200" s="9"/>
       <c r="B200" s="4"/>
-      <c r="C200" s="14" t="s">
+      <c r="C200" s="16" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="201" ht="18.75" spans="1:3">
       <c r="A201" s="19"/>
       <c r="B201" s="4"/>
-      <c r="C201" s="14"/>
+      <c r="C201" s="16"/>
     </row>
     <row r="202" ht="15" spans="1:3">
-      <c r="A202" s="13" t="s">
+      <c r="A202" s="9" t="s">
         <v>238</v>
       </c>
       <c r="B202" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="C202" s="14" t="s">
+      <c r="C202" s="16" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="203" ht="15" spans="1:3">
-      <c r="A203" s="13"/>
+      <c r="A203" s="9"/>
       <c r="B203" s="4"/>
-      <c r="C203" s="14" t="s">
+      <c r="C203" s="16" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="204" ht="15" spans="1:3">
-      <c r="A204" s="13"/>
+      <c r="A204" s="9"/>
       <c r="B204" s="4"/>
-      <c r="C204" s="14" t="s">
+      <c r="C204" s="16" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="205" ht="15" spans="1:3">
-      <c r="A205" s="13"/>
+      <c r="A205" s="9"/>
       <c r="B205" s="4"/>
-      <c r="C205" s="14" t="s">
+      <c r="C205" s="16" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="206" ht="15" spans="1:3">
-      <c r="A206" s="13"/>
+      <c r="A206" s="9"/>
       <c r="B206" s="4"/>
-      <c r="C206" s="14" t="s">
+      <c r="C206" s="16" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="207" ht="18.75" spans="1:3">
       <c r="A207" s="19"/>
       <c r="B207" s="4"/>
-      <c r="C207" s="14"/>
+      <c r="C207" s="16"/>
     </row>
     <row r="208" ht="15" spans="1:3">
-      <c r="A208" s="13" t="s">
+      <c r="A208" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="B208" s="16" t="s">
+      <c r="B208" s="10" t="s">
         <v>246</v>
       </c>
       <c r="C208" s="5" t="s">
@@ -4665,78 +4680,78 @@
       </c>
     </row>
     <row r="209" ht="15" spans="1:3">
-      <c r="A209" s="13"/>
-      <c r="B209" s="16"/>
+      <c r="A209" s="9"/>
+      <c r="B209" s="10"/>
       <c r="C209" s="5" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="210" ht="15" spans="1:3">
-      <c r="A210" s="13"/>
-      <c r="B210" s="16"/>
+      <c r="A210" s="9"/>
+      <c r="B210" s="10"/>
       <c r="C210" s="5" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="211" ht="15" customHeight="1" spans="1:3">
-      <c r="A211" s="13"/>
-      <c r="B211" s="16"/>
+      <c r="A211" s="9"/>
+      <c r="B211" s="10"/>
       <c r="C211" s="5" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="212" ht="15" spans="1:3">
-      <c r="A212" s="13"/>
-      <c r="B212" s="16"/>
+      <c r="A212" s="9"/>
+      <c r="B212" s="10"/>
       <c r="C212" s="5" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="213" ht="15" spans="1:3">
-      <c r="A213" s="13"/>
-      <c r="B213" s="16"/>
+      <c r="A213" s="9"/>
+      <c r="B213" s="10"/>
       <c r="C213" s="5" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="214" ht="18.75" spans="1:3">
-      <c r="A214" s="13"/>
+      <c r="A214" s="9"/>
       <c r="B214" s="4"/>
       <c r="C214" s="5"/>
     </row>
     <row r="215" ht="15" spans="1:3">
-      <c r="A215" s="13"/>
-      <c r="B215" s="16" t="s">
+      <c r="A215" s="9"/>
+      <c r="B215" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C215" s="17" t="s">
+      <c r="C215" s="11" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="216" ht="15" spans="1:3">
-      <c r="A216" s="13"/>
-      <c r="B216" s="16"/>
+      <c r="A216" s="9"/>
+      <c r="B216" s="10"/>
       <c r="C216" s="5" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="217" ht="15" spans="1:3">
-      <c r="A217" s="13"/>
-      <c r="B217" s="16"/>
+      <c r="A217" s="9"/>
+      <c r="B217" s="10"/>
       <c r="C217" s="5" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="218" ht="15" spans="1:3">
-      <c r="A218" s="13"/>
-      <c r="B218" s="16"/>
+      <c r="A218" s="9"/>
+      <c r="B218" s="10"/>
       <c r="C218" s="5" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="219" ht="15" spans="1:3">
-      <c r="A219" s="13"/>
-      <c r="B219" s="16"/>
+      <c r="A219" s="9"/>
+      <c r="B219" s="10"/>
       <c r="C219" s="5" t="s">
         <v>256</v>
       </c>
@@ -4751,7 +4766,7 @@
       <c r="A222" s="23" t="s">
         <v>257</v>
       </c>
-      <c r="B222" s="12">
+      <c r="B222" s="15">
         <v>5</v>
       </c>
     </row>
@@ -4759,7 +4774,7 @@
       <c r="A223" s="23" t="s">
         <v>258</v>
       </c>
-      <c r="B223" s="12">
+      <c r="B223" s="15">
         <v>40</v>
       </c>
     </row>
@@ -4819,12 +4834,12 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C46" sqref="C46:C56"/>
+      <selection pane="bottomLeft" activeCell="C57" sqref="$A57:$XFD59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -5093,7 +5108,7 @@
       </c>
     </row>
     <row r="38" ht="15" spans="1:3">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="9" t="s">
         <v>294</v>
       </c>
       <c r="B38" s="4" t="s">
@@ -5104,52 +5119,52 @@
       </c>
     </row>
     <row r="39" ht="15" spans="1:3">
-      <c r="A39" s="13"/>
+      <c r="A39" s="9"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="40" ht="15" spans="1:3">
-      <c r="A40" s="13"/>
+      <c r="A40" s="9"/>
       <c r="B40" s="4"/>
       <c r="C40" s="5" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="41" ht="15" spans="1:3">
-      <c r="A41" s="13"/>
+      <c r="A41" s="9"/>
       <c r="B41" s="4"/>
       <c r="C41" s="5" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="42" ht="15" spans="1:3">
-      <c r="A42" s="13"/>
+      <c r="A42" s="9"/>
       <c r="B42" s="4"/>
       <c r="C42" s="5" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="43" ht="15" spans="1:3">
-      <c r="A43" s="13"/>
+      <c r="A43" s="9"/>
       <c r="B43" s="4"/>
       <c r="C43" s="5" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="13"/>
+      <c r="A44" s="9"/>
       <c r="B44" s="4"/>
       <c r="C44" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="45" ht="16" customHeight="1" spans="1:1">
-      <c r="A45" s="13"/>
+      <c r="A45" s="9"/>
     </row>
     <row r="46" ht="15" spans="1:3">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="9" t="s">
         <v>303</v>
       </c>
       <c r="B46" s="4" t="s">
@@ -5160,102 +5175,126 @@
       </c>
     </row>
     <row r="47" ht="15" spans="1:3">
-      <c r="A47" s="13"/>
+      <c r="A47" s="9"/>
       <c r="B47" s="4"/>
       <c r="C47" s="5" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="48" ht="15" spans="1:3">
-      <c r="A48" s="13"/>
+      <c r="A48" s="9"/>
       <c r="B48" s="4"/>
       <c r="C48" s="5" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="49" ht="15" spans="1:3">
-      <c r="A49" s="13"/>
+      <c r="A49" s="9"/>
       <c r="B49" s="4"/>
       <c r="C49" s="5" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="50" ht="15" spans="1:3">
-      <c r="A50" s="13"/>
+      <c r="A50" s="9"/>
       <c r="B50" s="4"/>
       <c r="C50" s="5" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="51" ht="15" spans="1:3">
-      <c r="A51" s="13"/>
+      <c r="A51" s="9"/>
       <c r="B51" s="4"/>
       <c r="C51" s="5" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="52" ht="15" spans="1:3">
-      <c r="A52" s="13"/>
+      <c r="A52" s="9"/>
       <c r="B52" s="4"/>
       <c r="C52" s="5" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="53" ht="15" spans="1:3">
-      <c r="A53" s="13"/>
+      <c r="A53" s="9"/>
       <c r="B53" s="4"/>
       <c r="C53" s="5" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="54" ht="30" spans="1:3">
-      <c r="A54" s="13"/>
+      <c r="A54" s="9"/>
       <c r="B54" s="4"/>
-      <c r="C54" s="14" t="s">
+      <c r="C54" s="16" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="13"/>
+      <c r="A55" s="9"/>
       <c r="B55" s="4"/>
       <c r="C55" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="13"/>
+      <c r="A56" s="9"/>
       <c r="B56" s="4"/>
       <c r="C56" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="57" ht="7" customHeight="1" spans="1:3">
+    <row r="57" ht="15" spans="1:3">
       <c r="A57" s="9"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-    </row>
-    <row r="59" ht="37.5" spans="1:2">
-      <c r="A59" s="11" t="s">
+      <c r="B57" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C57" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="B59" s="12">
+    </row>
+    <row r="58" ht="15" spans="1:3">
+      <c r="A58" s="9"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="5" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="59" ht="15" spans="1:3">
+      <c r="A59" s="9"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="60" ht="7" customHeight="1" spans="1:3">
+      <c r="A60" s="12"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="13"/>
+    </row>
+    <row r="62" ht="37.5" spans="1:2">
+      <c r="A62" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="B62" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="60" ht="37.5" spans="1:2">
-      <c r="A60" s="11" t="s">
-        <v>317</v>
-      </c>
-      <c r="B60" s="12">
+    <row r="63" ht="37.5" spans="1:2">
+      <c r="A63" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="B63" s="15">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="15">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:A36"/>
     <mergeCell ref="A38:A44"/>
     <mergeCell ref="A46:A56"/>
+    <mergeCell ref="A57:A59"/>
     <mergeCell ref="B5:B9"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B14:B19"/>
@@ -5265,6 +5304,7 @@
     <mergeCell ref="B34:B36"/>
     <mergeCell ref="B38:B44"/>
     <mergeCell ref="B46:B56"/>
+    <mergeCell ref="B57:B59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -5274,12 +5314,12 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C79" sqref="C79"/>
+      <selection pane="bottomLeft" activeCell="C76" sqref="$A76:$XFD77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -5302,14 +5342,14 @@
     </row>
     <row r="2" ht="24.75" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" ht="15.75" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>261</v>
@@ -5326,10 +5366,10 @@
     <row r="5" ht="15" spans="1:3">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="6" ht="15" spans="1:3">
@@ -5343,49 +5383,49 @@
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:3">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:3">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
     </row>
     <row r="10" ht="15" spans="1:3">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="11" ht="15" spans="1:3">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:3">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:3">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="5" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -5395,7 +5435,7 @@
     <row r="15" ht="15" spans="1:3">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>59</v>
@@ -5405,77 +5445,77 @@
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
     </row>
     <row r="17" ht="15" spans="1:3">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="18" ht="15" spans="1:3">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="19" ht="15" spans="1:3">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
       <c r="C19" s="5" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="20" ht="15" spans="1:3">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="21" ht="15" spans="1:3">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
       <c r="C21" s="5" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="22" ht="15" spans="1:3">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
       <c r="C22" s="5" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="23" ht="15" spans="1:3">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="5" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="24" ht="15" spans="1:3">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="5" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="25" ht="15" spans="1:3">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="5" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="26" ht="15" spans="1:3">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="27" ht="15" spans="1:3">
@@ -5485,7 +5525,7 @@
     <row r="28" ht="15" spans="1:3">
       <c r="A28" s="3"/>
       <c r="B28" s="4" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>59</v>
@@ -5495,56 +5535,56 @@
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
       <c r="C29" s="5" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
     <row r="30" ht="15" spans="1:3">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="5" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
     </row>
     <row r="31" ht="15" spans="1:3">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="5" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
     <row r="32" ht="15" spans="1:3">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="5" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="33" ht="15" spans="1:3">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="5" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
     </row>
     <row r="34" ht="15" spans="1:3">
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
       <c r="C34" s="5" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
     </row>
     <row r="35" ht="15" spans="1:3">
       <c r="A35" s="3"/>
       <c r="B35" s="4"/>
       <c r="C35" s="5" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="36" ht="15" spans="1:3">
       <c r="A36" s="3"/>
       <c r="B36" s="4"/>
       <c r="C36" s="5" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
     </row>
     <row r="37" ht="15.75" spans="1:3">
@@ -5555,7 +5595,7 @@
     <row r="38" ht="15" spans="1:3">
       <c r="A38" s="3"/>
       <c r="B38" s="4" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>59</v>
@@ -5565,42 +5605,42 @@
       <c r="A39" s="3"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="40" ht="15" spans="1:3">
       <c r="A40" s="3"/>
       <c r="B40" s="4"/>
       <c r="C40" s="5" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="41" ht="15" spans="1:3">
       <c r="A41" s="3"/>
       <c r="B41" s="4"/>
       <c r="C41" s="5" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
     <row r="42" ht="15" spans="1:3">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="5" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="43" ht="15" spans="1:3">
       <c r="A43" s="3"/>
       <c r="B43" s="4"/>
       <c r="C43" s="5" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="44" ht="15" spans="1:3">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="5" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
     <row r="45" ht="15" spans="1:3">
@@ -5618,7 +5658,7 @@
     <row r="47" ht="15" spans="1:3">
       <c r="A47" s="3"/>
       <c r="B47" s="4" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>59</v>
@@ -5628,77 +5668,77 @@
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="5" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="49" ht="15" spans="1:3">
       <c r="A49" s="3"/>
       <c r="B49" s="4"/>
       <c r="C49" s="5" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="50" ht="15" spans="1:3">
       <c r="A50" s="3"/>
       <c r="B50" s="4"/>
       <c r="C50" s="5" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
     </row>
     <row r="51" ht="15" spans="1:3">
       <c r="A51" s="3"/>
       <c r="B51" s="4"/>
       <c r="C51" s="5" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="52" ht="15" spans="1:3">
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="5" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="53" ht="15" spans="1:3">
       <c r="A53" s="3"/>
       <c r="B53" s="4"/>
       <c r="C53" s="5" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="54" ht="15" spans="1:3">
       <c r="A54" s="3"/>
       <c r="B54" s="4"/>
       <c r="C54" s="5" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="55" ht="15" spans="1:3">
       <c r="A55" s="3"/>
       <c r="B55" s="4"/>
       <c r="C55" s="5" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="56" ht="15" spans="1:3">
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="5" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="57" ht="15" spans="1:3">
       <c r="A57" s="3"/>
       <c r="B57" s="4"/>
       <c r="C57" s="5" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="58" ht="15" spans="1:3">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="5" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="59" ht="15.75" spans="1:3">
@@ -5709,7 +5749,7 @@
     <row r="60" ht="15" spans="1:3">
       <c r="A60" s="3"/>
       <c r="B60" s="4" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>59</v>
@@ -5719,138 +5759,156 @@
       <c r="A61" s="3"/>
       <c r="B61" s="4"/>
       <c r="C61" s="5" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="62" ht="15" spans="1:3">
       <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="5" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="63" ht="15" spans="1:3">
       <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="5" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
     <row r="64" ht="15" spans="1:3">
       <c r="A64" s="3"/>
       <c r="B64" s="4"/>
       <c r="C64" s="5" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="65" ht="15" spans="1:3">
       <c r="A65" s="3"/>
       <c r="B65" s="4"/>
       <c r="C65" s="5" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="66" ht="15" spans="1:3">
       <c r="A66" s="3"/>
       <c r="B66" s="4"/>
       <c r="C66" s="5" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="67" ht="15" spans="1:3">
       <c r="A67" s="3"/>
       <c r="B67" s="4"/>
       <c r="C67" s="5" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="68" ht="15" spans="1:3">
       <c r="A68" s="3"/>
       <c r="B68" s="4"/>
       <c r="C68" s="5" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
     </row>
     <row r="69" ht="15" spans="1:3">
       <c r="A69" s="3"/>
       <c r="B69" s="4"/>
       <c r="C69" s="5" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="70" ht="15" spans="1:3">
       <c r="A70" s="3"/>
       <c r="B70" s="4"/>
       <c r="C70" s="5" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row r="71" ht="15" spans="1:3">
       <c r="A71" s="3"/>
       <c r="B71" s="4"/>
       <c r="C71" s="5" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
     </row>
     <row r="72" ht="15" spans="1:3">
       <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="5" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="73" ht="15" spans="1:3">
       <c r="A73" s="3"/>
       <c r="B73" s="4"/>
       <c r="C73" s="5" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="74" ht="15" spans="1:3">
       <c r="A74" s="3"/>
       <c r="B74" s="4"/>
       <c r="C74" s="5" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="75" ht="15" spans="1:3">
       <c r="A75" s="3"/>
       <c r="B75" s="4"/>
       <c r="C75" s="5" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="76" ht="7" customHeight="1" spans="1:3">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="76" ht="15" spans="1:3">
       <c r="A76" s="9"/>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
-    </row>
-    <row r="78" ht="18.75" spans="1:2">
-      <c r="A78" s="11" t="s">
-        <v>383</v>
-      </c>
-      <c r="B78" s="12">
+      <c r="B76" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C76" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" ht="15" spans="1:3">
+      <c r="A77" s="9"/>
+      <c r="B77" s="10"/>
+      <c r="C77" s="5" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="78" ht="7" customHeight="1" spans="1:3">
+      <c r="A78" s="12"/>
+      <c r="B78" s="13"/>
+      <c r="C78" s="13"/>
+    </row>
+    <row r="80" ht="18.75" spans="1:2">
+      <c r="A80" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="B80" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="79" ht="18.75" spans="1:2">
-      <c r="A79" s="11" t="s">
-        <v>384</v>
-      </c>
-      <c r="B79" s="12">
+    <row r="81" ht="18.75" spans="1:2">
+      <c r="A81" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="B81" s="15">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:A75"/>
+    <mergeCell ref="A76:A77"/>
     <mergeCell ref="B5:B13"/>
     <mergeCell ref="B15:B26"/>
     <mergeCell ref="B28:B36"/>
     <mergeCell ref="B38:B45"/>
     <mergeCell ref="B47:B58"/>
     <mergeCell ref="B60:B75"/>
+    <mergeCell ref="B76:B77"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -5860,12 +5918,12 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C86"/>
+  <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:A82"/>
+      <selection pane="bottomLeft" activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -5888,14 +5946,14 @@
     </row>
     <row r="2" ht="24.75" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" ht="15" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>59</v>
@@ -5908,35 +5966,35 @@
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
     </row>
     <row r="5" ht="15" spans="1:3">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
     </row>
     <row r="6" ht="15" spans="1:3">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="7" ht="15" spans="1:3">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:3">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:3">
@@ -5954,45 +6012,45 @@
     <row r="11" ht="15" spans="1:3">
       <c r="A11" s="3"/>
       <c r="B11" s="4" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:3">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:3">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="5" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
     </row>
     <row r="14" ht="15" spans="1:3">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
     </row>
     <row r="15" ht="15" spans="1:3">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
     </row>
     <row r="16" ht="15" spans="1:3">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -6002,73 +6060,73 @@
     <row r="18" ht="15" spans="1:3">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="19" ht="15" spans="1:3">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
       <c r="C19" s="5" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="20" ht="15" spans="1:3">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
     </row>
     <row r="21" ht="15" spans="1:3">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
       <c r="C21" s="5" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
     </row>
     <row r="22" ht="15" spans="1:3">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
       <c r="C22" s="5" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
     </row>
     <row r="23" ht="15" spans="1:3">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="5" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
     </row>
     <row r="24" ht="15" spans="1:3">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="5" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
     </row>
     <row r="25" ht="15" spans="1:3">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="5" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
     </row>
     <row r="26" ht="15" spans="1:3">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
     </row>
     <row r="27" ht="15" spans="1:3">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="5" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
     </row>
     <row r="28" ht="15" spans="1:3">
@@ -6085,52 +6143,52 @@
     <row r="30" ht="15" spans="1:3">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="31" ht="15" spans="1:3">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="5" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
     </row>
     <row r="32" ht="15" spans="1:3">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="5" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
     </row>
     <row r="33" ht="15" spans="1:3">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="5" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
     </row>
     <row r="34" ht="15" spans="1:3">
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
       <c r="C34" s="5" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
     </row>
     <row r="35" ht="15" spans="1:3">
       <c r="A35" s="3"/>
       <c r="B35" s="4"/>
       <c r="C35" s="5" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
     </row>
     <row r="36" ht="15" spans="1:3">
       <c r="A36" s="3"/>
       <c r="B36" s="4"/>
       <c r="C36" s="5" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
     </row>
     <row r="37" ht="15.75" spans="1:3">
@@ -6141,7 +6199,7 @@
     <row r="38" ht="15" spans="1:3">
       <c r="A38" s="3"/>
       <c r="B38" s="4" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>59</v>
@@ -6151,56 +6209,56 @@
       <c r="A39" s="3"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
     </row>
     <row r="40" ht="15" spans="1:3">
       <c r="A40" s="3"/>
       <c r="B40" s="4"/>
       <c r="C40" s="5" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
     </row>
     <row r="41" ht="15" spans="1:3">
       <c r="A41" s="3"/>
       <c r="B41" s="4"/>
       <c r="C41" s="5" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
     </row>
     <row r="42" ht="15" spans="1:3">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="5" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
     </row>
     <row r="43" ht="15" spans="1:3">
       <c r="A43" s="3"/>
       <c r="B43" s="4"/>
       <c r="C43" s="5" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
     </row>
     <row r="44" ht="15" spans="1:3">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="5" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
     </row>
     <row r="45" ht="15" spans="1:3">
       <c r="A45" s="3"/>
       <c r="B45" s="4"/>
       <c r="C45" s="5" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="46" ht="15" spans="1:3">
       <c r="A46" s="3"/>
       <c r="B46" s="4"/>
       <c r="C46" s="5" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
     </row>
     <row r="47" ht="15.75" spans="1:3">
@@ -6211,7 +6269,7 @@
     <row r="48" ht="15" spans="1:3">
       <c r="A48" s="3"/>
       <c r="B48" s="4" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>59</v>
@@ -6221,35 +6279,35 @@
       <c r="A49" s="3"/>
       <c r="B49" s="4"/>
       <c r="C49" s="5" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
     </row>
     <row r="50" ht="15" spans="1:3">
       <c r="A50" s="3"/>
       <c r="B50" s="4"/>
       <c r="C50" s="5" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="51" ht="15" spans="1:3">
       <c r="A51" s="3"/>
       <c r="B51" s="4"/>
       <c r="C51" s="5" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
     </row>
     <row r="52" ht="15" spans="1:3">
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="5" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
     </row>
     <row r="53" ht="15" spans="1:3">
       <c r="A53" s="3"/>
       <c r="B53" s="4"/>
       <c r="C53" s="5" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
     </row>
     <row r="54" ht="15.75" spans="1:3">
@@ -6260,7 +6318,7 @@
     <row r="55" ht="15" spans="1:3">
       <c r="A55" s="3"/>
       <c r="B55" s="4" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>59</v>
@@ -6270,216 +6328,233 @@
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="5" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
     </row>
     <row r="57" ht="15" spans="1:3">
       <c r="A57" s="3"/>
       <c r="B57" s="4"/>
       <c r="C57" s="5" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
     </row>
     <row r="58" ht="15" spans="1:3">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="5" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
     </row>
     <row r="59" ht="15" spans="1:3">
       <c r="A59" s="3"/>
       <c r="B59" s="4"/>
       <c r="C59" s="5" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
     </row>
     <row r="60" ht="15" spans="1:3">
       <c r="A60" s="3"/>
       <c r="B60" s="4"/>
       <c r="C60" s="5" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="61" customFormat="1" ht="18.75" spans="1:3">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="61" customFormat="1" ht="15.75" spans="1:3">
       <c r="A61" s="3"/>
       <c r="B61" s="4"/>
       <c r="C61" s="5"/>
     </row>
-    <row r="62" customFormat="1" ht="18.75" spans="1:3">
+    <row r="62" customFormat="1" ht="15" spans="1:3">
       <c r="A62" s="3"/>
       <c r="B62" s="4" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="63" customFormat="1" ht="18.75" spans="1:3">
+    <row r="63" customFormat="1" ht="15" spans="1:3">
       <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="5" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="64" customFormat="1" ht="18.75" spans="1:3">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="64" customFormat="1" ht="15" spans="1:3">
       <c r="A64" s="3"/>
       <c r="B64" s="4"/>
       <c r="C64" s="5" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="65" customFormat="1" ht="18.75" spans="1:3">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="65" customFormat="1" ht="15" spans="1:3">
       <c r="A65" s="3"/>
       <c r="B65" s="4"/>
       <c r="C65" s="5" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="66" customFormat="1" ht="18.75" spans="1:3">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="66" customFormat="1" ht="15" spans="1:3">
       <c r="A66" s="3"/>
       <c r="B66" s="4"/>
       <c r="C66" s="5" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="67" customFormat="1" ht="18.75" spans="1:3">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="67" customFormat="1" ht="15" spans="1:3">
       <c r="A67" s="3"/>
       <c r="B67" s="4"/>
       <c r="C67" s="5" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="68" customFormat="1" ht="18.75" spans="1:3">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="68" customFormat="1" ht="15.75" spans="1:3">
       <c r="A68" s="3"/>
       <c r="B68" s="4"/>
       <c r="C68" s="5"/>
     </row>
-    <row r="69" customFormat="1" ht="18.75" spans="1:3">
+    <row r="69" customFormat="1" ht="15" spans="1:3">
       <c r="A69" s="3"/>
       <c r="B69" s="4" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="70" customFormat="1" ht="18.75" spans="1:3">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="70" customFormat="1" ht="15" spans="1:3">
       <c r="A70" s="3"/>
       <c r="B70" s="4"/>
       <c r="C70" s="5" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="71" customFormat="1" ht="18.75" spans="1:3">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="71" customFormat="1" ht="15" spans="1:3">
       <c r="A71" s="3"/>
       <c r="B71" s="4"/>
       <c r="C71" s="5" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="72" customFormat="1" ht="18.75" spans="1:3">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="72" customFormat="1" ht="15" spans="1:3">
       <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="5" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="73" customFormat="1" ht="18.75" spans="1:3">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="73" customFormat="1" ht="15" spans="1:3">
       <c r="A73" s="3"/>
       <c r="B73" s="4"/>
       <c r="C73" s="5" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="74" customFormat="1" ht="18.75" spans="1:3">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="74" customFormat="1" ht="15" spans="1:3">
       <c r="A74" s="3"/>
       <c r="B74" s="4"/>
       <c r="C74" s="5" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="75" customFormat="1" ht="18.75" spans="1:3">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="75" customFormat="1" ht="15" spans="1:3">
       <c r="A75" s="3"/>
       <c r="B75" s="4"/>
       <c r="C75" s="5" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="76" customFormat="1" ht="18.75" spans="1:3">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="76" customFormat="1" ht="15" spans="1:3">
       <c r="A76" s="3"/>
       <c r="B76" s="4"/>
       <c r="C76" s="5" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="77" customFormat="1" ht="18.75" spans="1:3">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="77" customFormat="1" ht="15" spans="1:3">
       <c r="A77" s="3"/>
       <c r="B77" s="4"/>
       <c r="C77" s="5" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="78" customFormat="1" ht="18.75" spans="1:3">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="78" customFormat="1" ht="15" spans="1:3">
       <c r="A78" s="3"/>
       <c r="B78" s="4"/>
       <c r="C78" s="5" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="79" customFormat="1" ht="18.75" spans="1:3">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="79" customFormat="1" ht="15" spans="1:3">
       <c r="A79" s="3"/>
       <c r="B79" s="4"/>
       <c r="C79" s="5" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="80" customFormat="1" ht="18.75" spans="1:3">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="80" customFormat="1" ht="15" spans="1:3">
       <c r="A80" s="3"/>
       <c r="B80" s="4"/>
       <c r="C80" s="5" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="81" customFormat="1" ht="18.75" spans="1:3">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="81" customFormat="1" ht="15" spans="1:3">
       <c r="A81" s="3"/>
       <c r="B81" s="4"/>
       <c r="C81" s="5" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="82" customFormat="1" ht="18.75" spans="1:3">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="82" customFormat="1" ht="15" spans="1:3">
       <c r="A82" s="3"/>
       <c r="B82" s="4"/>
       <c r="C82" s="5" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="83" ht="7" customHeight="1" spans="1:3">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="83" customFormat="1" ht="15" spans="1:3">
       <c r="A83" s="9"/>
-      <c r="B83" s="10"/>
-      <c r="C83" s="10"/>
-    </row>
-    <row r="85" ht="37.5" spans="1:2">
-      <c r="A85" s="11" t="s">
-        <v>456</v>
-      </c>
-      <c r="B85" s="12">
+      <c r="B83" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C83" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" customFormat="1" ht="15" spans="1:3">
+      <c r="A84" s="9"/>
+      <c r="B84" s="10"/>
+      <c r="C84" s="5" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="85" ht="7" customHeight="1" spans="1:3">
+      <c r="A85" s="12"/>
+      <c r="B85" s="13"/>
+      <c r="C85" s="13"/>
+    </row>
+    <row r="87" ht="37.5" spans="1:2">
+      <c r="A87" s="14" t="s">
+        <v>461</v>
+      </c>
+      <c r="B87" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="86" ht="37.5" spans="1:2">
-      <c r="A86" s="11" t="s">
-        <v>457</v>
-      </c>
-      <c r="B86" s="12">
+    <row r="88" ht="37.5" spans="1:2">
+      <c r="A88" s="14" t="s">
+        <v>462</v>
+      </c>
+      <c r="B88" s="15">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:A82"/>
+    <mergeCell ref="A83:A84"/>
     <mergeCell ref="B3:B9"/>
     <mergeCell ref="B11:B16"/>
     <mergeCell ref="B18:B28"/>
@@ -6489,6 +6564,7 @@
     <mergeCell ref="B55:B60"/>
     <mergeCell ref="B62:B67"/>
     <mergeCell ref="B69:B82"/>
+    <mergeCell ref="B83:B84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>